<commit_message>
Fixed some facto bugs on expences - looking very good now;-)
</commit_message>
<xml_diff>
--- a/tests/Feature/config/fond_tenpercent.xlsx
+++ b/tests/Feature/config/fond_tenpercent.xlsx
@@ -996,7 +996,7 @@
     <col min="2" max="2" width="9.283" bestFit="true" customWidth="true" style="0"/>
     <col min="3" max="3" width="12.854" bestFit="true" customWidth="true" style="0"/>
     <col min="4" max="4" width="8.141" bestFit="true" customWidth="true" style="0"/>
-    <col min="5" max="5" width="16.425" bestFit="true" customWidth="true" style="0"/>
+    <col min="5" max="5" width="12.854" bestFit="true" customWidth="true" style="0"/>
     <col min="6" max="6" width="6.998" bestFit="true" customWidth="true" style="0"/>
     <col min="7" max="7" width="8.141" bestFit="true" customWidth="true" style="0"/>
     <col min="8" max="8" width="9.283" bestFit="true" customWidth="true" style="0"/>
@@ -1244,7 +1244,7 @@
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="5">
-        <v>2160000</v>
+        <v>180000</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="1">
@@ -1318,7 +1318,7 @@
       </c>
       <c r="D8" s="9"/>
       <c r="E8" s="8">
-        <v>2376000</v>
+        <v>198000</v>
       </c>
       <c r="F8" s="9"/>
       <c r="G8" s="8">
@@ -1394,7 +1394,7 @@
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="5">
-        <v>2613600</v>
+        <v>217800</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="1">
@@ -1470,7 +1470,7 @@
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="5">
-        <v>2874960</v>
+        <v>239580</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="1">
@@ -1546,7 +1546,7 @@
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="5">
-        <v>3162456</v>
+        <v>263538</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="1">
@@ -1622,7 +1622,7 @@
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="5">
-        <v>3478701.6</v>
+        <v>289891.8</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="1">
@@ -1698,7 +1698,7 @@
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="5">
-        <v>3826571.76</v>
+        <v>318880.98</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="1">
@@ -1774,7 +1774,7 @@
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="5">
-        <v>4209228.936</v>
+        <v>350769.078</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="1">
@@ -1850,7 +1850,7 @@
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="5">
-        <v>4630151.8296</v>
+        <v>385845.9858</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="1">
@@ -1926,7 +1926,7 @@
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="5">
-        <v>5093167.01256</v>
+        <v>424430.58438</v>
       </c>
       <c r="F16" s="2"/>
       <c r="G16" s="1">
@@ -2002,7 +2002,7 @@
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="5">
-        <v>5602483.713816</v>
+        <v>466873.642818</v>
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="1">
@@ -2078,7 +2078,7 @@
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="5">
-        <v>6162732.0851976</v>
+        <v>513561.0070998</v>
       </c>
       <c r="F18" s="2"/>
       <c r="G18" s="1">
@@ -2154,7 +2154,7 @@
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="5">
-        <v>6779005.2937174</v>
+        <v>564917.10780978</v>
       </c>
       <c r="F19" s="2"/>
       <c r="G19" s="1">
@@ -2230,7 +2230,7 @@
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="5">
-        <v>7456905.8230891</v>
+        <v>621408.81859076</v>
       </c>
       <c r="F20" s="2"/>
       <c r="G20" s="1">
@@ -2306,7 +2306,7 @@
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="5">
-        <v>8202596.4053981</v>
+        <v>683549.70044984</v>
       </c>
       <c r="F21" s="2"/>
       <c r="G21" s="1">
@@ -2382,7 +2382,7 @@
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="5">
-        <v>9022856.0459378</v>
+        <v>751904.67049482</v>
       </c>
       <c r="F22" s="2"/>
       <c r="G22" s="1">
@@ -2458,7 +2458,7 @@
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="5">
-        <v>9925141.6505316</v>
+        <v>827095.1375443</v>
       </c>
       <c r="F23" s="2"/>
       <c r="G23" s="1">
@@ -2534,7 +2534,7 @@
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="5">
-        <v>10917655.815585</v>
+        <v>909804.65129873</v>
       </c>
       <c r="F24" s="2"/>
       <c r="G24" s="1">
@@ -2610,7 +2610,7 @@
       </c>
       <c r="D25" s="2"/>
       <c r="E25" s="5">
-        <v>12009421.397143</v>
+        <v>1000785.1164286</v>
       </c>
       <c r="F25" s="2"/>
       <c r="G25" s="1">
@@ -2686,7 +2686,7 @@
       </c>
       <c r="D26" s="2"/>
       <c r="E26" s="5">
-        <v>13210363.536858</v>
+        <v>1100863.6280715</v>
       </c>
       <c r="F26" s="2"/>
       <c r="G26" s="1">
@@ -2762,7 +2762,7 @@
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="5">
-        <v>14531399.890543</v>
+        <v>1210949.9908786</v>
       </c>
       <c r="F27" s="2"/>
       <c r="G27" s="1">
@@ -2838,7 +2838,7 @@
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="5">
-        <v>15984539.879598</v>
+        <v>1332044.9899665</v>
       </c>
       <c r="F28" s="2"/>
       <c r="G28" s="1">
@@ -2914,7 +2914,7 @@
       </c>
       <c r="D29" s="2"/>
       <c r="E29" s="5">
-        <v>17582993.867558</v>
+        <v>1465249.4889632</v>
       </c>
       <c r="F29" s="2"/>
       <c r="G29" s="1">
@@ -2990,7 +2990,7 @@
       </c>
       <c r="D30" s="2"/>
       <c r="E30" s="5">
-        <v>19341293.254314</v>
+        <v>1611774.4378595</v>
       </c>
       <c r="F30" s="2"/>
       <c r="G30" s="1">
@@ -3066,7 +3066,7 @@
       </c>
       <c r="D31" s="2"/>
       <c r="E31" s="5">
-        <v>21275422.579746</v>
+        <v>1772951.8816455</v>
       </c>
       <c r="F31" s="2"/>
       <c r="G31" s="1">
@@ -3142,7 +3142,7 @@
       </c>
       <c r="D32" s="2"/>
       <c r="E32" s="5">
-        <v>23402964.837721</v>
+        <v>1950247.0698101</v>
       </c>
       <c r="F32" s="2"/>
       <c r="G32" s="1">
@@ -3218,7 +3218,7 @@
       </c>
       <c r="D33" s="2"/>
       <c r="E33" s="5">
-        <v>25743261.321493</v>
+        <v>2145271.7767911</v>
       </c>
       <c r="F33" s="2"/>
       <c r="G33" s="1">
@@ -3294,7 +3294,7 @@
       </c>
       <c r="D34" s="2"/>
       <c r="E34" s="5">
-        <v>28317587.453642</v>
+        <v>2359798.9544702</v>
       </c>
       <c r="F34" s="2"/>
       <c r="G34" s="1">
@@ -3370,7 +3370,7 @@
       </c>
       <c r="D35" s="2"/>
       <c r="E35" s="5">
-        <v>31149346.199006</v>
+        <v>2595778.8499172</v>
       </c>
       <c r="F35" s="2"/>
       <c r="G35" s="1">
@@ -3446,7 +3446,7 @@
       </c>
       <c r="D36" s="2"/>
       <c r="E36" s="5">
-        <v>34264280.818907</v>
+        <v>2855356.7349089</v>
       </c>
       <c r="F36" s="2"/>
       <c r="G36" s="1">
@@ -3522,7 +3522,7 @@
       </c>
       <c r="D37" s="2"/>
       <c r="E37" s="5">
-        <v>37690708.900798</v>
+        <v>3140892.4083998</v>
       </c>
       <c r="F37" s="2"/>
       <c r="G37" s="1">
@@ -3598,7 +3598,7 @@
       </c>
       <c r="D38" s="2"/>
       <c r="E38" s="5">
-        <v>41459779.790878</v>
+        <v>3454981.6492398</v>
       </c>
       <c r="F38" s="2"/>
       <c r="G38" s="1">
@@ -3674,7 +3674,7 @@
       </c>
       <c r="D39" s="2"/>
       <c r="E39" s="5">
-        <v>45605757.769966</v>
+        <v>3800479.8141638</v>
       </c>
       <c r="F39" s="2"/>
       <c r="G39" s="1">
@@ -3750,7 +3750,7 @@
       </c>
       <c r="D40" s="12"/>
       <c r="E40" s="11">
-        <v>50166333.546962</v>
+        <v>4180527.7955802</v>
       </c>
       <c r="F40" s="12"/>
       <c r="G40" s="11">
@@ -3826,7 +3826,7 @@
       </c>
       <c r="D41" s="2"/>
       <c r="E41" s="5">
-        <v>55182966.901658</v>
+        <v>4598580.5751382</v>
       </c>
       <c r="F41" s="2"/>
       <c r="G41" s="1">
@@ -3902,7 +3902,7 @@
       </c>
       <c r="D42" s="2"/>
       <c r="E42" s="5">
-        <v>60701263.591824</v>
+        <v>5058438.632652</v>
       </c>
       <c r="F42" s="2"/>
       <c r="G42" s="1">
@@ -3978,7 +3978,7 @@
       </c>
       <c r="D43" s="2"/>
       <c r="E43" s="5">
-        <v>66771389.951006</v>
+        <v>5564282.4959172</v>
       </c>
       <c r="F43" s="2"/>
       <c r="G43" s="1">
@@ -4054,7 +4054,7 @@
       </c>
       <c r="D44" s="2"/>
       <c r="E44" s="5">
-        <v>73448528.946107</v>
+        <v>6120710.7455089</v>
       </c>
       <c r="F44" s="2"/>
       <c r="G44" s="1">
@@ -4130,7 +4130,7 @@
       </c>
       <c r="D45" s="2"/>
       <c r="E45" s="5">
-        <v>80793381.840718</v>
+        <v>6732781.8200598</v>
       </c>
       <c r="F45" s="2"/>
       <c r="G45" s="1">
@@ -4206,7 +4206,7 @@
       </c>
       <c r="D46" s="2"/>
       <c r="E46" s="5">
-        <v>88872720.02479</v>
+        <v>7406060.0020658</v>
       </c>
       <c r="F46" s="2"/>
       <c r="G46" s="1">
@@ -4282,7 +4282,7 @@
       </c>
       <c r="D47" s="2"/>
       <c r="E47" s="5">
-        <v>97759992.027269</v>
+        <v>8146666.0022724</v>
       </c>
       <c r="F47" s="2"/>
       <c r="G47" s="1">
@@ -4358,7 +4358,7 @@
       </c>
       <c r="D48" s="2"/>
       <c r="E48" s="5">
-        <v>107535991.23</v>
+        <v>8961332.6024996</v>
       </c>
       <c r="F48" s="2"/>
       <c r="G48" s="1">
@@ -4434,7 +4434,7 @@
       </c>
       <c r="D49" s="2"/>
       <c r="E49" s="5">
-        <v>118289590.353</v>
+        <v>9857465.8627496</v>
       </c>
       <c r="F49" s="2"/>
       <c r="G49" s="1">
@@ -4510,7 +4510,7 @@
       </c>
       <c r="D50" s="2"/>
       <c r="E50" s="5">
-        <v>130118549.3883</v>
+        <v>10843212.449025</v>
       </c>
       <c r="F50" s="2"/>
       <c r="G50" s="1">
@@ -4586,7 +4586,7 @@
       </c>
       <c r="D51" s="2"/>
       <c r="E51" s="5">
-        <v>143130404.32714</v>
+        <v>11927533.693928</v>
       </c>
       <c r="F51" s="2"/>
       <c r="G51" s="1">
@@ -4662,7 +4662,7 @@
       </c>
       <c r="D52" s="2"/>
       <c r="E52" s="5">
-        <v>157443444.75985</v>
+        <v>13120287.063321</v>
       </c>
       <c r="F52" s="2"/>
       <c r="G52" s="1">
@@ -4738,7 +4738,7 @@
       </c>
       <c r="D53" s="14"/>
       <c r="E53" s="13">
-        <v>173187789.23584</v>
+        <v>14432315.769653</v>
       </c>
       <c r="F53" s="14"/>
       <c r="G53" s="13">
@@ -4814,7 +4814,7 @@
       </c>
       <c r="D54" s="2"/>
       <c r="E54" s="5">
-        <v>190506568.15942</v>
+        <v>15875547.346618</v>
       </c>
       <c r="F54" s="2"/>
       <c r="G54" s="1">
@@ -4890,7 +4890,7 @@
       </c>
       <c r="D55" s="2"/>
       <c r="E55" s="5">
-        <v>209557224.97536</v>
+        <v>17463102.08128</v>
       </c>
       <c r="F55" s="2"/>
       <c r="G55" s="1">
@@ -4966,7 +4966,7 @@
       </c>
       <c r="D56" s="2"/>
       <c r="E56" s="5">
-        <v>230512947.4729</v>
+        <v>19209412.289408</v>
       </c>
       <c r="F56" s="2"/>
       <c r="G56" s="1">
@@ -5042,7 +5042,7 @@
       </c>
       <c r="D57" s="14"/>
       <c r="E57" s="13">
-        <v>253564242.22019</v>
+        <v>21130353.518349</v>
       </c>
       <c r="F57" s="14"/>
       <c r="G57" s="13">
@@ -5118,7 +5118,7 @@
       </c>
       <c r="D58" s="2"/>
       <c r="E58" s="5">
-        <v>278920666.44221</v>
+        <v>23243388.870184</v>
       </c>
       <c r="F58" s="2"/>
       <c r="G58" s="1">
@@ -5194,7 +5194,7 @@
       </c>
       <c r="D59" s="2"/>
       <c r="E59" s="5">
-        <v>306812733.08642</v>
+        <v>25567727.757202</v>
       </c>
       <c r="F59" s="2"/>
       <c r="G59" s="1">
@@ -5270,7 +5270,7 @@
       </c>
       <c r="D60" s="2"/>
       <c r="E60" s="5">
-        <v>337494006.39506</v>
+        <v>28124500.532922</v>
       </c>
       <c r="F60" s="2"/>
       <c r="G60" s="1">
@@ -5346,7 +5346,7 @@
       </c>
       <c r="D61" s="2"/>
       <c r="E61" s="5">
-        <v>371243407.03457</v>
+        <v>30936950.586214</v>
       </c>
       <c r="F61" s="2"/>
       <c r="G61" s="1">
@@ -5422,7 +5422,7 @@
       </c>
       <c r="D62" s="2"/>
       <c r="E62" s="5">
-        <v>408367747.73802</v>
+        <v>34030645.644835</v>
       </c>
       <c r="F62" s="2"/>
       <c r="G62" s="1">
@@ -5498,7 +5498,7 @@
       </c>
       <c r="D63" s="2"/>
       <c r="E63" s="5">
-        <v>449204522.51183</v>
+        <v>37433710.209319</v>
       </c>
       <c r="F63" s="2"/>
       <c r="G63" s="1">
@@ -5574,7 +5574,7 @@
       </c>
       <c r="D64" s="2"/>
       <c r="E64" s="5">
-        <v>494124974.76301</v>
+        <v>41177081.230251</v>
       </c>
       <c r="F64" s="2"/>
       <c r="G64" s="1">
@@ -5650,7 +5650,7 @@
       </c>
       <c r="D65" s="2"/>
       <c r="E65" s="5">
-        <v>543537472.23931</v>
+        <v>45294789.353276</v>
       </c>
       <c r="F65" s="2"/>
       <c r="G65" s="1">
@@ -5726,7 +5726,7 @@
       </c>
       <c r="D66" s="2"/>
       <c r="E66" s="5">
-        <v>597891219.46325</v>
+        <v>49824268.288604</v>
       </c>
       <c r="F66" s="2"/>
       <c r="G66" s="1">
@@ -5802,7 +5802,7 @@
       </c>
       <c r="D67" s="2"/>
       <c r="E67" s="5">
-        <v>657680341.40957</v>
+        <v>54806695.117464</v>
       </c>
       <c r="F67" s="2"/>
       <c r="G67" s="1">
@@ -5878,7 +5878,7 @@
       </c>
       <c r="D68" s="2"/>
       <c r="E68" s="5">
-        <v>723448375.55052</v>
+        <v>60287364.62921</v>
       </c>
       <c r="F68" s="2"/>
       <c r="G68" s="1">
@@ -5954,7 +5954,7 @@
       </c>
       <c r="D69" s="2"/>
       <c r="E69" s="5">
-        <v>795793213.10557</v>
+        <v>66316101.092131</v>
       </c>
       <c r="F69" s="2"/>
       <c r="G69" s="1">
@@ -6030,7 +6030,7 @@
       </c>
       <c r="D70" s="2"/>
       <c r="E70" s="5">
-        <v>875372534.41613</v>
+        <v>72947711.201344</v>
       </c>
       <c r="F70" s="2"/>
       <c r="G70" s="1">
@@ -6106,7 +6106,7 @@
       </c>
       <c r="D71" s="2"/>
       <c r="E71" s="5">
-        <v>962909787.85774</v>
+        <v>80242482.321478</v>
       </c>
       <c r="F71" s="2"/>
       <c r="G71" s="1">
@@ -6182,7 +6182,7 @@
       </c>
       <c r="D72" s="16"/>
       <c r="E72" s="5">
-        <v>1059200766.6435</v>
+        <v>88266730.553626</v>
       </c>
       <c r="F72" s="16"/>
       <c r="G72" s="5">
@@ -6499,7 +6499,7 @@
     <col min="2" max="2" width="8.141" bestFit="true" customWidth="true" style="0"/>
     <col min="3" max="3" width="12.854" bestFit="true" customWidth="true" style="0"/>
     <col min="4" max="4" width="9.283" bestFit="true" customWidth="true" style="0"/>
-    <col min="5" max="5" width="16.425" bestFit="true" customWidth="true" style="0"/>
+    <col min="5" max="5" width="12.854" bestFit="true" customWidth="true" style="0"/>
     <col min="6" max="6" width="8.141" bestFit="true" customWidth="true" style="0"/>
     <col min="7" max="7" width="8.141" bestFit="true" customWidth="true" style="0"/>
     <col min="8" max="8" width="9.283" bestFit="true" customWidth="true" style="0"/>
@@ -6745,7 +6745,7 @@
         <v>0.1</v>
       </c>
       <c r="E7" s="5">
-        <v>2160000</v>
+        <v>180000</v>
       </c>
       <c r="F7" s="2">
         <v>0.1</v>
@@ -6813,7 +6813,7 @@
         <v>0.1</v>
       </c>
       <c r="E8" s="8">
-        <v>2376000</v>
+        <v>198000</v>
       </c>
       <c r="F8" s="9">
         <v>0.1</v>
@@ -6881,7 +6881,7 @@
         <v>0.1</v>
       </c>
       <c r="E9" s="5">
-        <v>2613600</v>
+        <v>217800</v>
       </c>
       <c r="F9" s="2">
         <v>0.1</v>
@@ -6949,7 +6949,7 @@
         <v>0.1</v>
       </c>
       <c r="E10" s="5">
-        <v>2874960</v>
+        <v>239580</v>
       </c>
       <c r="F10" s="2">
         <v>0.1</v>
@@ -7017,7 +7017,7 @@
         <v>0.1</v>
       </c>
       <c r="E11" s="5">
-        <v>3162456</v>
+        <v>263538</v>
       </c>
       <c r="F11" s="2">
         <v>0.1</v>
@@ -7085,7 +7085,7 @@
         <v>0.1</v>
       </c>
       <c r="E12" s="5">
-        <v>3478701.6</v>
+        <v>289891.8</v>
       </c>
       <c r="F12" s="2">
         <v>0.1</v>
@@ -7153,7 +7153,7 @@
         <v>0.1</v>
       </c>
       <c r="E13" s="5">
-        <v>3826571.76</v>
+        <v>318880.98</v>
       </c>
       <c r="F13" s="2">
         <v>0.1</v>
@@ -7221,7 +7221,7 @@
         <v>0.1</v>
       </c>
       <c r="E14" s="5">
-        <v>4209228.936</v>
+        <v>350769.078</v>
       </c>
       <c r="F14" s="2">
         <v>0.1</v>
@@ -7289,7 +7289,7 @@
         <v>0.1</v>
       </c>
       <c r="E15" s="5">
-        <v>4630151.8296</v>
+        <v>385845.9858</v>
       </c>
       <c r="F15" s="2">
         <v>0.1</v>
@@ -7357,7 +7357,7 @@
         <v>0.1</v>
       </c>
       <c r="E16" s="5">
-        <v>5093167.01256</v>
+        <v>424430.58438</v>
       </c>
       <c r="F16" s="2">
         <v>0.1</v>
@@ -7425,7 +7425,7 @@
         <v>0.1</v>
       </c>
       <c r="E17" s="5">
-        <v>5602483.713816</v>
+        <v>466873.642818</v>
       </c>
       <c r="F17" s="2">
         <v>0.1</v>
@@ -7493,7 +7493,7 @@
         <v>0.1</v>
       </c>
       <c r="E18" s="5">
-        <v>6162732.0851976</v>
+        <v>513561.0070998</v>
       </c>
       <c r="F18" s="2">
         <v>0.1</v>
@@ -7561,7 +7561,7 @@
         <v>0.1</v>
       </c>
       <c r="E19" s="5">
-        <v>6779005.2937174</v>
+        <v>564917.10780978</v>
       </c>
       <c r="F19" s="2">
         <v>0.1</v>
@@ -7629,7 +7629,7 @@
         <v>0.1</v>
       </c>
       <c r="E20" s="5">
-        <v>7456905.8230891</v>
+        <v>621408.81859076</v>
       </c>
       <c r="F20" s="2">
         <v>0.1</v>
@@ -7697,7 +7697,7 @@
         <v>0.1</v>
       </c>
       <c r="E21" s="5">
-        <v>8202596.4053981</v>
+        <v>683549.70044984</v>
       </c>
       <c r="F21" s="2">
         <v>0.1</v>
@@ -7765,7 +7765,7 @@
         <v>0.1</v>
       </c>
       <c r="E22" s="5">
-        <v>9022856.0459378</v>
+        <v>751904.67049482</v>
       </c>
       <c r="F22" s="2">
         <v>0.1</v>
@@ -7833,7 +7833,7 @@
         <v>0.1</v>
       </c>
       <c r="E23" s="5">
-        <v>9925141.6505316</v>
+        <v>827095.1375443</v>
       </c>
       <c r="F23" s="2">
         <v>0.1</v>
@@ -7901,7 +7901,7 @@
         <v>0.1</v>
       </c>
       <c r="E24" s="5">
-        <v>10917655.815585</v>
+        <v>909804.65129873</v>
       </c>
       <c r="F24" s="2">
         <v>0.1</v>
@@ -7969,7 +7969,7 @@
         <v>0.1</v>
       </c>
       <c r="E25" s="5">
-        <v>12009421.397143</v>
+        <v>1000785.1164286</v>
       </c>
       <c r="F25" s="2">
         <v>0.1</v>
@@ -8037,7 +8037,7 @@
         <v>0.1</v>
       </c>
       <c r="E26" s="5">
-        <v>13210363.536858</v>
+        <v>1100863.6280715</v>
       </c>
       <c r="F26" s="2">
         <v>0.1</v>
@@ -8105,7 +8105,7 @@
         <v>0.1</v>
       </c>
       <c r="E27" s="5">
-        <v>14531399.890543</v>
+        <v>1210949.9908786</v>
       </c>
       <c r="F27" s="2">
         <v>0.1</v>
@@ -8173,7 +8173,7 @@
         <v>0.1</v>
       </c>
       <c r="E28" s="5">
-        <v>15984539.879598</v>
+        <v>1332044.9899665</v>
       </c>
       <c r="F28" s="2">
         <v>0.1</v>
@@ -8241,7 +8241,7 @@
         <v>0.1</v>
       </c>
       <c r="E29" s="5">
-        <v>17582993.867558</v>
+        <v>1465249.4889632</v>
       </c>
       <c r="F29" s="2">
         <v>0.1</v>
@@ -8309,7 +8309,7 @@
         <v>0.1</v>
       </c>
       <c r="E30" s="5">
-        <v>19341293.254314</v>
+        <v>1611774.4378595</v>
       </c>
       <c r="F30" s="2">
         <v>0.1</v>
@@ -8377,7 +8377,7 @@
         <v>0.1</v>
       </c>
       <c r="E31" s="5">
-        <v>21275422.579746</v>
+        <v>1772951.8816455</v>
       </c>
       <c r="F31" s="2">
         <v>0.1</v>
@@ -8445,7 +8445,7 @@
         <v>0.1</v>
       </c>
       <c r="E32" s="5">
-        <v>23402964.837721</v>
+        <v>1950247.0698101</v>
       </c>
       <c r="F32" s="2">
         <v>0.1</v>
@@ -8513,7 +8513,7 @@
         <v>0.1</v>
       </c>
       <c r="E33" s="5">
-        <v>25743261.321493</v>
+        <v>2145271.7767911</v>
       </c>
       <c r="F33" s="2">
         <v>0.1</v>
@@ -8581,7 +8581,7 @@
         <v>0.1</v>
       </c>
       <c r="E34" s="5">
-        <v>28317587.453642</v>
+        <v>2359798.9544702</v>
       </c>
       <c r="F34" s="2">
         <v>0.1</v>
@@ -8649,7 +8649,7 @@
         <v>0.1</v>
       </c>
       <c r="E35" s="5">
-        <v>31149346.199006</v>
+        <v>2595778.8499172</v>
       </c>
       <c r="F35" s="2">
         <v>0.1</v>
@@ -8717,7 +8717,7 @@
         <v>0.1</v>
       </c>
       <c r="E36" s="5">
-        <v>34264280.818907</v>
+        <v>2855356.7349089</v>
       </c>
       <c r="F36" s="2">
         <v>0.1</v>
@@ -8785,7 +8785,7 @@
         <v>0.1</v>
       </c>
       <c r="E37" s="5">
-        <v>37690708.900798</v>
+        <v>3140892.4083998</v>
       </c>
       <c r="F37" s="2">
         <v>0.1</v>
@@ -8853,7 +8853,7 @@
         <v>0.1</v>
       </c>
       <c r="E38" s="5">
-        <v>41459779.790878</v>
+        <v>3454981.6492398</v>
       </c>
       <c r="F38" s="2">
         <v>0.1</v>
@@ -8921,7 +8921,7 @@
         <v>0.1</v>
       </c>
       <c r="E39" s="5">
-        <v>45605757.769966</v>
+        <v>3800479.8141638</v>
       </c>
       <c r="F39" s="2">
         <v>0.1</v>
@@ -8989,7 +8989,7 @@
         <v>0.1</v>
       </c>
       <c r="E40" s="11">
-        <v>50166333.546962</v>
+        <v>4180527.7955802</v>
       </c>
       <c r="F40" s="12">
         <v>0.1</v>
@@ -9057,7 +9057,7 @@
         <v>0.1</v>
       </c>
       <c r="E41" s="5">
-        <v>55182966.901658</v>
+        <v>4598580.5751382</v>
       </c>
       <c r="F41" s="2">
         <v>0.1</v>
@@ -9125,7 +9125,7 @@
         <v>0.1</v>
       </c>
       <c r="E42" s="5">
-        <v>60701263.591824</v>
+        <v>5058438.632652</v>
       </c>
       <c r="F42" s="2">
         <v>0.1</v>
@@ -9193,7 +9193,7 @@
         <v>0.1</v>
       </c>
       <c r="E43" s="5">
-        <v>66771389.951006</v>
+        <v>5564282.4959172</v>
       </c>
       <c r="F43" s="2">
         <v>0.1</v>
@@ -9261,7 +9261,7 @@
         <v>0.1</v>
       </c>
       <c r="E44" s="5">
-        <v>73448528.946107</v>
+        <v>6120710.7455089</v>
       </c>
       <c r="F44" s="2">
         <v>0.1</v>
@@ -9329,7 +9329,7 @@
         <v>0.1</v>
       </c>
       <c r="E45" s="5">
-        <v>80793381.840718</v>
+        <v>6732781.8200598</v>
       </c>
       <c r="F45" s="2">
         <v>0.1</v>
@@ -9397,7 +9397,7 @@
         <v>0.1</v>
       </c>
       <c r="E46" s="5">
-        <v>88872720.02479</v>
+        <v>7406060.0020658</v>
       </c>
       <c r="F46" s="2">
         <v>0.1</v>
@@ -9465,7 +9465,7 @@
         <v>0.1</v>
       </c>
       <c r="E47" s="5">
-        <v>97759992.027269</v>
+        <v>8146666.0022724</v>
       </c>
       <c r="F47" s="2">
         <v>0.1</v>
@@ -9533,7 +9533,7 @@
         <v>0.1</v>
       </c>
       <c r="E48" s="5">
-        <v>107535991.23</v>
+        <v>8961332.6024996</v>
       </c>
       <c r="F48" s="2">
         <v>0.1</v>
@@ -9601,7 +9601,7 @@
         <v>0.1</v>
       </c>
       <c r="E49" s="5">
-        <v>118289590.353</v>
+        <v>9857465.8627496</v>
       </c>
       <c r="F49" s="2">
         <v>0.1</v>
@@ -9669,7 +9669,7 @@
         <v>0.1</v>
       </c>
       <c r="E50" s="5">
-        <v>130118549.3883</v>
+        <v>10843212.449025</v>
       </c>
       <c r="F50" s="2">
         <v>0.1</v>
@@ -9737,7 +9737,7 @@
         <v>0.1</v>
       </c>
       <c r="E51" s="5">
-        <v>143130404.32714</v>
+        <v>11927533.693928</v>
       </c>
       <c r="F51" s="2">
         <v>0.1</v>
@@ -9805,7 +9805,7 @@
         <v>0.1</v>
       </c>
       <c r="E52" s="5">
-        <v>157443444.75985</v>
+        <v>13120287.063321</v>
       </c>
       <c r="F52" s="2">
         <v>0.1</v>
@@ -9871,7 +9871,7 @@
       </c>
       <c r="D53" s="14"/>
       <c r="E53" s="13">
-        <v>173187789.23584</v>
+        <v>14432315.769653</v>
       </c>
       <c r="F53" s="14">
         <v>0.1</v>
@@ -9937,7 +9937,7 @@
       </c>
       <c r="D54" s="2"/>
       <c r="E54" s="5">
-        <v>190506568.15942</v>
+        <v>15875547.346618</v>
       </c>
       <c r="F54" s="2">
         <v>0.1</v>
@@ -10003,7 +10003,7 @@
       </c>
       <c r="D55" s="2"/>
       <c r="E55" s="5">
-        <v>209557224.97536</v>
+        <v>17463102.08128</v>
       </c>
       <c r="F55" s="2">
         <v>0.1</v>
@@ -10069,7 +10069,7 @@
       </c>
       <c r="D56" s="2"/>
       <c r="E56" s="5">
-        <v>230512947.4729</v>
+        <v>19209412.289408</v>
       </c>
       <c r="F56" s="2">
         <v>0.1</v>
@@ -10135,7 +10135,7 @@
       </c>
       <c r="D57" s="14"/>
       <c r="E57" s="13">
-        <v>253564242.22019</v>
+        <v>21130353.518349</v>
       </c>
       <c r="F57" s="14">
         <v>0.1</v>
@@ -10201,7 +10201,7 @@
       </c>
       <c r="D58" s="2"/>
       <c r="E58" s="5">
-        <v>278920666.44221</v>
+        <v>23243388.870184</v>
       </c>
       <c r="F58" s="2">
         <v>0.1</v>
@@ -10267,7 +10267,7 @@
       </c>
       <c r="D59" s="2"/>
       <c r="E59" s="5">
-        <v>306812733.08642</v>
+        <v>25567727.757202</v>
       </c>
       <c r="F59" s="2">
         <v>0.1</v>
@@ -10333,7 +10333,7 @@
       </c>
       <c r="D60" s="2"/>
       <c r="E60" s="5">
-        <v>337494006.39506</v>
+        <v>28124500.532922</v>
       </c>
       <c r="F60" s="2">
         <v>0.1</v>
@@ -10399,7 +10399,7 @@
       </c>
       <c r="D61" s="2"/>
       <c r="E61" s="5">
-        <v>371243407.03457</v>
+        <v>30936950.586214</v>
       </c>
       <c r="F61" s="2">
         <v>0.1</v>
@@ -10465,7 +10465,7 @@
       </c>
       <c r="D62" s="2"/>
       <c r="E62" s="5">
-        <v>408367747.73802</v>
+        <v>34030645.644835</v>
       </c>
       <c r="F62" s="2">
         <v>0.1</v>
@@ -10531,7 +10531,7 @@
       </c>
       <c r="D63" s="2"/>
       <c r="E63" s="5">
-        <v>449204522.51183</v>
+        <v>37433710.209319</v>
       </c>
       <c r="F63" s="2">
         <v>0.1</v>
@@ -10597,7 +10597,7 @@
       </c>
       <c r="D64" s="2"/>
       <c r="E64" s="5">
-        <v>494124974.76301</v>
+        <v>41177081.230251</v>
       </c>
       <c r="F64" s="2">
         <v>0.1</v>
@@ -10663,7 +10663,7 @@
       </c>
       <c r="D65" s="2"/>
       <c r="E65" s="5">
-        <v>543537472.23931</v>
+        <v>45294789.353276</v>
       </c>
       <c r="F65" s="2">
         <v>0.1</v>
@@ -10729,7 +10729,7 @@
       </c>
       <c r="D66" s="2"/>
       <c r="E66" s="5">
-        <v>597891219.46325</v>
+        <v>49824268.288604</v>
       </c>
       <c r="F66" s="2">
         <v>0.1</v>
@@ -10795,7 +10795,7 @@
       </c>
       <c r="D67" s="2"/>
       <c r="E67" s="5">
-        <v>657680341.40957</v>
+        <v>54806695.117464</v>
       </c>
       <c r="F67" s="2">
         <v>0.1</v>
@@ -10861,7 +10861,7 @@
       </c>
       <c r="D68" s="2"/>
       <c r="E68" s="5">
-        <v>723448375.55052</v>
+        <v>60287364.62921</v>
       </c>
       <c r="F68" s="2">
         <v>0.1</v>
@@ -10927,7 +10927,7 @@
       </c>
       <c r="D69" s="2"/>
       <c r="E69" s="5">
-        <v>795793213.10557</v>
+        <v>66316101.092131</v>
       </c>
       <c r="F69" s="2">
         <v>0.1</v>
@@ -10993,7 +10993,7 @@
       </c>
       <c r="D70" s="2"/>
       <c r="E70" s="5">
-        <v>875372534.41613</v>
+        <v>72947711.201344</v>
       </c>
       <c r="F70" s="2">
         <v>0.1</v>
@@ -11059,7 +11059,7 @@
       </c>
       <c r="D71" s="2"/>
       <c r="E71" s="5">
-        <v>962909787.85774</v>
+        <v>80242482.321478</v>
       </c>
       <c r="F71" s="2">
         <v>0.1</v>
@@ -11125,7 +11125,7 @@
       </c>
       <c r="D72" s="16"/>
       <c r="E72" s="5">
-        <v>1059200766.6435</v>
+        <v>88266730.553626</v>
       </c>
       <c r="F72" s="16">
         <v>0.1</v>

</xml_diff>

<commit_message>
Major refactoring to more consistent naming convention between configured datastructure and calculated data structure - to make less misunderstandings
</commit_message>
<xml_diff>
--- a/tests/Feature/config/fond_tenpercent.xlsx
+++ b/tests/Feature/config/fond_tenpercent.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="private" sheetId="1" r:id="rId4"/>
     <sheet name="Income" sheetId="2" r:id="rId5"/>
-    <sheet name="fond privat" sheetId="3" r:id="rId6"/>
+    <sheet name="fond" sheetId="3" r:id="rId6"/>
     <sheet name="Statistics" sheetId="4" r:id="rId7"/>
   </sheets>
   <definedNames/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="131">
   <si>
     <t>private</t>
   </si>
@@ -144,448 +144,445 @@
   </si>
   <si>
     <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous value: 0 Asset rule  no transferResource &amp;&amp; transferRule
+Using previous amount: 0 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
     <t xml:space="preserve">Income no transferResource &amp;&amp; transferRule
-Using current value: 15000 * 12 Asset rule  no transferResource &amp;&amp; transferRule
+Using current amount: 15000 * 12 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
     <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous value: 198000 Asset rule  no transferResource &amp;&amp; transferRule
+Using previous amount: 198000 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
     <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous value: 217800 Asset rule  no transferResource &amp;&amp; transferRule
+Using previous amount: 217800 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
     <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous value: 239580 Asset rule  no transferResource &amp;&amp; transferRule
+Using previous amount: 239580 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
     <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous value: 263538 Asset rule  no transferResource &amp;&amp; transferRule
+Using previous amount: 263538 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
     <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous value: 289892 Asset rule  no transferResource &amp;&amp; transferRule
+Using previous amount: 289892 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
     <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous value: 318881 Asset rule  no transferResource &amp;&amp; transferRule
+Using previous amount: 318881 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
     <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous value: 350769 Asset rule  no transferResource &amp;&amp; transferRule
+Using previous amount: 350769 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
     <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous value: 385846 Asset rule  no transferResource &amp;&amp; transferRule
+Using previous amount: 385846 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
     <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous value: 424431 Asset rule  no transferResource &amp;&amp; transferRule
+Using previous amount: 424431 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
     <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous value: 466874 Asset rule  no transferResource &amp;&amp; transferRule
+Using previous amount: 466874 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
     <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous value: 513561 Asset rule  no transferResource &amp;&amp; transferRule
+Using previous amount: 513561 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
     <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous value: 564917 Asset rule  no transferResource &amp;&amp; transferRule
+Using previous amount: 564917 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
     <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous value: 621409 Asset rule  no transferResource &amp;&amp; transferRule
+Using previous amount: 621409 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
     <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous value: 683550 Asset rule  no transferResource &amp;&amp; transferRule
+Using previous amount: 683550 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
     <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous value: 751905 Asset rule  no transferResource &amp;&amp; transferRule
+Using previous amount: 751905 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
     <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous value: 827095 Asset rule  no transferResource &amp;&amp; transferRule
+Using previous amount: 827095 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
     <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous value: 909805 Asset rule  no transferResource &amp;&amp; transferRule
+Using previous amount: 909805 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
     <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous value: 1000785 Asset rule  no transferResource &amp;&amp; transferRule
+Using previous amount: 1000785 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
     <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous value: 1100864 Asset rule  no transferResource &amp;&amp; transferRule
+Using previous amount: 1100864 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
     <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous value: 1210950 Asset rule  no transferResource &amp;&amp; transferRule
+Using previous amount: 1210950 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
     <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous value: 1332045 Asset rule  no transferResource &amp;&amp; transferRule
+Using previous amount: 1332045 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
     <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous value: 1465249 Asset rule  no transferResource &amp;&amp; transferRule
+Using previous amount: 1465249 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
     <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous value: 1611774 Asset rule  no transferResource &amp;&amp; transferRule
+Using previous amount: 1611774 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
     <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous value: 1772952 Asset rule  no transferResource &amp;&amp; transferRule
+Using previous amount: 1772952 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
     <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous value: 1950247 Asset rule  no transferResource &amp;&amp; transferRule
+Using previous amount: 1950247 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
     <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous value: 2145272 Asset rule  no transferResource &amp;&amp; transferRule
+Using previous amount: 2145272 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
     <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous value: 2359799 Asset rule  no transferResource &amp;&amp; transferRule
+Using previous amount: 2359799 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
     <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous value: 2595779 Asset rule  no transferResource &amp;&amp; transferRule
+Using previous amount: 2595779 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
     <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous value: 2855357 Asset rule  no transferResource &amp;&amp; transferRule
+Using previous amount: 2855357 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
     <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous value: 3140892 Asset rule  no transferResource &amp;&amp; transferRule
+Using previous amount: 3140892 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
     <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous value: 3454982 Asset rule  no transferResource &amp;&amp; transferRule
+Using previous amount: 3454982 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
     <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous value: 3800480 Asset rule  no transferResource &amp;&amp; transferRule
+Using previous amount: 3800480 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
     <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous value: 4180528 Asset rule  no transferResource &amp;&amp; transferRule
+Using previous amount: 4180528 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
     <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous value: 4598581 Asset rule  no transferResource &amp;&amp; transferRule
+Using previous amount: 4598581 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
     <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous value: 5058439 Asset rule  no transferResource &amp;&amp; transferRule
+Using previous amount: 5058439 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
     <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous value: 5564282 Asset rule  no transferResource &amp;&amp; transferRule
+Using previous amount: 5564282 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
     <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous value: 6120711 Asset rule  no transferResource &amp;&amp; transferRule
+Using previous amount: 6120711 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
     <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous value: 6732782 Asset rule  no transferResource &amp;&amp; transferRule
+Using previous amount: 6732782 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
     <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous value: 7406060 Asset rule  no transferResource &amp;&amp; transferRule
+Using previous amount: 7406060 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
     <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous value: 8146666 Asset rule  no transferResource &amp;&amp; transferRule
+Using previous amount: 8146666 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
     <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous value: 8961333 Asset rule  no transferResource &amp;&amp; transferRule
+Using previous amount: 8961333 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
     <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous value: 9857466 Asset rule  no transferResource &amp;&amp; transferRule
+Using previous amount: 9857466 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
     <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous value: 10843212 Asset rule  no transferResource &amp;&amp; transferRule
+Using previous amount: 10843212 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
     <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous value: 11927534 Asset rule  no transferResource &amp;&amp; transferRule
+Using previous amount: 11927534 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
     <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous value: 13120287 Asset rule  no transferResource &amp;&amp; transferRule
+Using previous amount: 13120287 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
     <t xml:space="preserve">Pensioned, no more salary from here no transferResource &amp;&amp; transferRule
-Using previous value: 14432316 Asset rule  no transferResource &amp;&amp; transferRule
+Using previous amount: 14432316 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
     <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous value: 15875547 Asset rule  no transferResource &amp;&amp; transferRule
+Using previous amount: 15875547 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
     <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous value: 17463102 Asset rule  no transferResource &amp;&amp; transferRule
+Using previous amount: 17463102 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
     <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous value: 19209412 Asset rule  no transferResource &amp;&amp; transferRule
+Using previous amount: 19209412 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
     <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous value: 21130354 Asset rule  no transferResource &amp;&amp; transferRule
+Using previous amount: 21130354 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
     <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous value: 23243389 Asset rule  no transferResource &amp;&amp; transferRule
+Using previous amount: 23243389 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
     <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous value: 25567728 Asset rule  no transferResource &amp;&amp; transferRule
+Using previous amount: 25567728 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
     <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous value: 28124501 Asset rule  no transferResource &amp;&amp; transferRule
+Using previous amount: 28124501 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
     <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous value: 30936951 Asset rule  no transferResource &amp;&amp; transferRule
+Using previous amount: 30936951 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
     <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous value: 34030646 Asset rule  no transferResource &amp;&amp; transferRule
+Using previous amount: 34030646 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
     <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous value: 37433710 Asset rule  no transferResource &amp;&amp; transferRule
+Using previous amount: 37433710 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
     <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous value: 41177081 Asset rule  no transferResource &amp;&amp; transferRule
+Using previous amount: 41177081 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
     <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous value: 45294789 Asset rule  no transferResource &amp;&amp; transferRule
+Using previous amount: 45294789 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
     <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous value: 49824268 Asset rule  no transferResource &amp;&amp; transferRule
+Using previous amount: 49824268 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
     <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous value: 54806695 Asset rule  no transferResource &amp;&amp; transferRule
+Using previous amount: 54806695 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
     <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous value: 60287365 Asset rule  no transferResource &amp;&amp; transferRule
+Using previous amount: 60287365 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
     <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous value: 66316101 Asset rule  no transferResource &amp;&amp; transferRule
+Using previous amount: 66316101 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
     <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous value: 72947711 Asset rule  no transferResource &amp;&amp; transferRule
+Using previous amount: 72947711 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
     <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous value: 80242482 Asset rule  no transferResource &amp;&amp; transferRule
+Using previous amount: 80242482 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
     <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous value: 88266731 Asset rule  no transferResource &amp;&amp; transferRule
+Using previous amount: 88266731 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
-  </si>
-  <si>
-    <t>fond privat</t>
   </si>
   <si>
     <t>fond</t>
   </si>
   <si>
     <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous value: 0 Asset rule +5000 no transferResource &amp;&amp; transferRule
+Using previous amount: 0 Asset rule +5000 no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
     <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous value: 0Uttak fra 2068, 1/20 Asset rule +5000Divisor is: 544181 new rule: 1/19 transfer 544181 to income.2068.income.amount reduce fond.2068 by 544181
+Using previous amount: 0Uttak fra 2068, 1/20 Asset rule +5000Divisor is: 544181 new rule: 1/19 transfer 544181 to income.2068.income.amount reduce fond.2068 by 544181
 </t>
   </si>
   <si>
     <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous value: 0 Asset rule +5000Divisor is: 598862 new rule: 1/18 transfer 598862 to income.2069.income.amount reduce fond.2069 by 598862
+Using previous amount: 0 Asset rule +5000Divisor is: 598862 new rule: 1/18 transfer 598862 to income.2069.income.amount reduce fond.2069 by 598862
 </t>
   </si>
   <si>
     <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous value: 0 Asset rule +5000Divisor is: 659026 new rule: 1/17 transfer 659026 to income.2070.income.amount reduce fond.2070 by 659026
+Using previous amount: 0 Asset rule +5000Divisor is: 659026 new rule: 1/17 transfer 659026 to income.2070.income.amount reduce fond.2070 by 659026
 </t>
   </si>
   <si>
     <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous value: 0 Asset rule +5000Divisor is: 725223 new rule: 1/16 transfer 725223 to income.2071.income.amount reduce fond.2071 by 725223
+Using previous amount: 0 Asset rule +5000Divisor is: 725223 new rule: 1/16 transfer 725223 to income.2071.income.amount reduce fond.2071 by 725223
 </t>
   </si>
   <si>
     <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous value: 0 Asset rule +5000Divisor is: 798058 new rule: 1/15 transfer 798058 to income.2072.income.amount reduce fond.2072 by 798058
+Using previous amount: 0 Asset rule +5000Divisor is: 798058 new rule: 1/15 transfer 798058 to income.2072.income.amount reduce fond.2072 by 798058
 </t>
   </si>
   <si>
     <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous value: 0 Asset rule +5000Divisor is: 878197 new rule: 1/14 transfer 878197 to income.2073.income.amount reduce fond.2073 by 878197
+Using previous amount: 0 Asset rule +5000Divisor is: 878197 new rule: 1/14 transfer 878197 to income.2073.income.amount reduce fond.2073 by 878197
 </t>
   </si>
   <si>
     <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous value: 0 Asset rule +5000Divisor is: 966373 new rule: 1/13 transfer 966373 to income.2074.income.amount reduce fond.2074 by 966373
+Using previous amount: 0 Asset rule +5000Divisor is: 966373 new rule: 1/13 transfer 966373 to income.2074.income.amount reduce fond.2074 by 966373
 </t>
   </si>
   <si>
     <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous value: 0 Asset rule +5000Divisor is: 1063395 new rule: 1/12 transfer 1063395 to income.2075.income.amount reduce fond.2075 by 1063395
+Using previous amount: 0 Asset rule +5000Divisor is: 1063395 new rule: 1/12 transfer 1063395 to income.2075.income.amount reduce fond.2075 by 1063395
 </t>
   </si>
   <si>
     <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous value: 0 Asset rule +5000Divisor is: 1170152 new rule: 1/11 transfer 1170152 to income.2076.income.amount reduce fond.2076 by 1170152
+Using previous amount: 0 Asset rule +5000Divisor is: 1170152 new rule: 1/11 transfer 1170152 to income.2076.income.amount reduce fond.2076 by 1170152
 </t>
   </si>
   <si>
     <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous value: 0 Asset rule +5000Divisor is: 1287621 new rule: 1/10 transfer 1287621 to income.2077.income.amount reduce fond.2077 by 1287621
+Using previous amount: 0 Asset rule +5000Divisor is: 1287621 new rule: 1/10 transfer 1287621 to income.2077.income.amount reduce fond.2077 by 1287621
 </t>
   </si>
   <si>
     <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous value: 0 Asset rule +5000Divisor is: 1416884 new rule: 1/9 transfer 1416884 to income.2078.income.amount reduce fond.2078 by 1416884
+Using previous amount: 0 Asset rule +5000Divisor is: 1416884 new rule: 1/9 transfer 1416884 to income.2078.income.amount reduce fond.2078 by 1416884
 </t>
   </si>
   <si>
     <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous value: 0 Asset rule +5000Divisor is: 1559128 new rule: 1/8 transfer 1559128 to income.2079.income.amount reduce fond.2079 by 1559128
+Using previous amount: 0 Asset rule +5000Divisor is: 1559128 new rule: 1/8 transfer 1559128 to income.2079.income.amount reduce fond.2079 by 1559128
 </t>
   </si>
   <si>
     <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous value: 0 Asset rule +5000Divisor is: 1715665 new rule: 1/7 transfer 1715665 to income.2080.income.amount reduce fond.2080 by 1715665
+Using previous amount: 0 Asset rule +5000Divisor is: 1715665 new rule: 1/7 transfer 1715665 to income.2080.income.amount reduce fond.2080 by 1715665
 </t>
   </si>
   <si>
     <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous value: 0 Asset rule +5000Divisor is: 1887946 new rule: 1/6 transfer 1887946 to income.2081.income.amount reduce fond.2081 by 1887946
+Using previous amount: 0 Asset rule +5000Divisor is: 1887946 new rule: 1/6 transfer 1887946 to income.2081.income.amount reduce fond.2081 by 1887946
 </t>
   </si>
   <si>
     <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous value: 0 Asset rule +5000Divisor is: 2077574 new rule: 1/5 transfer 2077574 to income.2082.income.amount reduce fond.2082 by 2077574
+Using previous amount: 0 Asset rule +5000Divisor is: 2077574 new rule: 1/5 transfer 2077574 to income.2082.income.amount reduce fond.2082 by 2077574
 </t>
   </si>
   <si>
     <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous value: 0 Asset rule +5000Divisor is: 2286332 new rule: 1/4 transfer 2286332 to income.2083.income.amount reduce fond.2083 by 2286332
+Using previous amount: 0 Asset rule +5000Divisor is: 2286332 new rule: 1/4 transfer 2286332 to income.2083.income.amount reduce fond.2083 by 2286332
 </t>
   </si>
   <si>
     <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous value: 0 Asset rule +5000Divisor is: 2516215 new rule: 1/3 transfer 2516215 to income.2084.income.amount reduce fond.2084 by 2516215
+Using previous amount: 0 Asset rule +5000Divisor is: 2516215 new rule: 1/3 transfer 2516215 to income.2084.income.amount reduce fond.2084 by 2516215
 </t>
   </si>
   <si>
     <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous value: 0 Asset rule +5000Divisor is: 2769503 new rule: 1/2 transfer 2769503 to income.2085.income.amount reduce fond.2085 by 2769503
+Using previous amount: 0 Asset rule +5000Divisor is: 2769503 new rule: 1/2 transfer 2769503 to income.2085.income.amount reduce fond.2085 by 2769503
 </t>
   </si>
   <si>
     <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous value: 0 Asset rule +5000Divisor is: 3048953 new rule: 1/1 transfer 3048953 to income.2086.income.amount reduce fond.2086 by 3048953
+Using previous amount: 0 Asset rule +5000Divisor is: 3048953 new rule: 1/1 transfer 3048953 to income.2086.income.amount reduce fond.2086 by 3048953
 </t>
   </si>
   <si>
     <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous value: 0 Asset rule +5000Divisor is: 3358848 new rule:  transfer 3358848 to income.2087.income.amount reduce fond.2087 by 3358848
+Using previous amount: 0 Asset rule +5000Divisor is: 3358848 new rule:  transfer 3358848 to income.2087.income.amount reduce fond.2087 by 3358848
 </t>
   </si>
   <si>
@@ -11432,8 +11429,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="13.997" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="13.997" bestFit="true" customWidth="true" style="0"/>
+    <col min="1" max="1" width="10.569" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="6.998" bestFit="true" customWidth="true" style="0"/>
     <col min="3" max="3" width="9.283" bestFit="true" customWidth="true" style="0"/>
     <col min="4" max="4" width="9.283" bestFit="true" customWidth="true" style="0"/>
     <col min="5" max="5" width="8.141" bestFit="true" customWidth="true" style="0"/>
@@ -11482,7 +11479,7 @@
         <v>3</v>
       </c>
       <c r="F2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G2" t="s">
         <v>4</v>
@@ -11863,7 +11860,7 @@
       </c>
       <c r="AC9" s="2"/>
       <c r="AD9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="10" spans="1:31">
@@ -11931,7 +11928,7 @@
       </c>
       <c r="AC10" s="2"/>
       <c r="AD10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="11" spans="1:31">
@@ -11999,7 +11996,7 @@
       </c>
       <c r="AC11" s="2"/>
       <c r="AD11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="12" spans="1:31">
@@ -12067,7 +12064,7 @@
       </c>
       <c r="AC12" s="2"/>
       <c r="AD12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="13" spans="1:31">
@@ -12135,7 +12132,7 @@
       </c>
       <c r="AC13" s="2"/>
       <c r="AD13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="14" spans="1:31">
@@ -12203,7 +12200,7 @@
       </c>
       <c r="AC14" s="2"/>
       <c r="AD14" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="15" spans="1:31">
@@ -12271,7 +12268,7 @@
       </c>
       <c r="AC15" s="2"/>
       <c r="AD15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="16" spans="1:31">
@@ -12339,7 +12336,7 @@
       </c>
       <c r="AC16" s="2"/>
       <c r="AD16" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="17" spans="1:31">
@@ -12407,7 +12404,7 @@
       </c>
       <c r="AC17" s="2"/>
       <c r="AD17" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="18" spans="1:31">
@@ -12475,7 +12472,7 @@
       </c>
       <c r="AC18" s="2"/>
       <c r="AD18" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="19" spans="1:31">
@@ -12543,7 +12540,7 @@
       </c>
       <c r="AC19" s="2"/>
       <c r="AD19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="20" spans="1:31">
@@ -12611,7 +12608,7 @@
       </c>
       <c r="AC20" s="2"/>
       <c r="AD20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="21" spans="1:31">
@@ -12679,7 +12676,7 @@
       </c>
       <c r="AC21" s="2"/>
       <c r="AD21" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="22" spans="1:31">
@@ -12747,7 +12744,7 @@
       </c>
       <c r="AC22" s="2"/>
       <c r="AD22" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="23" spans="1:31">
@@ -12815,7 +12812,7 @@
       </c>
       <c r="AC23" s="2"/>
       <c r="AD23" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="24" spans="1:31">
@@ -12883,7 +12880,7 @@
       </c>
       <c r="AC24" s="2"/>
       <c r="AD24" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="25" spans="1:31">
@@ -12951,7 +12948,7 @@
       </c>
       <c r="AC25" s="2"/>
       <c r="AD25" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="26" spans="1:31">
@@ -13019,7 +13016,7 @@
       </c>
       <c r="AC26" s="2"/>
       <c r="AD26" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="27" spans="1:31">
@@ -13087,7 +13084,7 @@
       </c>
       <c r="AC27" s="2"/>
       <c r="AD27" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="28" spans="1:31">
@@ -13155,7 +13152,7 @@
       </c>
       <c r="AC28" s="2"/>
       <c r="AD28" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="29" spans="1:31">
@@ -13223,7 +13220,7 @@
       </c>
       <c r="AC29" s="2"/>
       <c r="AD29" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="30" spans="1:31">
@@ -13291,7 +13288,7 @@
       </c>
       <c r="AC30" s="2"/>
       <c r="AD30" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="31" spans="1:31">
@@ -13359,7 +13356,7 @@
       </c>
       <c r="AC31" s="2"/>
       <c r="AD31" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="32" spans="1:31">
@@ -13427,7 +13424,7 @@
       </c>
       <c r="AC32" s="2"/>
       <c r="AD32" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="33" spans="1:31">
@@ -13495,7 +13492,7 @@
       </c>
       <c r="AC33" s="2"/>
       <c r="AD33" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="34" spans="1:31">
@@ -13563,7 +13560,7 @@
       </c>
       <c r="AC34" s="2"/>
       <c r="AD34" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="35" spans="1:31">
@@ -13631,7 +13628,7 @@
       </c>
       <c r="AC35" s="2"/>
       <c r="AD35" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="36" spans="1:31">
@@ -13699,7 +13696,7 @@
       </c>
       <c r="AC36" s="2"/>
       <c r="AD36" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="37" spans="1:31">
@@ -13767,7 +13764,7 @@
       </c>
       <c r="AC37" s="2"/>
       <c r="AD37" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="38" spans="1:31">
@@ -13835,7 +13832,7 @@
       </c>
       <c r="AC38" s="2"/>
       <c r="AD38" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="39" spans="1:31">
@@ -13903,7 +13900,7 @@
       </c>
       <c r="AC39" s="2"/>
       <c r="AD39" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="40" spans="1:31">
@@ -13971,7 +13968,7 @@
       </c>
       <c r="AC40" s="12"/>
       <c r="AD40" s="10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="41" spans="1:31">
@@ -14039,7 +14036,7 @@
       </c>
       <c r="AC41" s="2"/>
       <c r="AD41" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="42" spans="1:31">
@@ -14107,7 +14104,7 @@
       </c>
       <c r="AC42" s="2"/>
       <c r="AD42" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="43" spans="1:31">
@@ -14175,7 +14172,7 @@
       </c>
       <c r="AC43" s="2"/>
       <c r="AD43" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="44" spans="1:31">
@@ -14243,7 +14240,7 @@
       </c>
       <c r="AC44" s="2"/>
       <c r="AD44" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="45" spans="1:31">
@@ -14311,7 +14308,7 @@
       </c>
       <c r="AC45" s="2"/>
       <c r="AD45" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="46" spans="1:31">
@@ -14379,7 +14376,7 @@
       </c>
       <c r="AC46" s="2"/>
       <c r="AD46" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="47" spans="1:31">
@@ -14447,7 +14444,7 @@
       </c>
       <c r="AC47" s="2"/>
       <c r="AD47" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="48" spans="1:31">
@@ -14515,7 +14512,7 @@
       </c>
       <c r="AC48" s="2"/>
       <c r="AD48" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="49" spans="1:31">
@@ -14583,7 +14580,7 @@
       </c>
       <c r="AC49" s="2"/>
       <c r="AD49" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="50" spans="1:31">
@@ -14651,7 +14648,7 @@
       </c>
       <c r="AC50" s="2"/>
       <c r="AD50" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="51" spans="1:31">
@@ -14719,7 +14716,7 @@
       </c>
       <c r="AC51" s="2"/>
       <c r="AD51" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="52" spans="1:31">
@@ -14787,7 +14784,7 @@
       </c>
       <c r="AC52" s="2"/>
       <c r="AD52" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="53" spans="1:31">
@@ -14855,7 +14852,7 @@
       </c>
       <c r="AC53" s="14"/>
       <c r="AD53" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="54" spans="1:31">
@@ -14923,7 +14920,7 @@
       </c>
       <c r="AC54" s="2"/>
       <c r="AD54" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="55" spans="1:31">
@@ -14991,7 +14988,7 @@
       </c>
       <c r="AC55" s="2"/>
       <c r="AD55" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="56" spans="1:31">
@@ -15059,7 +15056,7 @@
       </c>
       <c r="AC56" s="2"/>
       <c r="AD56" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="57" spans="1:31">
@@ -15127,7 +15124,7 @@
       </c>
       <c r="AC57" s="14"/>
       <c r="AD57" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="58" spans="1:31">
@@ -15195,7 +15192,7 @@
       </c>
       <c r="AC58" s="2"/>
       <c r="AD58" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="59" spans="1:31">
@@ -15263,7 +15260,7 @@
       </c>
       <c r="AC59" s="2"/>
       <c r="AD59" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="60" spans="1:31">
@@ -15331,7 +15328,7 @@
       </c>
       <c r="AC60" s="2"/>
       <c r="AD60" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="61" spans="1:31">
@@ -15399,7 +15396,7 @@
       </c>
       <c r="AC61" s="2"/>
       <c r="AD61" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="62" spans="1:31">
@@ -15467,7 +15464,7 @@
       </c>
       <c r="AC62" s="2"/>
       <c r="AD62" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="63" spans="1:31">
@@ -15535,7 +15532,7 @@
       </c>
       <c r="AC63" s="2"/>
       <c r="AD63" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="64" spans="1:31">
@@ -15603,7 +15600,7 @@
       </c>
       <c r="AC64" s="2"/>
       <c r="AD64" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="65" spans="1:31">
@@ -15671,7 +15668,7 @@
       </c>
       <c r="AC65" s="2"/>
       <c r="AD65" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="66" spans="1:31">
@@ -15739,7 +15736,7 @@
       </c>
       <c r="AC66" s="2"/>
       <c r="AD66" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="67" spans="1:31">
@@ -15807,7 +15804,7 @@
       </c>
       <c r="AC67" s="2"/>
       <c r="AD67" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="68" spans="1:31">
@@ -15875,7 +15872,7 @@
       </c>
       <c r="AC68" s="2"/>
       <c r="AD68" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="69" spans="1:31">
@@ -15943,7 +15940,7 @@
       </c>
       <c r="AC69" s="2"/>
       <c r="AD69" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="70" spans="1:31">
@@ -16011,7 +16008,7 @@
       </c>
       <c r="AC70" s="2"/>
       <c r="AD70" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="71" spans="1:31">
@@ -16079,7 +16076,7 @@
       </c>
       <c r="AC71" s="2"/>
       <c r="AD71" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="72" spans="1:31">
@@ -16145,7 +16142,7 @@
       </c>
       <c r="AC72" s="16"/>
       <c r="AD72" s="15" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="73" spans="1:31">
@@ -16403,10 +16400,10 @@
   <sheetData>
     <row r="5" spans="1:3">
       <c r="B5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="6" spans="1:3">

</xml_diff>

<commit_message>
Decent deposited amount handling added - gives a good feeling of dividend growth
</commit_message>
<xml_diff>
--- a/tests/Feature/config/fond_tenpercent.xlsx
+++ b/tests/Feature/config/fond_tenpercent.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="132">
   <si>
     <t>private</t>
   </si>
@@ -146,356 +146,359 @@
     <t>income</t>
   </si>
   <si>
-    <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous amount: 0 Asset rule  no transferResource &amp;&amp; transferRule
+    <t xml:space="preserve">Using previous amount: 0 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Income no transferResource &amp;&amp; transferRule
-Using current amount: 15000 * 12 Asset rule  no transferResource &amp;&amp; transferRule
+    <t xml:space="preserve">IncomeUsing current amount: 15000 * 12 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
-    <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous amount: 198000 Asset rule  no transferResource &amp;&amp; transferRule
+    <t xml:space="preserve">Using previous amount: 198000 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
-    <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous amount: 217800 Asset rule  no transferResource &amp;&amp; transferRule
+    <t xml:space="preserve">Using previous amount: 217800 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
-    <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous amount: 239580 Asset rule  no transferResource &amp;&amp; transferRule
+    <t xml:space="preserve">Using previous amount: 239580 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
-    <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous amount: 263538 Asset rule  no transferResource &amp;&amp; transferRule
+    <t xml:space="preserve">Using previous amount: 263538 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
-    <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous amount: 289892 Asset rule  no transferResource &amp;&amp; transferRule
+    <t xml:space="preserve">Using previous amount: 289892 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
-    <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous amount: 318881 Asset rule  no transferResource &amp;&amp; transferRule
+    <t xml:space="preserve">Using previous amount: 318881 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
-    <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous amount: 350769 Asset rule  no transferResource &amp;&amp; transferRule
+    <t xml:space="preserve">Using previous amount: 350769 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
-    <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous amount: 385846 Asset rule  no transferResource &amp;&amp; transferRule
+    <t xml:space="preserve">Using previous amount: 385846 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
-    <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous amount: 424431 Asset rule  no transferResource &amp;&amp; transferRule
+    <t xml:space="preserve">Using previous amount: 424431 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
-    <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous amount: 466874 Asset rule  no transferResource &amp;&amp; transferRule
+    <t xml:space="preserve">Using previous amount: 466874 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
-    <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous amount: 513561 Asset rule  no transferResource &amp;&amp; transferRule
+    <t xml:space="preserve">Using previous amount: 513561 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
-    <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous amount: 564917 Asset rule  no transferResource &amp;&amp; transferRule
+    <t xml:space="preserve">Using previous amount: 564917 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
-    <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous amount: 621409 Asset rule  no transferResource &amp;&amp; transferRule
+    <t xml:space="preserve">Using previous amount: 621409 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
-    <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous amount: 683550 Asset rule  no transferResource &amp;&amp; transferRule
+    <t xml:space="preserve">Using previous amount: 683550 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
-    <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous amount: 751905 Asset rule  no transferResource &amp;&amp; transferRule
+    <t xml:space="preserve">Using previous amount: 751905 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
-    <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous amount: 827095 Asset rule  no transferResource &amp;&amp; transferRule
+    <t xml:space="preserve">Using previous amount: 827095 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
-    <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous amount: 909805 Asset rule  no transferResource &amp;&amp; transferRule
+    <t xml:space="preserve">Using previous amount: 909805 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
-    <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous amount: 1000785 Asset rule  no transferResource &amp;&amp; transferRule
+    <t xml:space="preserve">Using previous amount: 1000785 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
-    <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous amount: 1100864 Asset rule  no transferResource &amp;&amp; transferRule
+    <t xml:space="preserve">Using previous amount: 1100864 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
-    <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous amount: 1210950 Asset rule  no transferResource &amp;&amp; transferRule
+    <t xml:space="preserve">Using previous amount: 1210950 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
-    <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous amount: 1332045 Asset rule  no transferResource &amp;&amp; transferRule
+    <t xml:space="preserve">Using previous amount: 1332045 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
-    <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous amount: 1465249 Asset rule  no transferResource &amp;&amp; transferRule
+    <t xml:space="preserve">Using previous amount: 1465249 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
-    <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous amount: 1611774 Asset rule  no transferResource &amp;&amp; transferRule
+    <t xml:space="preserve">Using previous amount: 1611774 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
-    <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous amount: 1772952 Asset rule  no transferResource &amp;&amp; transferRule
+    <t xml:space="preserve">Using previous amount: 1772952 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
-    <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous amount: 1950247 Asset rule  no transferResource &amp;&amp; transferRule
+    <t xml:space="preserve">Using previous amount: 1950247 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
-    <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous amount: 2145272 Asset rule  no transferResource &amp;&amp; transferRule
+    <t xml:space="preserve">Using previous amount: 2145272 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
-    <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous amount: 2359799 Asset rule  no transferResource &amp;&amp; transferRule
+    <t xml:space="preserve">Using previous amount: 2359799 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
-    <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous amount: 2595779 Asset rule  no transferResource &amp;&amp; transferRule
+    <t xml:space="preserve">Using previous amount: 2595779 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
-    <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous amount: 2855357 Asset rule  no transferResource &amp;&amp; transferRule
+    <t xml:space="preserve">Using previous amount: 2855357 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
-    <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous amount: 3140892 Asset rule  no transferResource &amp;&amp; transferRule
+    <t xml:space="preserve">Using previous amount: 3140892 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
-    <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous amount: 3454982 Asset rule  no transferResource &amp;&amp; transferRule
+    <t xml:space="preserve">Using previous amount: 3454982 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
-    <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous amount: 3800480 Asset rule  no transferResource &amp;&amp; transferRule
+    <t xml:space="preserve">Using previous amount: 3800480 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
-    <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous amount: 4180528 Asset rule  no transferResource &amp;&amp; transferRule
+    <t xml:space="preserve">Using previous amount: 4180528 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
-    <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous amount: 4598581 Asset rule  no transferResource &amp;&amp; transferRule
+    <t xml:space="preserve">Using previous amount: 4598581 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
-    <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous amount: 5058439 Asset rule  no transferResource &amp;&amp; transferRule
+    <t xml:space="preserve">Using previous amount: 5058439 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
-    <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous amount: 5564282 Asset rule  no transferResource &amp;&amp; transferRule
+    <t xml:space="preserve">Using previous amount: 5564282 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
-    <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous amount: 6120711 Asset rule  no transferResource &amp;&amp; transferRule
+    <t xml:space="preserve">Using previous amount: 6120711 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
-    <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous amount: 6732782 Asset rule  no transferResource &amp;&amp; transferRule
+    <t xml:space="preserve">Using previous amount: 6732782 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
-    <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous amount: 7406060 Asset rule  no transferResource &amp;&amp; transferRule
+    <t xml:space="preserve">Using previous amount: 7406060 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
-    <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous amount: 8146666 Asset rule  no transferResource &amp;&amp; transferRule
+    <t xml:space="preserve">Using previous amount: 8146666 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
-    <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous amount: 8961333 Asset rule  no transferResource &amp;&amp; transferRule
+    <t xml:space="preserve">Using previous amount: 8961333 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
-    <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous amount: 9857466 Asset rule  no transferResource &amp;&amp; transferRule
+    <t xml:space="preserve">Using previous amount: 9857466 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
-    <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous amount: 10843212 Asset rule  no transferResource &amp;&amp; transferRule
+    <t xml:space="preserve">Using previous amount: 10843212 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
-    <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous amount: 11927534 Asset rule  no transferResource &amp;&amp; transferRule
+    <t xml:space="preserve">Using previous amount: 11927534 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
-    <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous amount: 13120287 Asset rule  no transferResource &amp;&amp; transferRule
+    <t xml:space="preserve">Using previous amount: 13120287 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Pensioned, no more salary from here no transferResource &amp;&amp; transferRule
-Using previous amount: 14432316 Asset rule  no transferResource &amp;&amp; transferRule
+    <t xml:space="preserve">Pensioned, no more salary from hereUsing previous amount: 14432316 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
-    <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous amount: 15875547 Asset rule  no transferResource &amp;&amp; transferRule
+    <t xml:space="preserve">Using previous amount: 15875547 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
-    <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous amount: 17463102 Asset rule  no transferResource &amp;&amp; transferRule
+    <t xml:space="preserve">Using previous amount: 17463102 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
-    <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous amount: 19209412 Asset rule  no transferResource &amp;&amp; transferRule
+    <t xml:space="preserve">Using previous amount: 19209412 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
-    <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous amount: 21130354 Asset rule  no transferResource &amp;&amp; transferRule
+    <t xml:space="preserve">Using previous amount: 21130354 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
-    <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous amount: 23243389 Asset rule  no transferResource &amp;&amp; transferRule
+    <t xml:space="preserve">Using previous amount: 23243389 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
-    <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous amount: 25567728 Asset rule  no transferResource &amp;&amp; transferRule
+    <t xml:space="preserve">Using previous amount: 25567728 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
-    <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous amount: 28124501 Asset rule  no transferResource &amp;&amp; transferRule
+    <t xml:space="preserve">Using previous amount: 28124501 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
-    <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous amount: 30936951 Asset rule  no transferResource &amp;&amp; transferRule
+    <t xml:space="preserve">Using previous amount: 30936951 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
-    <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous amount: 34030646 Asset rule  no transferResource &amp;&amp; transferRule
+    <t xml:space="preserve">Using previous amount: 34030646 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
-    <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous amount: 37433710 Asset rule  no transferResource &amp;&amp; transferRule
+    <t xml:space="preserve">Using previous amount: 37433710 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
-    <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous amount: 41177081 Asset rule  no transferResource &amp;&amp; transferRule
+    <t xml:space="preserve">Using previous amount: 41177081 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
-    <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous amount: 45294789 Asset rule  no transferResource &amp;&amp; transferRule
+    <t xml:space="preserve">Using previous amount: 45294789 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
-    <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous amount: 49824268 Asset rule  no transferResource &amp;&amp; transferRule
+    <t xml:space="preserve">Using previous amount: 49824268 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
-    <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous amount: 54806695 Asset rule  no transferResource &amp;&amp; transferRule
+    <t xml:space="preserve">Using previous amount: 54806695 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
-    <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous amount: 60287365 Asset rule  no transferResource &amp;&amp; transferRule
+    <t xml:space="preserve">Using previous amount: 60287365 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
-    <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous amount: 66316101 Asset rule  no transferResource &amp;&amp; transferRule
+    <t xml:space="preserve">Using previous amount: 66316101 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
-    <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous amount: 72947711 Asset rule  no transferResource &amp;&amp; transferRule
+    <t xml:space="preserve">Using previous amount: 72947711 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
-    <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous amount: 80242482 Asset rule  no transferResource &amp;&amp; transferRule
+    <t xml:space="preserve">Using previous amount: 80242482 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
-    <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous amount: 88266731 Asset rule  no transferResource &amp;&amp; transferRule
+    <t xml:space="preserve">Using previous amount: 88266731 Asset rule  no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
     <t>fond</t>
   </si>
   <si>
-    <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous amount: 0 Asset rule +5000 no transferResource &amp;&amp; transferRule
+    <t xml:space="preserve">Using previous amount: 0 Asset rule +5000 no transferResource &amp;&amp; transferRule
 </t>
   </si>
   <si>
-    <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous amount: 0Uttak fra 2068, 1/20 Asset rule +50001/19 transfer 544181 to income.2068.income.amount reduce fond.2068 by 544181
+    <t xml:space="preserve">Using previous amount: 0Uttak fra 2068, 1/20 Asset rule +5000Divisor is: 544181 new rule: 1/19 transfer 544181 to income.2068.income.amount reduce fond.2068 by 544181
 </t>
   </si>
   <si>
-    <t xml:space="preserve"> no transferResource &amp;&amp; transferRule
-Using previous amount: 0 Asset rule +50000</t>
+    <t xml:space="preserve">Using previous amount: 0 Asset rule +5000Divisor is: 598862 new rule: 1/18 transfer 598862 to income.2069.income.amount reduce fond.2069 by 598862
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Using previous amount: 0 Asset rule +5000Divisor is: 659026 new rule: 1/17 transfer 659026 to income.2070.income.amount reduce fond.2070 by 659026
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Using previous amount: 0 Asset rule +5000Divisor is: 725223 new rule: 1/16 transfer 725223 to income.2071.income.amount reduce fond.2071 by 725223
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Using previous amount: 0 Asset rule +5000Divisor is: 798058 new rule: 1/15 transfer 798058 to income.2072.income.amount reduce fond.2072 by 798058
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Using previous amount: 0 Asset rule +5000Divisor is: 878197 new rule: 1/14 transfer 878197 to income.2073.income.amount reduce fond.2073 by 878197
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Using previous amount: 0 Asset rule +5000Divisor is: 966373 new rule: 1/13 transfer 966373 to income.2074.income.amount reduce fond.2074 by 966373
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Using previous amount: 0 Asset rule +5000Divisor is: 1063395 new rule: 1/12 transfer 1063395 to income.2075.income.amount reduce fond.2075 by 1063395
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Using previous amount: 0 Asset rule +5000Divisor is: 1170152 new rule: 1/11 transfer 1170152 to income.2076.income.amount reduce fond.2076 by 1170152
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Using previous amount: 0 Asset rule +5000Divisor is: 1287621 new rule: 1/10 transfer 1287621 to income.2077.income.amount reduce fond.2077 by 1287621
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Using previous amount: 0 Asset rule +5000Divisor is: 1416884 new rule: 1/9 transfer 1416884 to income.2078.income.amount reduce fond.2078 by 1416884
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Using previous amount: 0 Asset rule +5000Divisor is: 1559128 new rule: 1/8 transfer 1559128 to income.2079.income.amount reduce fond.2079 by 1559128
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Using previous amount: 0 Asset rule +5000Divisor is: 1715665 new rule: 1/7 transfer 1715665 to income.2080.income.amount reduce fond.2080 by 1715665
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Using previous amount: 0 Asset rule +5000Divisor is: 1887946 new rule: 1/6 transfer 1887946 to income.2081.income.amount reduce fond.2081 by 1887946
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Using previous amount: 0 Asset rule +5000Divisor is: 2077574 new rule: 1/5 transfer 2077574 to income.2082.income.amount reduce fond.2082 by 2077574
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Using previous amount: 0 Asset rule +5000Divisor is: 2286332 new rule: 1/4 transfer 2286332 to income.2083.income.amount reduce fond.2083 by 2286332
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Using previous amount: 0 Asset rule +5000Divisor is: 2516215 new rule: 1/3 transfer 2516215 to income.2084.income.amount reduce fond.2084 by 2516215
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Using previous amount: 0 Asset rule +5000Divisor is: 2769503 new rule: 1/2 transfer 2769503 to income.2085.income.amount reduce fond.2085 by 2769503
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Using previous amount: 0 Asset rule +5000Divisor is: 3048953 new rule: 1/1 transfer 3048953 to income.2086.income.amount reduce fond.2086 by 3048953
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Using previous amount: 0 Asset rule +5000Divisor is: 3358848 new rule:  transfer 3358848 to income.2087.income.amount reduce fond.2087 by 3358848
+</t>
   </si>
   <si>
     <t>total</t>
@@ -1259,7 +1262,7 @@
       </c>
       <c r="Q8" s="9"/>
       <c r="R8" s="8">
-        <v>100000.0</v>
+        <v>100000</v>
       </c>
       <c r="S8" s="8">
         <v>80000.0</v>
@@ -1334,7 +1337,7 @@
       </c>
       <c r="Q9" s="2"/>
       <c r="R9" s="1">
-        <v>5000.0</v>
+        <v>105000</v>
       </c>
       <c r="S9" s="1">
         <v>92000.0</v>
@@ -1409,7 +1412,7 @@
       </c>
       <c r="Q10" s="2"/>
       <c r="R10" s="1">
-        <v>5000.0</v>
+        <v>110000</v>
       </c>
       <c r="S10" s="1">
         <v>105200.0</v>
@@ -1484,7 +1487,7 @@
       </c>
       <c r="Q11" s="2"/>
       <c r="R11" s="1">
-        <v>5000.0</v>
+        <v>115000</v>
       </c>
       <c r="S11" s="1">
         <v>119720.0</v>
@@ -1559,7 +1562,7 @@
       </c>
       <c r="Q12" s="2"/>
       <c r="R12" s="1">
-        <v>5000.0</v>
+        <v>120000</v>
       </c>
       <c r="S12" s="1">
         <v>135692.0</v>
@@ -1634,7 +1637,7 @@
       </c>
       <c r="Q13" s="2"/>
       <c r="R13" s="1">
-        <v>5000.0</v>
+        <v>125000</v>
       </c>
       <c r="S13" s="1">
         <v>153261.6</v>
@@ -1709,7 +1712,7 @@
       </c>
       <c r="Q14" s="2"/>
       <c r="R14" s="1">
-        <v>5000.0</v>
+        <v>130000</v>
       </c>
       <c r="S14" s="1">
         <v>172588.0</v>
@@ -1784,7 +1787,7 @@
       </c>
       <c r="Q15" s="2"/>
       <c r="R15" s="1">
-        <v>5000.0</v>
+        <v>135000</v>
       </c>
       <c r="S15" s="1">
         <v>193847.2</v>
@@ -1859,7 +1862,7 @@
       </c>
       <c r="Q16" s="2"/>
       <c r="R16" s="1">
-        <v>5000.0</v>
+        <v>140000</v>
       </c>
       <c r="S16" s="1">
         <v>217232.0</v>
@@ -1934,7 +1937,7 @@
       </c>
       <c r="Q17" s="2"/>
       <c r="R17" s="1">
-        <v>5000.0</v>
+        <v>145000</v>
       </c>
       <c r="S17" s="1">
         <v>242955.2</v>
@@ -2009,7 +2012,7 @@
       </c>
       <c r="Q18" s="2"/>
       <c r="R18" s="1">
-        <v>5000.0</v>
+        <v>150000</v>
       </c>
       <c r="S18" s="1">
         <v>271250.4</v>
@@ -2084,7 +2087,7 @@
       </c>
       <c r="Q19" s="2"/>
       <c r="R19" s="1">
-        <v>5000.0</v>
+        <v>155000</v>
       </c>
       <c r="S19" s="1">
         <v>302375.2</v>
@@ -2159,7 +2162,7 @@
       </c>
       <c r="Q20" s="2"/>
       <c r="R20" s="1">
-        <v>5000.0</v>
+        <v>160000</v>
       </c>
       <c r="S20" s="1">
         <v>336612.8</v>
@@ -2234,7 +2237,7 @@
       </c>
       <c r="Q21" s="2"/>
       <c r="R21" s="1">
-        <v>5000.0</v>
+        <v>165000</v>
       </c>
       <c r="S21" s="1">
         <v>374274.4</v>
@@ -2309,7 +2312,7 @@
       </c>
       <c r="Q22" s="2"/>
       <c r="R22" s="1">
-        <v>5000.0</v>
+        <v>170000</v>
       </c>
       <c r="S22" s="1">
         <v>415701.6</v>
@@ -2384,7 +2387,7 @@
       </c>
       <c r="Q23" s="2"/>
       <c r="R23" s="1">
-        <v>5000.0</v>
+        <v>175000</v>
       </c>
       <c r="S23" s="1">
         <v>461272.0</v>
@@ -2459,7 +2462,7 @@
       </c>
       <c r="Q24" s="2"/>
       <c r="R24" s="1">
-        <v>5000.0</v>
+        <v>180000</v>
       </c>
       <c r="S24" s="1">
         <v>511399.2</v>
@@ -2534,7 +2537,7 @@
       </c>
       <c r="Q25" s="2"/>
       <c r="R25" s="1">
-        <v>5000.0</v>
+        <v>185000</v>
       </c>
       <c r="S25" s="1">
         <v>566539.2</v>
@@ -2609,7 +2612,7 @@
       </c>
       <c r="Q26" s="2"/>
       <c r="R26" s="1">
-        <v>5000.0</v>
+        <v>190000</v>
       </c>
       <c r="S26" s="1">
         <v>627192.8</v>
@@ -2684,7 +2687,7 @@
       </c>
       <c r="Q27" s="2"/>
       <c r="R27" s="1">
-        <v>5000.0</v>
+        <v>195000</v>
       </c>
       <c r="S27" s="1">
         <v>693912.0</v>
@@ -2759,7 +2762,7 @@
       </c>
       <c r="Q28" s="2"/>
       <c r="R28" s="1">
-        <v>5000.0</v>
+        <v>200000</v>
       </c>
       <c r="S28" s="1">
         <v>767303.2</v>
@@ -2834,7 +2837,7 @@
       </c>
       <c r="Q29" s="2"/>
       <c r="R29" s="1">
-        <v>5000.0</v>
+        <v>205000</v>
       </c>
       <c r="S29" s="1">
         <v>848033.6</v>
@@ -2909,7 +2912,7 @@
       </c>
       <c r="Q30" s="2"/>
       <c r="R30" s="1">
-        <v>5000.0</v>
+        <v>210000</v>
       </c>
       <c r="S30" s="1">
         <v>936836.8</v>
@@ -2984,7 +2987,7 @@
       </c>
       <c r="Q31" s="2"/>
       <c r="R31" s="1">
-        <v>5000.0</v>
+        <v>215000</v>
       </c>
       <c r="S31" s="1">
         <v>1034520.8</v>
@@ -3059,7 +3062,7 @@
       </c>
       <c r="Q32" s="2"/>
       <c r="R32" s="1">
-        <v>5000.0</v>
+        <v>220000</v>
       </c>
       <c r="S32" s="1">
         <v>1141972.8</v>
@@ -3134,7 +3137,7 @@
       </c>
       <c r="Q33" s="2"/>
       <c r="R33" s="1">
-        <v>5000.0</v>
+        <v>225000</v>
       </c>
       <c r="S33" s="1">
         <v>1260170.4</v>
@@ -3209,7 +3212,7 @@
       </c>
       <c r="Q34" s="2"/>
       <c r="R34" s="1">
-        <v>5000.0</v>
+        <v>230000</v>
       </c>
       <c r="S34" s="1">
         <v>1390187.2</v>
@@ -3284,7 +3287,7 @@
       </c>
       <c r="Q35" s="2"/>
       <c r="R35" s="1">
-        <v>5000.0</v>
+        <v>235000</v>
       </c>
       <c r="S35" s="1">
         <v>1533205.6</v>
@@ -3359,7 +3362,7 @@
       </c>
       <c r="Q36" s="2"/>
       <c r="R36" s="1">
-        <v>5000.0</v>
+        <v>240000</v>
       </c>
       <c r="S36" s="1">
         <v>1690526.4</v>
@@ -3434,7 +3437,7 @@
       </c>
       <c r="Q37" s="2"/>
       <c r="R37" s="1">
-        <v>5000.0</v>
+        <v>245000</v>
       </c>
       <c r="S37" s="1">
         <v>1863579.2</v>
@@ -3509,7 +3512,7 @@
       </c>
       <c r="Q38" s="2"/>
       <c r="R38" s="1">
-        <v>5000.0</v>
+        <v>250000</v>
       </c>
       <c r="S38" s="1">
         <v>2053936.8</v>
@@ -3584,7 +3587,7 @@
       </c>
       <c r="Q39" s="2"/>
       <c r="R39" s="1">
-        <v>5000.0</v>
+        <v>255000</v>
       </c>
       <c r="S39" s="1">
         <v>2263330.4</v>
@@ -3659,7 +3662,7 @@
       </c>
       <c r="Q40" s="12"/>
       <c r="R40" s="11">
-        <v>5000.0</v>
+        <v>260000</v>
       </c>
       <c r="S40" s="11">
         <v>2493663.2</v>
@@ -3734,7 +3737,7 @@
       </c>
       <c r="Q41" s="2"/>
       <c r="R41" s="1">
-        <v>5000.0</v>
+        <v>265000</v>
       </c>
       <c r="S41" s="1">
         <v>2747029.6</v>
@@ -3809,7 +3812,7 @@
       </c>
       <c r="Q42" s="2"/>
       <c r="R42" s="1">
-        <v>5000.0</v>
+        <v>270000</v>
       </c>
       <c r="S42" s="1">
         <v>3025732.8</v>
@@ -3884,7 +3887,7 @@
       </c>
       <c r="Q43" s="2"/>
       <c r="R43" s="1">
-        <v>5000.0</v>
+        <v>275000</v>
       </c>
       <c r="S43" s="1">
         <v>3332306.4</v>
@@ -3959,7 +3962,7 @@
       </c>
       <c r="Q44" s="2"/>
       <c r="R44" s="1">
-        <v>5000.0</v>
+        <v>280000</v>
       </c>
       <c r="S44" s="1">
         <v>3669536.8</v>
@@ -4034,7 +4037,7 @@
       </c>
       <c r="Q45" s="2"/>
       <c r="R45" s="1">
-        <v>5000.0</v>
+        <v>285000</v>
       </c>
       <c r="S45" s="1">
         <v>4040490.4</v>
@@ -4109,7 +4112,7 @@
       </c>
       <c r="Q46" s="2"/>
       <c r="R46" s="1">
-        <v>5000.0</v>
+        <v>290000</v>
       </c>
       <c r="S46" s="1">
         <v>4448539.2</v>
@@ -4184,7 +4187,7 @@
       </c>
       <c r="Q47" s="2"/>
       <c r="R47" s="1">
-        <v>5000.0</v>
+        <v>295000</v>
       </c>
       <c r="S47" s="1">
         <v>4897392.8</v>
@@ -4259,7 +4262,7 @@
       </c>
       <c r="Q48" s="2"/>
       <c r="R48" s="1">
-        <v>5000.0</v>
+        <v>300000</v>
       </c>
       <c r="S48" s="1">
         <v>5391132.0</v>
@@ -4334,7 +4337,7 @@
       </c>
       <c r="Q49" s="2"/>
       <c r="R49" s="1">
-        <v>5000.0</v>
+        <v>305000</v>
       </c>
       <c r="S49" s="1">
         <v>5934245.6</v>
@@ -4409,7 +4412,7 @@
       </c>
       <c r="Q50" s="2"/>
       <c r="R50" s="1">
-        <v>5000.0</v>
+        <v>310000</v>
       </c>
       <c r="S50" s="1">
         <v>6531670.4</v>
@@ -4484,7 +4487,7 @@
       </c>
       <c r="Q51" s="2"/>
       <c r="R51" s="1">
-        <v>5000.0</v>
+        <v>315000</v>
       </c>
       <c r="S51" s="1">
         <v>7188837.6</v>
@@ -4559,7 +4562,7 @@
       </c>
       <c r="Q52" s="2"/>
       <c r="R52" s="1">
-        <v>5000.0</v>
+        <v>320000</v>
       </c>
       <c r="S52" s="1">
         <v>7911721.6</v>
@@ -4634,7 +4637,7 @@
       </c>
       <c r="Q53" s="14"/>
       <c r="R53" s="13">
-        <v>5000.0</v>
+        <v>0</v>
       </c>
       <c r="S53" s="13">
         <v>8271548.8</v>
@@ -4676,7 +4679,7 @@
         <v>64</v>
       </c>
       <c r="C54" s="4">
-        <v>0</v>
+        <v>598862.0</v>
       </c>
       <c r="D54" s="2"/>
       <c r="E54" s="5">
@@ -4705,22 +4708,22 @@
         <v>0</v>
       </c>
       <c r="P54" s="6">
-        <v>0</v>
+        <v>10779518.0</v>
       </c>
       <c r="Q54" s="2"/>
       <c r="R54" s="1">
-        <v>5000.0</v>
+        <v>0</v>
       </c>
       <c r="S54" s="1">
-        <v>0.0</v>
+        <v>8623614.4</v>
       </c>
       <c r="T54" s="1"/>
       <c r="U54" s="6"/>
       <c r="V54" s="1">
-        <v>-15875547.0</v>
+        <v>-15961783.144</v>
       </c>
       <c r="W54" s="1">
-        <v>0</v>
+        <v>10779518.0</v>
       </c>
       <c r="X54" s="1"/>
       <c r="Y54" s="1">
@@ -4736,7 +4739,10 @@
         <v>0.0</v>
       </c>
       <c r="AC54">
-        <v>-15875547.0</v>
+        <v>-15444366.0</v>
+      </c>
+      <c r="AD54">
+        <v>-35.818776869244</v>
       </c>
       <c r="AE54"/>
     </row>
@@ -4748,7 +4754,7 @@
         <v>65</v>
       </c>
       <c r="C55" s="4">
-        <v>0</v>
+        <v>659026.0</v>
       </c>
       <c r="D55" s="2"/>
       <c r="E55" s="5">
@@ -4777,22 +4783,22 @@
         <v>0</v>
       </c>
       <c r="P55" s="6">
-        <v>0</v>
+        <v>11203444.0</v>
       </c>
       <c r="Q55" s="2"/>
       <c r="R55" s="1">
         <v>0</v>
       </c>
       <c r="S55" s="1">
-        <v>0.0</v>
+        <v>8962755.2</v>
       </c>
       <c r="T55" s="1"/>
       <c r="U55" s="6"/>
       <c r="V55" s="1">
-        <v>-17463102.0</v>
+        <v>-17552729.552</v>
       </c>
       <c r="W55" s="1">
-        <v>0</v>
+        <v>11203444.0</v>
       </c>
       <c r="X55" s="1"/>
       <c r="Y55" s="1">
@@ -4808,7 +4814,10 @@
         <v>0.0</v>
       </c>
       <c r="AC55">
-        <v>-17463102.0</v>
+        <v>-17014964.0</v>
+      </c>
+      <c r="AD55">
+        <v>-37.968155149434</v>
       </c>
       <c r="AE55"/>
     </row>
@@ -4820,7 +4829,7 @@
         <v>66</v>
       </c>
       <c r="C56" s="4">
-        <v>0</v>
+        <v>725223.0</v>
       </c>
       <c r="D56" s="2"/>
       <c r="E56" s="5">
@@ -4849,22 +4858,22 @@
         <v>0</v>
       </c>
       <c r="P56" s="6">
-        <v>0</v>
+        <v>11603565.0</v>
       </c>
       <c r="Q56" s="2"/>
       <c r="R56" s="1">
         <v>0</v>
       </c>
       <c r="S56" s="1">
-        <v>0.0</v>
+        <v>9282852.0</v>
       </c>
       <c r="T56" s="1"/>
       <c r="U56" s="6"/>
       <c r="V56" s="1">
-        <v>-19209412.0</v>
+        <v>-19302240.52</v>
       </c>
       <c r="W56" s="1">
-        <v>0</v>
+        <v>11603565.0</v>
       </c>
       <c r="X56" s="1"/>
       <c r="Y56" s="1">
@@ -4880,7 +4889,10 @@
         <v>0.0</v>
       </c>
       <c r="AC56">
-        <v>-19209412.0</v>
+        <v>-18745269.0</v>
+      </c>
+      <c r="AD56">
+        <v>-40.386874637234</v>
       </c>
       <c r="AE56"/>
     </row>
@@ -4892,7 +4904,7 @@
         <v>67</v>
       </c>
       <c r="C57" s="13">
-        <v>0</v>
+        <v>798058.0</v>
       </c>
       <c r="D57" s="14"/>
       <c r="E57" s="13">
@@ -4921,22 +4933,22 @@
         <v>0</v>
       </c>
       <c r="P57" s="13">
-        <v>0</v>
+        <v>11970864.0</v>
       </c>
       <c r="Q57" s="14"/>
       <c r="R57" s="13">
         <v>0</v>
       </c>
       <c r="S57" s="13">
-        <v>0.0</v>
+        <v>9576691.2</v>
       </c>
       <c r="T57" s="13"/>
       <c r="U57" s="13"/>
       <c r="V57" s="13">
-        <v>-21130353.0</v>
+        <v>-21226119.912</v>
       </c>
       <c r="W57" s="13">
-        <v>0</v>
+        <v>11970864.0</v>
       </c>
       <c r="X57" s="13"/>
       <c r="Y57" s="13">
@@ -4952,9 +4964,11 @@
         <v>0.0</v>
       </c>
       <c r="AC57" s="3">
-        <v>-21130354.0</v>
-      </c>
-      <c r="AD57" s="3"/>
+        <v>-20651519.0</v>
+      </c>
+      <c r="AD57" s="3">
+        <v>-43.128714435316</v>
+      </c>
       <c r="AE57"/>
     </row>
     <row r="58" spans="1:31">
@@ -4965,7 +4979,7 @@
         <v>68</v>
       </c>
       <c r="C58" s="4">
-        <v>0</v>
+        <v>878197.0</v>
       </c>
       <c r="D58" s="2"/>
       <c r="E58" s="5">
@@ -4994,22 +5008,22 @@
         <v>0</v>
       </c>
       <c r="P58" s="6">
-        <v>0</v>
+        <v>12294753.0</v>
       </c>
       <c r="Q58" s="2"/>
       <c r="R58" s="1">
         <v>0</v>
       </c>
       <c r="S58" s="1">
-        <v>0.0</v>
+        <v>9835802.4</v>
       </c>
       <c r="T58" s="1"/>
       <c r="U58" s="6"/>
       <c r="V58" s="1">
-        <v>-23243388.0</v>
+        <v>-23341746.024</v>
       </c>
       <c r="W58" s="1">
-        <v>0</v>
+        <v>12294753.0</v>
       </c>
       <c r="X58" s="1"/>
       <c r="Y58" s="1">
@@ -5025,7 +5039,10 @@
         <v>0.0</v>
       </c>
       <c r="AC58">
-        <v>-23243389.0</v>
+        <v>-22751599.0</v>
+      </c>
+      <c r="AD58">
+        <v>-46.262822441411</v>
       </c>
       <c r="AE58"/>
     </row>
@@ -5037,7 +5054,7 @@
         <v>69</v>
       </c>
       <c r="C59" s="4">
-        <v>0</v>
+        <v>966373.0</v>
       </c>
       <c r="D59" s="2"/>
       <c r="E59" s="5">
@@ -5066,22 +5083,22 @@
         <v>0</v>
       </c>
       <c r="P59" s="6">
-        <v>0</v>
+        <v>12562855.0</v>
       </c>
       <c r="Q59" s="2"/>
       <c r="R59" s="1">
         <v>0</v>
       </c>
       <c r="S59" s="1">
-        <v>0.0</v>
+        <v>10050284.0</v>
       </c>
       <c r="T59" s="1"/>
       <c r="U59" s="6"/>
       <c r="V59" s="1">
-        <v>-25567727.0</v>
+        <v>-25668229.84</v>
       </c>
       <c r="W59" s="1">
-        <v>0</v>
+        <v>12562855.0</v>
       </c>
       <c r="X59" s="1"/>
       <c r="Y59" s="1">
@@ -5097,7 +5114,10 @@
         <v>0.0</v>
       </c>
       <c r="AC59">
-        <v>-25567728.0</v>
+        <v>-25065214.0</v>
+      </c>
+      <c r="AD59">
+        <v>-49.87961335222</v>
       </c>
       <c r="AE59"/>
     </row>
@@ -5109,7 +5129,7 @@
         <v>70</v>
       </c>
       <c r="C60" s="4">
-        <v>0</v>
+        <v>1063395.0</v>
       </c>
       <c r="D60" s="2"/>
       <c r="E60" s="5">
@@ -5138,22 +5158,22 @@
         <v>0</v>
       </c>
       <c r="P60" s="6">
-        <v>0</v>
+        <v>12760746.0</v>
       </c>
       <c r="Q60" s="2"/>
       <c r="R60" s="1">
         <v>0</v>
       </c>
       <c r="S60" s="1">
-        <v>0.0</v>
+        <v>10208596.8</v>
       </c>
       <c r="T60" s="1"/>
       <c r="U60" s="6"/>
       <c r="V60" s="1">
-        <v>-28124500.0</v>
+        <v>-28226585.968</v>
       </c>
       <c r="W60" s="1">
-        <v>0</v>
+        <v>12760746.0</v>
       </c>
       <c r="X60" s="1"/>
       <c r="Y60" s="1">
@@ -5169,7 +5189,10 @@
         <v>0.0</v>
       </c>
       <c r="AC60">
-        <v>-28124501.0</v>
+        <v>-27614071.0</v>
+      </c>
+      <c r="AD60">
+        <v>-54.099640804699</v>
       </c>
       <c r="AE60"/>
     </row>
@@ -5181,7 +5204,7 @@
         <v>71</v>
       </c>
       <c r="C61" s="4">
-        <v>0</v>
+        <v>1170152.0</v>
       </c>
       <c r="D61" s="2"/>
       <c r="E61" s="5">
@@ -5210,22 +5233,22 @@
         <v>0</v>
       </c>
       <c r="P61" s="6">
-        <v>0</v>
+        <v>12871669.0</v>
       </c>
       <c r="Q61" s="2"/>
       <c r="R61" s="1">
         <v>0</v>
       </c>
       <c r="S61" s="1">
-        <v>0.0</v>
+        <v>10297335.2</v>
       </c>
       <c r="T61" s="1"/>
       <c r="U61" s="6"/>
       <c r="V61" s="1">
-        <v>-30936950.0</v>
+        <v>-31039923.352</v>
       </c>
       <c r="W61" s="1">
-        <v>0</v>
+        <v>12871669.0</v>
       </c>
       <c r="X61" s="1"/>
       <c r="Y61" s="1">
@@ -5241,7 +5264,10 @@
         <v>0.0</v>
       </c>
       <c r="AC61">
-        <v>-30936951.0</v>
+        <v>-30422084.0</v>
+      </c>
+      <c r="AD61">
+        <v>-59.087294740099</v>
       </c>
       <c r="AE61"/>
     </row>
@@ -5253,7 +5279,7 @@
         <v>72</v>
       </c>
       <c r="C62" s="4">
-        <v>0</v>
+        <v>1287621.0</v>
       </c>
       <c r="D62" s="2"/>
       <c r="E62" s="5">
@@ -5282,22 +5308,22 @@
         <v>0</v>
       </c>
       <c r="P62" s="6">
-        <v>0</v>
+        <v>12876215.0</v>
       </c>
       <c r="Q62" s="2"/>
       <c r="R62" s="1">
         <v>0</v>
       </c>
       <c r="S62" s="1">
-        <v>0.0</v>
+        <v>10300972.0</v>
       </c>
       <c r="T62" s="1"/>
       <c r="U62" s="6"/>
       <c r="V62" s="1">
-        <v>-34030645.0</v>
+        <v>-34133654.72</v>
       </c>
       <c r="W62" s="1">
-        <v>0</v>
+        <v>12876215.0</v>
       </c>
       <c r="X62" s="1"/>
       <c r="Y62" s="1">
@@ -5313,7 +5339,10 @@
         <v>0.0</v>
       </c>
       <c r="AC62">
-        <v>-34030646.0</v>
+        <v>-33515597.0</v>
+      </c>
+      <c r="AD62">
+        <v>-65.072688286115</v>
       </c>
       <c r="AE62"/>
     </row>
@@ -5325,7 +5354,7 @@
         <v>73</v>
       </c>
       <c r="C63" s="4">
-        <v>0</v>
+        <v>1416884.0</v>
       </c>
       <c r="D63" s="2"/>
       <c r="E63" s="5">
@@ -5354,22 +5383,22 @@
         <v>0</v>
       </c>
       <c r="P63" s="6">
-        <v>0</v>
+        <v>12751953.0</v>
       </c>
       <c r="Q63" s="2"/>
       <c r="R63" s="1">
         <v>0</v>
       </c>
       <c r="S63" s="1">
-        <v>0.0</v>
+        <v>10201562.4</v>
       </c>
       <c r="T63" s="1"/>
       <c r="U63" s="6"/>
       <c r="V63" s="1">
-        <v>-37433710.0</v>
+        <v>-37535725.624</v>
       </c>
       <c r="W63" s="1">
-        <v>0</v>
+        <v>12751953.0</v>
       </c>
       <c r="X63" s="1"/>
       <c r="Y63" s="1">
@@ -5385,7 +5414,10 @@
         <v>0.0</v>
       </c>
       <c r="AC63">
-        <v>-37433710.0</v>
+        <v>-36923632.0</v>
+      </c>
+      <c r="AD63">
+        <v>-72.388190263876</v>
       </c>
       <c r="AE63"/>
     </row>
@@ -5397,7 +5429,7 @@
         <v>74</v>
       </c>
       <c r="C64" s="4">
-        <v>0</v>
+        <v>1559128.0</v>
       </c>
       <c r="D64" s="2"/>
       <c r="E64" s="5">
@@ -5426,22 +5458,22 @@
         <v>0</v>
       </c>
       <c r="P64" s="6">
-        <v>0</v>
+        <v>12473020.0</v>
       </c>
       <c r="Q64" s="2"/>
       <c r="R64" s="1">
         <v>0</v>
       </c>
       <c r="S64" s="1">
-        <v>0.0</v>
+        <v>9978416.0</v>
       </c>
       <c r="T64" s="1"/>
       <c r="U64" s="6"/>
       <c r="V64" s="1">
-        <v>-41177081.0</v>
+        <v>-41276865.16</v>
       </c>
       <c r="W64" s="1">
-        <v>0</v>
+        <v>12473020.0</v>
       </c>
       <c r="X64" s="1"/>
       <c r="Y64" s="1">
@@ -5457,7 +5489,10 @@
         <v>0.0</v>
       </c>
       <c r="AC64">
-        <v>-41177081.0</v>
+        <v>-40678160.0</v>
+      </c>
+      <c r="AD64">
+        <v>-81.532299314841</v>
       </c>
       <c r="AE64"/>
     </row>
@@ -5469,7 +5504,7 @@
         <v>75</v>
       </c>
       <c r="C65" s="4">
-        <v>0</v>
+        <v>1715665.0</v>
       </c>
       <c r="D65" s="2"/>
       <c r="E65" s="5">
@@ -5498,22 +5533,22 @@
         <v>0</v>
       </c>
       <c r="P65" s="6">
-        <v>0</v>
+        <v>12009657.0</v>
       </c>
       <c r="Q65" s="2"/>
       <c r="R65" s="1">
         <v>0</v>
       </c>
       <c r="S65" s="1">
-        <v>0.0</v>
+        <v>9607725.6</v>
       </c>
       <c r="T65" s="1"/>
       <c r="U65" s="6"/>
       <c r="V65" s="1">
-        <v>-45294789.0</v>
+        <v>-45390866.256</v>
       </c>
       <c r="W65" s="1">
-        <v>0</v>
+        <v>12009657.0</v>
       </c>
       <c r="X65" s="1"/>
       <c r="Y65" s="1">
@@ -5529,7 +5564,10 @@
         <v>0.0</v>
       </c>
       <c r="AC65">
-        <v>-45294789.0</v>
+        <v>-44814403.0</v>
+      </c>
+      <c r="AD65">
+        <v>-93.288265851389</v>
       </c>
       <c r="AE65"/>
     </row>
@@ -5541,7 +5579,7 @@
         <v>76</v>
       </c>
       <c r="C66" s="4">
-        <v>0</v>
+        <v>1887946.0</v>
       </c>
       <c r="D66" s="2"/>
       <c r="E66" s="5">
@@ -5570,22 +5608,22 @@
         <v>0</v>
       </c>
       <c r="P66" s="6">
-        <v>0</v>
+        <v>11327677.0</v>
       </c>
       <c r="Q66" s="2"/>
       <c r="R66" s="1">
         <v>0</v>
       </c>
       <c r="S66" s="1">
-        <v>0.0</v>
+        <v>9062141.6</v>
       </c>
       <c r="T66" s="1"/>
       <c r="U66" s="6"/>
       <c r="V66" s="1">
-        <v>-49824268.0</v>
+        <v>-49914889.416</v>
       </c>
       <c r="W66" s="1">
-        <v>0</v>
+        <v>11327677.0</v>
       </c>
       <c r="X66" s="1"/>
       <c r="Y66" s="1">
@@ -5601,7 +5639,10 @@
         <v>0.0</v>
       </c>
       <c r="AC66">
-        <v>-49824268.0</v>
+        <v>-49371161.0</v>
+      </c>
+      <c r="AD66">
+        <v>-108.96135412406</v>
       </c>
       <c r="AE66"/>
     </row>
@@ -5613,7 +5654,7 @@
         <v>77</v>
       </c>
       <c r="C67" s="4">
-        <v>0</v>
+        <v>2077574.0</v>
       </c>
       <c r="D67" s="2"/>
       <c r="E67" s="5">
@@ -5642,22 +5683,22 @@
         <v>0</v>
       </c>
       <c r="P67" s="6">
-        <v>0</v>
+        <v>10387871.0</v>
       </c>
       <c r="Q67" s="2"/>
       <c r="R67" s="1">
         <v>0</v>
       </c>
       <c r="S67" s="1">
-        <v>0.0</v>
+        <v>8310296.8</v>
       </c>
       <c r="T67" s="1"/>
       <c r="U67" s="6"/>
       <c r="V67" s="1">
-        <v>-54806695.0</v>
+        <v>-54889797.968</v>
       </c>
       <c r="W67" s="1">
-        <v>0</v>
+        <v>10387871.0</v>
       </c>
       <c r="X67" s="1"/>
       <c r="Y67" s="1">
@@ -5673,7 +5714,10 @@
         <v>0.0</v>
       </c>
       <c r="AC67">
-        <v>-54806695.0</v>
+        <v>-54391180.0</v>
+      </c>
+      <c r="AD67">
+        <v>-130.90069177794</v>
       </c>
       <c r="AE67"/>
     </row>
@@ -5685,7 +5729,7 @@
         <v>78</v>
       </c>
       <c r="C68" s="4">
-        <v>0</v>
+        <v>2286332.0</v>
       </c>
       <c r="D68" s="2"/>
       <c r="E68" s="5">
@@ -5714,22 +5758,22 @@
         <v>0</v>
       </c>
       <c r="P68" s="6">
-        <v>0</v>
+        <v>9145326.0</v>
       </c>
       <c r="Q68" s="2"/>
       <c r="R68" s="1">
         <v>0</v>
       </c>
       <c r="S68" s="1">
-        <v>0.0</v>
+        <v>7316260.8</v>
       </c>
       <c r="T68" s="1"/>
       <c r="U68" s="6"/>
       <c r="V68" s="1">
-        <v>-60287364.0</v>
+        <v>-60360526.608</v>
       </c>
       <c r="W68" s="1">
-        <v>0</v>
+        <v>9145326.0</v>
       </c>
       <c r="X68" s="1"/>
       <c r="Y68" s="1">
@@ -5745,7 +5789,10 @@
         <v>0.0</v>
       </c>
       <c r="AC68">
-        <v>-60287365.0</v>
+        <v>-59921552.0</v>
+      </c>
+      <c r="AD68">
+        <v>-163.8037616155</v>
       </c>
       <c r="AE68"/>
     </row>
@@ -5757,7 +5804,7 @@
         <v>79</v>
       </c>
       <c r="C69" s="4">
-        <v>0</v>
+        <v>2516215.0</v>
       </c>
       <c r="D69" s="2"/>
       <c r="E69" s="5">
@@ -5786,22 +5833,22 @@
         <v>0</v>
       </c>
       <c r="P69" s="6">
-        <v>0</v>
+        <v>7548644.0</v>
       </c>
       <c r="Q69" s="2"/>
       <c r="R69" s="1">
         <v>0</v>
       </c>
       <c r="S69" s="1">
-        <v>0.0</v>
+        <v>6038915.2</v>
       </c>
       <c r="T69" s="1"/>
       <c r="U69" s="6"/>
       <c r="V69" s="1">
-        <v>-66316101.0</v>
+        <v>-66376490.152</v>
       </c>
       <c r="W69" s="1">
-        <v>0</v>
+        <v>7548644.0</v>
       </c>
       <c r="X69" s="1"/>
       <c r="Y69" s="1">
@@ -5817,7 +5864,10 @@
         <v>0.0</v>
       </c>
       <c r="AC69">
-        <v>-66316101.0</v>
+        <v>-66014155.0</v>
+      </c>
+      <c r="AD69">
+        <v>-218.62918359907</v>
       </c>
       <c r="AE69"/>
     </row>
@@ -5829,7 +5879,7 @@
         <v>80</v>
       </c>
       <c r="C70" s="4">
-        <v>0</v>
+        <v>2769503.0</v>
       </c>
       <c r="D70" s="2"/>
       <c r="E70" s="5">
@@ -5858,22 +5908,22 @@
         <v>0</v>
       </c>
       <c r="P70" s="6">
-        <v>0</v>
+        <v>5539005.0</v>
       </c>
       <c r="Q70" s="2"/>
       <c r="R70" s="1">
         <v>0</v>
       </c>
       <c r="S70" s="1">
-        <v>0.0</v>
+        <v>4431204.0</v>
       </c>
       <c r="T70" s="1"/>
       <c r="U70" s="6"/>
       <c r="V70" s="1">
-        <v>-72947711.0</v>
+        <v>-72992023.04</v>
       </c>
       <c r="W70" s="1">
-        <v>0</v>
+        <v>5539005.0</v>
       </c>
       <c r="X70" s="1"/>
       <c r="Y70" s="1">
@@ -5889,7 +5939,10 @@
         <v>0.0</v>
       </c>
       <c r="AC70">
-        <v>-72947711.0</v>
+        <v>-72726151.0</v>
+      </c>
+      <c r="AD70">
+        <v>-328.24555583539</v>
       </c>
       <c r="AE70"/>
     </row>
@@ -5901,7 +5954,7 @@
         <v>81</v>
       </c>
       <c r="C71" s="4">
-        <v>0</v>
+        <v>3048953.0</v>
       </c>
       <c r="D71" s="2"/>
       <c r="E71" s="5">
@@ -5930,22 +5983,22 @@
         <v>0</v>
       </c>
       <c r="P71" s="6">
-        <v>0</v>
+        <v>3048953.0</v>
       </c>
       <c r="Q71" s="2"/>
       <c r="R71" s="1">
         <v>0</v>
       </c>
       <c r="S71" s="1">
-        <v>0.0</v>
+        <v>2439162.4</v>
       </c>
       <c r="T71" s="1"/>
       <c r="U71" s="6"/>
       <c r="V71" s="1">
-        <v>-80242482.0</v>
+        <v>-80266873.624</v>
       </c>
       <c r="W71" s="1">
-        <v>0</v>
+        <v>3048953.0</v>
       </c>
       <c r="X71" s="1"/>
       <c r="Y71" s="1">
@@ -5961,7 +6014,10 @@
         <v>0.0</v>
       </c>
       <c r="AC71">
-        <v>-80242482.0</v>
+        <v>-80120524.0</v>
+      </c>
+      <c r="AD71">
+        <v>-656.95112387761</v>
       </c>
       <c r="AE71"/>
     </row>
@@ -5973,7 +6029,7 @@
         <v>82</v>
       </c>
       <c r="C72" s="5">
-        <v>0</v>
+        <v>3358848.0</v>
       </c>
       <c r="D72" s="16"/>
       <c r="E72" s="5">
@@ -6002,7 +6058,7 @@
         <v>0</v>
       </c>
       <c r="P72" s="5">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="Q72" s="16"/>
       <c r="R72" s="5">
@@ -6017,7 +6073,7 @@
         <v>-88266730.0</v>
       </c>
       <c r="W72" s="5">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="X72" s="5"/>
       <c r="Y72" s="5">
@@ -9822,7 +9878,7 @@
         <v>64</v>
       </c>
       <c r="C54" s="4">
-        <v>0</v>
+        <v>598862.0</v>
       </c>
       <c r="D54" s="2"/>
       <c r="E54" s="5">
@@ -9890,7 +9946,7 @@
         <v>65</v>
       </c>
       <c r="C55" s="4">
-        <v>0</v>
+        <v>659026.0</v>
       </c>
       <c r="D55" s="2"/>
       <c r="E55" s="5">
@@ -9958,7 +10014,7 @@
         <v>66</v>
       </c>
       <c r="C56" s="4">
-        <v>0</v>
+        <v>725223.0</v>
       </c>
       <c r="D56" s="2"/>
       <c r="E56" s="5">
@@ -10026,7 +10082,7 @@
         <v>67</v>
       </c>
       <c r="C57" s="13">
-        <v>0</v>
+        <v>798058.0</v>
       </c>
       <c r="D57" s="14"/>
       <c r="E57" s="13">
@@ -10095,7 +10151,7 @@
         <v>68</v>
       </c>
       <c r="C58" s="4">
-        <v>0</v>
+        <v>878197.0</v>
       </c>
       <c r="D58" s="2"/>
       <c r="E58" s="5">
@@ -10163,7 +10219,7 @@
         <v>69</v>
       </c>
       <c r="C59" s="4">
-        <v>0</v>
+        <v>966373.0</v>
       </c>
       <c r="D59" s="2"/>
       <c r="E59" s="5">
@@ -10231,7 +10287,7 @@
         <v>70</v>
       </c>
       <c r="C60" s="4">
-        <v>0</v>
+        <v>1063395.0</v>
       </c>
       <c r="D60" s="2"/>
       <c r="E60" s="5">
@@ -10299,7 +10355,7 @@
         <v>71</v>
       </c>
       <c r="C61" s="4">
-        <v>0</v>
+        <v>1170152.0</v>
       </c>
       <c r="D61" s="2"/>
       <c r="E61" s="5">
@@ -10367,7 +10423,7 @@
         <v>72</v>
       </c>
       <c r="C62" s="4">
-        <v>0</v>
+        <v>1287621.0</v>
       </c>
       <c r="D62" s="2"/>
       <c r="E62" s="5">
@@ -10435,7 +10491,7 @@
         <v>73</v>
       </c>
       <c r="C63" s="4">
-        <v>0</v>
+        <v>1416884.0</v>
       </c>
       <c r="D63" s="2"/>
       <c r="E63" s="5">
@@ -10503,7 +10559,7 @@
         <v>74</v>
       </c>
       <c r="C64" s="4">
-        <v>0</v>
+        <v>1559128.0</v>
       </c>
       <c r="D64" s="2"/>
       <c r="E64" s="5">
@@ -10571,7 +10627,7 @@
         <v>75</v>
       </c>
       <c r="C65" s="4">
-        <v>0</v>
+        <v>1715665.0</v>
       </c>
       <c r="D65" s="2"/>
       <c r="E65" s="5">
@@ -10639,7 +10695,7 @@
         <v>76</v>
       </c>
       <c r="C66" s="4">
-        <v>0</v>
+        <v>1887946.0</v>
       </c>
       <c r="D66" s="2"/>
       <c r="E66" s="5">
@@ -10707,7 +10763,7 @@
         <v>77</v>
       </c>
       <c r="C67" s="4">
-        <v>0</v>
+        <v>2077574.0</v>
       </c>
       <c r="D67" s="2"/>
       <c r="E67" s="5">
@@ -10775,7 +10831,7 @@
         <v>78</v>
       </c>
       <c r="C68" s="4">
-        <v>0</v>
+        <v>2286332.0</v>
       </c>
       <c r="D68" s="2"/>
       <c r="E68" s="5">
@@ -10843,7 +10899,7 @@
         <v>79</v>
       </c>
       <c r="C69" s="4">
-        <v>0</v>
+        <v>2516215.0</v>
       </c>
       <c r="D69" s="2"/>
       <c r="E69" s="5">
@@ -10911,7 +10967,7 @@
         <v>80</v>
       </c>
       <c r="C70" s="4">
-        <v>0</v>
+        <v>2769503.0</v>
       </c>
       <c r="D70" s="2"/>
       <c r="E70" s="5">
@@ -10979,7 +11035,7 @@
         <v>81</v>
       </c>
       <c r="C71" s="4">
-        <v>0</v>
+        <v>3048953.0</v>
       </c>
       <c r="D71" s="2"/>
       <c r="E71" s="5">
@@ -11047,7 +11103,7 @@
         <v>82</v>
       </c>
       <c r="C72" s="5">
-        <v>0</v>
+        <v>3358848.0</v>
       </c>
       <c r="D72" s="16"/>
       <c r="E72" s="5">
@@ -11373,7 +11429,7 @@
     <col min="18" max="18" width="18.71" bestFit="true" customWidth="true" style="0"/>
     <col min="19" max="19" width="18.71" bestFit="true" customWidth="true" style="0"/>
     <col min="20" max="20" width="9.283" bestFit="true" customWidth="true" style="0"/>
-    <col min="21" max="21" width="8.141" bestFit="true" customWidth="true" style="0"/>
+    <col min="21" max="21" width="9.283" bestFit="true" customWidth="true" style="0"/>
     <col min="22" max="22" width="10.569" bestFit="true" customWidth="true" style="0"/>
     <col min="23" max="23" width="25.851" bestFit="true" customWidth="true" style="0"/>
     <col min="24" max="24" width="5.856" bestFit="true" customWidth="true" style="0"/>
@@ -11692,7 +11748,7 @@
         <v>0.1</v>
       </c>
       <c r="R8" s="8">
-        <v>100000.0</v>
+        <v>100000</v>
       </c>
       <c r="S8" s="8">
         <v>80000.0</v>
@@ -11761,7 +11817,7 @@
         <v>0.1</v>
       </c>
       <c r="R9" s="1">
-        <v>5000.0</v>
+        <v>105000</v>
       </c>
       <c r="S9" s="1">
         <v>92000.0</v>
@@ -11829,7 +11885,7 @@
         <v>0.1</v>
       </c>
       <c r="R10" s="1">
-        <v>5000.0</v>
+        <v>110000</v>
       </c>
       <c r="S10" s="1">
         <v>105200.0</v>
@@ -11897,7 +11953,7 @@
         <v>0.1</v>
       </c>
       <c r="R11" s="1">
-        <v>5000.0</v>
+        <v>115000</v>
       </c>
       <c r="S11" s="1">
         <v>119720.0</v>
@@ -11965,7 +12021,7 @@
         <v>0.1</v>
       </c>
       <c r="R12" s="1">
-        <v>5000.0</v>
+        <v>120000</v>
       </c>
       <c r="S12" s="1">
         <v>135692.0</v>
@@ -12033,7 +12089,7 @@
         <v>0.1</v>
       </c>
       <c r="R13" s="1">
-        <v>5000.0</v>
+        <v>125000</v>
       </c>
       <c r="S13" s="1">
         <v>153261.6</v>
@@ -12101,7 +12157,7 @@
         <v>0.1</v>
       </c>
       <c r="R14" s="1">
-        <v>5000.0</v>
+        <v>130000</v>
       </c>
       <c r="S14" s="1">
         <v>172588.0</v>
@@ -12169,7 +12225,7 @@
         <v>0.1</v>
       </c>
       <c r="R15" s="1">
-        <v>5000.0</v>
+        <v>135000</v>
       </c>
       <c r="S15" s="1">
         <v>193847.2</v>
@@ -12237,7 +12293,7 @@
         <v>0.1</v>
       </c>
       <c r="R16" s="1">
-        <v>5000.0</v>
+        <v>140000</v>
       </c>
       <c r="S16" s="1">
         <v>217232.0</v>
@@ -12305,7 +12361,7 @@
         <v>0.1</v>
       </c>
       <c r="R17" s="1">
-        <v>5000.0</v>
+        <v>145000</v>
       </c>
       <c r="S17" s="1">
         <v>242955.2</v>
@@ -12373,7 +12429,7 @@
         <v>0.1</v>
       </c>
       <c r="R18" s="1">
-        <v>5000.0</v>
+        <v>150000</v>
       </c>
       <c r="S18" s="1">
         <v>271250.4</v>
@@ -12441,7 +12497,7 @@
         <v>0.1</v>
       </c>
       <c r="R19" s="1">
-        <v>5000.0</v>
+        <v>155000</v>
       </c>
       <c r="S19" s="1">
         <v>302375.2</v>
@@ -12509,7 +12565,7 @@
         <v>0.1</v>
       </c>
       <c r="R20" s="1">
-        <v>5000.0</v>
+        <v>160000</v>
       </c>
       <c r="S20" s="1">
         <v>336612.8</v>
@@ -12577,7 +12633,7 @@
         <v>0.1</v>
       </c>
       <c r="R21" s="1">
-        <v>5000.0</v>
+        <v>165000</v>
       </c>
       <c r="S21" s="1">
         <v>374274.4</v>
@@ -12645,7 +12701,7 @@
         <v>0.1</v>
       </c>
       <c r="R22" s="1">
-        <v>5000.0</v>
+        <v>170000</v>
       </c>
       <c r="S22" s="1">
         <v>415701.6</v>
@@ -12713,7 +12769,7 @@
         <v>0.1</v>
       </c>
       <c r="R23" s="1">
-        <v>5000.0</v>
+        <v>175000</v>
       </c>
       <c r="S23" s="1">
         <v>461272.0</v>
@@ -12781,7 +12837,7 @@
         <v>0.1</v>
       </c>
       <c r="R24" s="1">
-        <v>5000.0</v>
+        <v>180000</v>
       </c>
       <c r="S24" s="1">
         <v>511399.2</v>
@@ -12849,7 +12905,7 @@
         <v>0.1</v>
       </c>
       <c r="R25" s="1">
-        <v>5000.0</v>
+        <v>185000</v>
       </c>
       <c r="S25" s="1">
         <v>566539.2</v>
@@ -12917,7 +12973,7 @@
         <v>0.1</v>
       </c>
       <c r="R26" s="1">
-        <v>5000.0</v>
+        <v>190000</v>
       </c>
       <c r="S26" s="1">
         <v>627192.8</v>
@@ -12985,7 +13041,7 @@
         <v>0.1</v>
       </c>
       <c r="R27" s="1">
-        <v>5000.0</v>
+        <v>195000</v>
       </c>
       <c r="S27" s="1">
         <v>693912.0</v>
@@ -13053,7 +13109,7 @@
         <v>0.1</v>
       </c>
       <c r="R28" s="1">
-        <v>5000.0</v>
+        <v>200000</v>
       </c>
       <c r="S28" s="1">
         <v>767303.2</v>
@@ -13121,7 +13177,7 @@
         <v>0.1</v>
       </c>
       <c r="R29" s="1">
-        <v>5000.0</v>
+        <v>205000</v>
       </c>
       <c r="S29" s="1">
         <v>848033.6</v>
@@ -13189,7 +13245,7 @@
         <v>0.1</v>
       </c>
       <c r="R30" s="1">
-        <v>5000.0</v>
+        <v>210000</v>
       </c>
       <c r="S30" s="1">
         <v>936836.8</v>
@@ -13257,7 +13313,7 @@
         <v>0.1</v>
       </c>
       <c r="R31" s="1">
-        <v>5000.0</v>
+        <v>215000</v>
       </c>
       <c r="S31" s="1">
         <v>1034520.8</v>
@@ -13325,7 +13381,7 @@
         <v>0.1</v>
       </c>
       <c r="R32" s="1">
-        <v>5000.0</v>
+        <v>220000</v>
       </c>
       <c r="S32" s="1">
         <v>1141972.8</v>
@@ -13393,7 +13449,7 @@
         <v>0.1</v>
       </c>
       <c r="R33" s="1">
-        <v>5000.0</v>
+        <v>225000</v>
       </c>
       <c r="S33" s="1">
         <v>1260170.4</v>
@@ -13461,7 +13517,7 @@
         <v>0.1</v>
       </c>
       <c r="R34" s="1">
-        <v>5000.0</v>
+        <v>230000</v>
       </c>
       <c r="S34" s="1">
         <v>1390187.2</v>
@@ -13529,7 +13585,7 @@
         <v>0.1</v>
       </c>
       <c r="R35" s="1">
-        <v>5000.0</v>
+        <v>235000</v>
       </c>
       <c r="S35" s="1">
         <v>1533205.6</v>
@@ -13597,7 +13653,7 @@
         <v>0.1</v>
       </c>
       <c r="R36" s="1">
-        <v>5000.0</v>
+        <v>240000</v>
       </c>
       <c r="S36" s="1">
         <v>1690526.4</v>
@@ -13665,7 +13721,7 @@
         <v>0.1</v>
       </c>
       <c r="R37" s="1">
-        <v>5000.0</v>
+        <v>245000</v>
       </c>
       <c r="S37" s="1">
         <v>1863579.2</v>
@@ -13733,7 +13789,7 @@
         <v>0.1</v>
       </c>
       <c r="R38" s="1">
-        <v>5000.0</v>
+        <v>250000</v>
       </c>
       <c r="S38" s="1">
         <v>2053936.8</v>
@@ -13801,7 +13857,7 @@
         <v>0.1</v>
       </c>
       <c r="R39" s="1">
-        <v>5000.0</v>
+        <v>255000</v>
       </c>
       <c r="S39" s="1">
         <v>2263330.4</v>
@@ -13869,7 +13925,7 @@
         <v>0.1</v>
       </c>
       <c r="R40" s="11">
-        <v>5000.0</v>
+        <v>260000</v>
       </c>
       <c r="S40" s="11">
         <v>2493663.2</v>
@@ -13938,7 +13994,7 @@
         <v>0.1</v>
       </c>
       <c r="R41" s="1">
-        <v>5000.0</v>
+        <v>265000</v>
       </c>
       <c r="S41" s="1">
         <v>2747029.6</v>
@@ -14006,7 +14062,7 @@
         <v>0.1</v>
       </c>
       <c r="R42" s="1">
-        <v>5000.0</v>
+        <v>270000</v>
       </c>
       <c r="S42" s="1">
         <v>3025732.8</v>
@@ -14074,7 +14130,7 @@
         <v>0.1</v>
       </c>
       <c r="R43" s="1">
-        <v>5000.0</v>
+        <v>275000</v>
       </c>
       <c r="S43" s="1">
         <v>3332306.4</v>
@@ -14142,7 +14198,7 @@
         <v>0.1</v>
       </c>
       <c r="R44" s="1">
-        <v>5000.0</v>
+        <v>280000</v>
       </c>
       <c r="S44" s="1">
         <v>3669536.8</v>
@@ -14210,7 +14266,7 @@
         <v>0.1</v>
       </c>
       <c r="R45" s="1">
-        <v>5000.0</v>
+        <v>285000</v>
       </c>
       <c r="S45" s="1">
         <v>4040490.4</v>
@@ -14278,7 +14334,7 @@
         <v>0.1</v>
       </c>
       <c r="R46" s="1">
-        <v>5000.0</v>
+        <v>290000</v>
       </c>
       <c r="S46" s="1">
         <v>4448539.2</v>
@@ -14346,7 +14402,7 @@
         <v>0.1</v>
       </c>
       <c r="R47" s="1">
-        <v>5000.0</v>
+        <v>295000</v>
       </c>
       <c r="S47" s="1">
         <v>4897392.8</v>
@@ -14414,7 +14470,7 @@
         <v>0.1</v>
       </c>
       <c r="R48" s="1">
-        <v>5000.0</v>
+        <v>300000</v>
       </c>
       <c r="S48" s="1">
         <v>5391132.0</v>
@@ -14482,7 +14538,7 @@
         <v>0.1</v>
       </c>
       <c r="R49" s="1">
-        <v>5000.0</v>
+        <v>305000</v>
       </c>
       <c r="S49" s="1">
         <v>5934245.6</v>
@@ -14550,7 +14606,7 @@
         <v>0.1</v>
       </c>
       <c r="R50" s="1">
-        <v>5000.0</v>
+        <v>310000</v>
       </c>
       <c r="S50" s="1">
         <v>6531670.4</v>
@@ -14618,7 +14674,7 @@
         <v>0.1</v>
       </c>
       <c r="R51" s="1">
-        <v>5000.0</v>
+        <v>315000</v>
       </c>
       <c r="S51" s="1">
         <v>7188837.6</v>
@@ -14686,7 +14742,7 @@
         <v>0.1</v>
       </c>
       <c r="R52" s="1">
-        <v>5000.0</v>
+        <v>320000</v>
       </c>
       <c r="S52" s="1">
         <v>7911721.6</v>
@@ -14754,7 +14810,7 @@
         <v>0.1</v>
       </c>
       <c r="R53" s="13">
-        <v>5000.0</v>
+        <v>0</v>
       </c>
       <c r="S53" s="13">
         <v>8271548.8</v>
@@ -14817,26 +14873,26 @@
         <v>0</v>
       </c>
       <c r="P54" s="6">
-        <v>0</v>
+        <v>10779518.0</v>
       </c>
       <c r="Q54" s="2">
         <v>0.1</v>
       </c>
       <c r="R54" s="1">
-        <v>5000.0</v>
+        <v>0</v>
       </c>
       <c r="S54" s="1">
-        <v>0.0</v>
+        <v>8623614.4</v>
       </c>
       <c r="T54" s="1"/>
       <c r="U54" s="6">
-        <v>0.0</v>
+        <v>86236.144</v>
       </c>
       <c r="V54" s="1">
-        <v>0.0</v>
+        <v>-86236.144</v>
       </c>
       <c r="W54" s="1">
-        <v>0</v>
+        <v>10779518.0</v>
       </c>
       <c r="X54" s="1"/>
       <c r="Y54" s="1">
@@ -14850,7 +14906,7 @@
         <v>0.0</v>
       </c>
       <c r="AC54">
-        <v>0.0</v>
+        <v>431181.0</v>
       </c>
       <c r="AE54" t="s">
         <v>112</v>
@@ -14885,7 +14941,7 @@
         <v>0</v>
       </c>
       <c r="P55" s="6">
-        <v>0</v>
+        <v>11203444.0</v>
       </c>
       <c r="Q55" s="2">
         <v>0.1</v>
@@ -14894,17 +14950,17 @@
         <v>0</v>
       </c>
       <c r="S55" s="1">
-        <v>0.0</v>
+        <v>8962755.2</v>
       </c>
       <c r="T55" s="1"/>
       <c r="U55" s="6">
-        <v>0.0</v>
+        <v>89627.552</v>
       </c>
       <c r="V55" s="1">
-        <v>0.0</v>
+        <v>-89627.552</v>
       </c>
       <c r="W55" s="1">
-        <v>0</v>
+        <v>11203444.0</v>
       </c>
       <c r="X55" s="1"/>
       <c r="Y55" s="1">
@@ -14918,10 +14974,10 @@
         <v>0.0</v>
       </c>
       <c r="AC55">
-        <v>0.0</v>
+        <v>448138.0</v>
       </c>
       <c r="AE55" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="56" spans="1:31">
@@ -14953,7 +15009,7 @@
         <v>0</v>
       </c>
       <c r="P56" s="6">
-        <v>0</v>
+        <v>11603565.0</v>
       </c>
       <c r="Q56" s="2">
         <v>0.1</v>
@@ -14962,17 +15018,17 @@
         <v>0</v>
       </c>
       <c r="S56" s="1">
-        <v>0.0</v>
+        <v>9282852.0</v>
       </c>
       <c r="T56" s="1"/>
       <c r="U56" s="6">
-        <v>0.0</v>
+        <v>92828.52</v>
       </c>
       <c r="V56" s="1">
-        <v>0.0</v>
+        <v>-92828.52</v>
       </c>
       <c r="W56" s="1">
-        <v>0</v>
+        <v>11603565.0</v>
       </c>
       <c r="X56" s="1"/>
       <c r="Y56" s="1">
@@ -14986,10 +15042,10 @@
         <v>0.0</v>
       </c>
       <c r="AC56">
-        <v>0.0</v>
+        <v>464143.0</v>
       </c>
       <c r="AE56" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="57" spans="1:31">
@@ -15021,7 +15077,7 @@
         <v>0</v>
       </c>
       <c r="P57" s="13">
-        <v>0</v>
+        <v>11970864.0</v>
       </c>
       <c r="Q57" s="14">
         <v>0.1</v>
@@ -15030,17 +15086,17 @@
         <v>0</v>
       </c>
       <c r="S57" s="13">
-        <v>0.0</v>
+        <v>9576691.2</v>
       </c>
       <c r="T57" s="13"/>
       <c r="U57" s="13">
-        <v>0.0</v>
+        <v>95766.912</v>
       </c>
       <c r="V57" s="13">
-        <v>0.0</v>
+        <v>-95766.912</v>
       </c>
       <c r="W57" s="13">
-        <v>0</v>
+        <v>11970864.0</v>
       </c>
       <c r="X57" s="13"/>
       <c r="Y57" s="13">
@@ -15054,11 +15110,11 @@
         <v>0.0</v>
       </c>
       <c r="AC57" s="3">
-        <v>0.0</v>
+        <v>478835.0</v>
       </c>
       <c r="AD57" s="3"/>
       <c r="AE57" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="58" spans="1:31">
@@ -15090,7 +15146,7 @@
         <v>0</v>
       </c>
       <c r="P58" s="6">
-        <v>0</v>
+        <v>12294753.0</v>
       </c>
       <c r="Q58" s="2">
         <v>0.1</v>
@@ -15099,17 +15155,17 @@
         <v>0</v>
       </c>
       <c r="S58" s="1">
-        <v>0.0</v>
+        <v>9835802.4</v>
       </c>
       <c r="T58" s="1"/>
       <c r="U58" s="6">
-        <v>0.0</v>
+        <v>98358.024</v>
       </c>
       <c r="V58" s="1">
-        <v>0.0</v>
+        <v>-98358.024</v>
       </c>
       <c r="W58" s="1">
-        <v>0</v>
+        <v>12294753.0</v>
       </c>
       <c r="X58" s="1"/>
       <c r="Y58" s="1">
@@ -15123,10 +15179,10 @@
         <v>0.0</v>
       </c>
       <c r="AC58">
-        <v>0.0</v>
+        <v>491790.0</v>
       </c>
       <c r="AE58" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
     </row>
     <row r="59" spans="1:31">
@@ -15158,7 +15214,7 @@
         <v>0</v>
       </c>
       <c r="P59" s="6">
-        <v>0</v>
+        <v>12562855.0</v>
       </c>
       <c r="Q59" s="2">
         <v>0.1</v>
@@ -15167,17 +15223,17 @@
         <v>0</v>
       </c>
       <c r="S59" s="1">
-        <v>0.0</v>
+        <v>10050284.0</v>
       </c>
       <c r="T59" s="1"/>
       <c r="U59" s="6">
-        <v>0.0</v>
+        <v>100502.84</v>
       </c>
       <c r="V59" s="1">
-        <v>0.0</v>
+        <v>-100502.84</v>
       </c>
       <c r="W59" s="1">
-        <v>0</v>
+        <v>12562855.0</v>
       </c>
       <c r="X59" s="1"/>
       <c r="Y59" s="1">
@@ -15191,10 +15247,10 @@
         <v>0.0</v>
       </c>
       <c r="AC59">
-        <v>0.0</v>
+        <v>502514.0</v>
       </c>
       <c r="AE59" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
     </row>
     <row r="60" spans="1:31">
@@ -15226,7 +15282,7 @@
         <v>0</v>
       </c>
       <c r="P60" s="6">
-        <v>0</v>
+        <v>12760746.0</v>
       </c>
       <c r="Q60" s="2">
         <v>0.1</v>
@@ -15235,17 +15291,17 @@
         <v>0</v>
       </c>
       <c r="S60" s="1">
-        <v>0.0</v>
+        <v>10208596.8</v>
       </c>
       <c r="T60" s="1"/>
       <c r="U60" s="6">
-        <v>0.0</v>
+        <v>102085.968</v>
       </c>
       <c r="V60" s="1">
-        <v>0.0</v>
+        <v>-102085.968</v>
       </c>
       <c r="W60" s="1">
-        <v>0</v>
+        <v>12760746.0</v>
       </c>
       <c r="X60" s="1"/>
       <c r="Y60" s="1">
@@ -15259,10 +15315,10 @@
         <v>0.0</v>
       </c>
       <c r="AC60">
-        <v>0.0</v>
+        <v>510430.0</v>
       </c>
       <c r="AE60" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
     </row>
     <row r="61" spans="1:31">
@@ -15294,7 +15350,7 @@
         <v>0</v>
       </c>
       <c r="P61" s="6">
-        <v>0</v>
+        <v>12871669.0</v>
       </c>
       <c r="Q61" s="2">
         <v>0.1</v>
@@ -15303,17 +15359,17 @@
         <v>0</v>
       </c>
       <c r="S61" s="1">
-        <v>0.0</v>
+        <v>10297335.2</v>
       </c>
       <c r="T61" s="1"/>
       <c r="U61" s="6">
-        <v>0.0</v>
+        <v>102973.352</v>
       </c>
       <c r="V61" s="1">
-        <v>0.0</v>
+        <v>-102973.352</v>
       </c>
       <c r="W61" s="1">
-        <v>0</v>
+        <v>12871669.0</v>
       </c>
       <c r="X61" s="1"/>
       <c r="Y61" s="1">
@@ -15327,10 +15383,10 @@
         <v>0.0</v>
       </c>
       <c r="AC61">
-        <v>0.0</v>
+        <v>514867.0</v>
       </c>
       <c r="AE61" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
     </row>
     <row r="62" spans="1:31">
@@ -15362,7 +15418,7 @@
         <v>0</v>
       </c>
       <c r="P62" s="6">
-        <v>0</v>
+        <v>12876215.0</v>
       </c>
       <c r="Q62" s="2">
         <v>0.1</v>
@@ -15371,17 +15427,17 @@
         <v>0</v>
       </c>
       <c r="S62" s="1">
-        <v>0.0</v>
+        <v>10300972.0</v>
       </c>
       <c r="T62" s="1"/>
       <c r="U62" s="6">
-        <v>0.0</v>
+        <v>103009.72</v>
       </c>
       <c r="V62" s="1">
-        <v>0.0</v>
+        <v>-103009.72</v>
       </c>
       <c r="W62" s="1">
-        <v>0</v>
+        <v>12876215.0</v>
       </c>
       <c r="X62" s="1"/>
       <c r="Y62" s="1">
@@ -15395,10 +15451,10 @@
         <v>0.0</v>
       </c>
       <c r="AC62">
-        <v>0.0</v>
+        <v>515049.0</v>
       </c>
       <c r="AE62" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
     </row>
     <row r="63" spans="1:31">
@@ -15430,7 +15486,7 @@
         <v>0</v>
       </c>
       <c r="P63" s="6">
-        <v>0</v>
+        <v>12751953.0</v>
       </c>
       <c r="Q63" s="2">
         <v>0.1</v>
@@ -15439,17 +15495,17 @@
         <v>0</v>
       </c>
       <c r="S63" s="1">
-        <v>0.0</v>
+        <v>10201562.4</v>
       </c>
       <c r="T63" s="1"/>
       <c r="U63" s="6">
-        <v>0.0</v>
+        <v>102015.624</v>
       </c>
       <c r="V63" s="1">
-        <v>0.0</v>
+        <v>-102015.624</v>
       </c>
       <c r="W63" s="1">
-        <v>0</v>
+        <v>12751953.0</v>
       </c>
       <c r="X63" s="1"/>
       <c r="Y63" s="1">
@@ -15463,10 +15519,10 @@
         <v>0.0</v>
       </c>
       <c r="AC63">
-        <v>0.0</v>
+        <v>510078.0</v>
       </c>
       <c r="AE63" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
     </row>
     <row r="64" spans="1:31">
@@ -15498,7 +15554,7 @@
         <v>0</v>
       </c>
       <c r="P64" s="6">
-        <v>0</v>
+        <v>12473020.0</v>
       </c>
       <c r="Q64" s="2">
         <v>0.1</v>
@@ -15507,17 +15563,17 @@
         <v>0</v>
       </c>
       <c r="S64" s="1">
-        <v>0.0</v>
+        <v>9978416.0</v>
       </c>
       <c r="T64" s="1"/>
       <c r="U64" s="6">
-        <v>0.0</v>
+        <v>99784.16</v>
       </c>
       <c r="V64" s="1">
-        <v>0.0</v>
+        <v>-99784.16</v>
       </c>
       <c r="W64" s="1">
-        <v>0</v>
+        <v>12473020.0</v>
       </c>
       <c r="X64" s="1"/>
       <c r="Y64" s="1">
@@ -15531,10 +15587,10 @@
         <v>0.0</v>
       </c>
       <c r="AC64">
-        <v>0.0</v>
+        <v>498921.0</v>
       </c>
       <c r="AE64" t="s">
-        <v>112</v>
+        <v>122</v>
       </c>
     </row>
     <row r="65" spans="1:31">
@@ -15566,7 +15622,7 @@
         <v>0</v>
       </c>
       <c r="P65" s="6">
-        <v>0</v>
+        <v>12009657.0</v>
       </c>
       <c r="Q65" s="2">
         <v>0.1</v>
@@ -15575,17 +15631,17 @@
         <v>0</v>
       </c>
       <c r="S65" s="1">
-        <v>0.0</v>
+        <v>9607725.6</v>
       </c>
       <c r="T65" s="1"/>
       <c r="U65" s="6">
-        <v>0.0</v>
+        <v>96077.256</v>
       </c>
       <c r="V65" s="1">
-        <v>0.0</v>
+        <v>-96077.256</v>
       </c>
       <c r="W65" s="1">
-        <v>0</v>
+        <v>12009657.0</v>
       </c>
       <c r="X65" s="1"/>
       <c r="Y65" s="1">
@@ -15599,10 +15655,10 @@
         <v>0.0</v>
       </c>
       <c r="AC65">
-        <v>0.0</v>
+        <v>480386.0</v>
       </c>
       <c r="AE65" t="s">
-        <v>112</v>
+        <v>123</v>
       </c>
     </row>
     <row r="66" spans="1:31">
@@ -15634,7 +15690,7 @@
         <v>0</v>
       </c>
       <c r="P66" s="6">
-        <v>0</v>
+        <v>11327677.0</v>
       </c>
       <c r="Q66" s="2">
         <v>0.1</v>
@@ -15643,17 +15699,17 @@
         <v>0</v>
       </c>
       <c r="S66" s="1">
-        <v>0.0</v>
+        <v>9062141.6</v>
       </c>
       <c r="T66" s="1"/>
       <c r="U66" s="6">
-        <v>0.0</v>
+        <v>90621.416</v>
       </c>
       <c r="V66" s="1">
-        <v>0.0</v>
+        <v>-90621.416</v>
       </c>
       <c r="W66" s="1">
-        <v>0</v>
+        <v>11327677.0</v>
       </c>
       <c r="X66" s="1"/>
       <c r="Y66" s="1">
@@ -15667,10 +15723,10 @@
         <v>0.0</v>
       </c>
       <c r="AC66">
-        <v>0.0</v>
+        <v>453107.0</v>
       </c>
       <c r="AE66" t="s">
-        <v>112</v>
+        <v>124</v>
       </c>
     </row>
     <row r="67" spans="1:31">
@@ -15702,7 +15758,7 @@
         <v>0</v>
       </c>
       <c r="P67" s="6">
-        <v>0</v>
+        <v>10387871.0</v>
       </c>
       <c r="Q67" s="2">
         <v>0.1</v>
@@ -15711,17 +15767,17 @@
         <v>0</v>
       </c>
       <c r="S67" s="1">
-        <v>0.0</v>
+        <v>8310296.8</v>
       </c>
       <c r="T67" s="1"/>
       <c r="U67" s="6">
-        <v>0.0</v>
+        <v>83102.968</v>
       </c>
       <c r="V67" s="1">
-        <v>0.0</v>
+        <v>-83102.968</v>
       </c>
       <c r="W67" s="1">
-        <v>0</v>
+        <v>10387871.0</v>
       </c>
       <c r="X67" s="1"/>
       <c r="Y67" s="1">
@@ -15735,10 +15791,10 @@
         <v>0.0</v>
       </c>
       <c r="AC67">
-        <v>0.0</v>
+        <v>415515.0</v>
       </c>
       <c r="AE67" t="s">
-        <v>112</v>
+        <v>125</v>
       </c>
     </row>
     <row r="68" spans="1:31">
@@ -15770,7 +15826,7 @@
         <v>0</v>
       </c>
       <c r="P68" s="6">
-        <v>0</v>
+        <v>9145326.0</v>
       </c>
       <c r="Q68" s="2">
         <v>0.1</v>
@@ -15779,17 +15835,17 @@
         <v>0</v>
       </c>
       <c r="S68" s="1">
-        <v>0.0</v>
+        <v>7316260.8</v>
       </c>
       <c r="T68" s="1"/>
       <c r="U68" s="6">
-        <v>0.0</v>
+        <v>73162.608</v>
       </c>
       <c r="V68" s="1">
-        <v>0.0</v>
+        <v>-73162.608</v>
       </c>
       <c r="W68" s="1">
-        <v>0</v>
+        <v>9145326.0</v>
       </c>
       <c r="X68" s="1"/>
       <c r="Y68" s="1">
@@ -15803,10 +15859,10 @@
         <v>0.0</v>
       </c>
       <c r="AC68">
-        <v>0.0</v>
+        <v>365813.0</v>
       </c>
       <c r="AE68" t="s">
-        <v>112</v>
+        <v>126</v>
       </c>
     </row>
     <row r="69" spans="1:31">
@@ -15838,7 +15894,7 @@
         <v>0</v>
       </c>
       <c r="P69" s="6">
-        <v>0</v>
+        <v>7548644.0</v>
       </c>
       <c r="Q69" s="2">
         <v>0.1</v>
@@ -15847,17 +15903,17 @@
         <v>0</v>
       </c>
       <c r="S69" s="1">
-        <v>0.0</v>
+        <v>6038915.2</v>
       </c>
       <c r="T69" s="1"/>
       <c r="U69" s="6">
-        <v>0.0</v>
+        <v>60389.152</v>
       </c>
       <c r="V69" s="1">
-        <v>0.0</v>
+        <v>-60389.152</v>
       </c>
       <c r="W69" s="1">
-        <v>0</v>
+        <v>7548644.0</v>
       </c>
       <c r="X69" s="1"/>
       <c r="Y69" s="1">
@@ -15871,10 +15927,10 @@
         <v>0.0</v>
       </c>
       <c r="AC69">
-        <v>0.0</v>
+        <v>301946.0</v>
       </c>
       <c r="AE69" t="s">
-        <v>112</v>
+        <v>127</v>
       </c>
     </row>
     <row r="70" spans="1:31">
@@ -15906,7 +15962,7 @@
         <v>0</v>
       </c>
       <c r="P70" s="6">
-        <v>0</v>
+        <v>5539005.0</v>
       </c>
       <c r="Q70" s="2">
         <v>0.1</v>
@@ -15915,17 +15971,17 @@
         <v>0</v>
       </c>
       <c r="S70" s="1">
-        <v>0.0</v>
+        <v>4431204.0</v>
       </c>
       <c r="T70" s="1"/>
       <c r="U70" s="6">
-        <v>0.0</v>
+        <v>44312.04</v>
       </c>
       <c r="V70" s="1">
-        <v>0.0</v>
+        <v>-44312.04</v>
       </c>
       <c r="W70" s="1">
-        <v>0</v>
+        <v>5539005.0</v>
       </c>
       <c r="X70" s="1"/>
       <c r="Y70" s="1">
@@ -15939,10 +15995,10 @@
         <v>0.0</v>
       </c>
       <c r="AC70">
-        <v>0.0</v>
+        <v>221560.0</v>
       </c>
       <c r="AE70" t="s">
-        <v>112</v>
+        <v>128</v>
       </c>
     </row>
     <row r="71" spans="1:31">
@@ -15974,7 +16030,7 @@
         <v>0</v>
       </c>
       <c r="P71" s="6">
-        <v>0</v>
+        <v>3048953.0</v>
       </c>
       <c r="Q71" s="2">
         <v>0.1</v>
@@ -15983,17 +16039,17 @@
         <v>0</v>
       </c>
       <c r="S71" s="1">
-        <v>0.0</v>
+        <v>2439162.4</v>
       </c>
       <c r="T71" s="1"/>
       <c r="U71" s="6">
-        <v>0.0</v>
+        <v>24391.624</v>
       </c>
       <c r="V71" s="1">
-        <v>0.0</v>
+        <v>-24391.624</v>
       </c>
       <c r="W71" s="1">
-        <v>0</v>
+        <v>3048953.0</v>
       </c>
       <c r="X71" s="1"/>
       <c r="Y71" s="1">
@@ -16007,10 +16063,10 @@
         <v>0.0</v>
       </c>
       <c r="AC71">
-        <v>0.0</v>
+        <v>121958.0</v>
       </c>
       <c r="AE71" t="s">
-        <v>112</v>
+        <v>129</v>
       </c>
     </row>
     <row r="72" spans="1:31">
@@ -16042,7 +16098,7 @@
         <v>0</v>
       </c>
       <c r="P72" s="5">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="Q72" s="16">
         <v>0.1</v>
@@ -16061,7 +16117,7 @@
         <v>0.0</v>
       </c>
       <c r="W72" s="5">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="X72" s="5"/>
       <c r="Y72" s="5">
@@ -16079,7 +16135,7 @@
       </c>
       <c r="AD72" s="15"/>
       <c r="AE72" t="s">
-        <v>112</v>
+        <v>130</v>
       </c>
     </row>
     <row r="73" spans="1:31">
@@ -16332,7 +16388,7 @@
         <v>109</v>
       </c>
       <c r="C5" t="s">
-        <v>113</v>
+        <v>131</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -16855,90 +16911,198 @@
       <c r="A54">
         <v>2069</v>
       </c>
+      <c r="B54">
+        <v>100.0</v>
+      </c>
+      <c r="C54">
+        <v>100.0</v>
+      </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55">
         <v>2070</v>
       </c>
+      <c r="B55">
+        <v>100.0</v>
+      </c>
+      <c r="C55">
+        <v>100.0</v>
+      </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56">
         <v>2071</v>
       </c>
+      <c r="B56">
+        <v>100.0</v>
+      </c>
+      <c r="C56">
+        <v>100.0</v>
+      </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57">
         <v>2072</v>
       </c>
+      <c r="B57">
+        <v>100.0</v>
+      </c>
+      <c r="C57">
+        <v>100.0</v>
+      </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58">
         <v>2073</v>
       </c>
+      <c r="B58">
+        <v>100.0</v>
+      </c>
+      <c r="C58">
+        <v>100.0</v>
+      </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59">
         <v>2074</v>
       </c>
+      <c r="B59">
+        <v>100.0</v>
+      </c>
+      <c r="C59">
+        <v>100.0</v>
+      </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60">
         <v>2075</v>
       </c>
+      <c r="B60">
+        <v>100.0</v>
+      </c>
+      <c r="C60">
+        <v>100.0</v>
+      </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61">
         <v>2076</v>
       </c>
+      <c r="B61">
+        <v>100.0</v>
+      </c>
+      <c r="C61">
+        <v>100.0</v>
+      </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62">
         <v>2077</v>
       </c>
+      <c r="B62">
+        <v>100.0</v>
+      </c>
+      <c r="C62">
+        <v>100.0</v>
+      </c>
     </row>
     <row r="63" spans="1:3">
       <c r="A63">
         <v>2078</v>
       </c>
+      <c r="B63">
+        <v>100.0</v>
+      </c>
+      <c r="C63">
+        <v>100.0</v>
+      </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64">
         <v>2079</v>
       </c>
+      <c r="B64">
+        <v>100.0</v>
+      </c>
+      <c r="C64">
+        <v>100.0</v>
+      </c>
     </row>
     <row r="65" spans="1:3">
       <c r="A65">
         <v>2080</v>
       </c>
+      <c r="B65">
+        <v>100.0</v>
+      </c>
+      <c r="C65">
+        <v>100.0</v>
+      </c>
     </row>
     <row r="66" spans="1:3">
       <c r="A66">
         <v>2081</v>
       </c>
+      <c r="B66">
+        <v>100.0</v>
+      </c>
+      <c r="C66">
+        <v>100.0</v>
+      </c>
     </row>
     <row r="67" spans="1:3">
       <c r="A67">
         <v>2082</v>
       </c>
+      <c r="B67">
+        <v>100.0</v>
+      </c>
+      <c r="C67">
+        <v>100.0</v>
+      </c>
     </row>
     <row r="68" spans="1:3">
       <c r="A68">
         <v>2083</v>
       </c>
+      <c r="B68">
+        <v>100.0</v>
+      </c>
+      <c r="C68">
+        <v>100.0</v>
+      </c>
     </row>
     <row r="69" spans="1:3">
       <c r="A69">
         <v>2084</v>
       </c>
+      <c r="B69">
+        <v>100.0</v>
+      </c>
+      <c r="C69">
+        <v>100.0</v>
+      </c>
     </row>
     <row r="70" spans="1:3">
       <c r="A70">
         <v>2085</v>
       </c>
+      <c r="B70">
+        <v>100.0</v>
+      </c>
+      <c r="C70">
+        <v>100.0</v>
+      </c>
     </row>
     <row r="71" spans="1:3">
       <c r="A71">
         <v>2086</v>
+      </c>
+      <c r="B71">
+        <v>100.0</v>
+      </c>
+      <c r="C71">
+        <v>100.0</v>
       </c>
     </row>
     <row r="72" spans="1:3">

</xml_diff>

<commit_message>
NPN-8335 - removed kti-b2c templates since they are not in use
</commit_message>
<xml_diff>
--- a/tests/Feature/config/fond_tenpercent.xlsx
+++ b/tests/Feature/config/fond_tenpercent.xlsx
@@ -164,28 +164,28 @@
     <t>income</t>
   </si>
   <si>
-    <t xml:space="preserve">transfered 7978710 - 2381964.38 (tax) = 5596745.62 from fond.2068.asset.marketAmount </t>
+    <t xml:space="preserve">transfered 7978710 - 0 (tax) = 7978710 from fond.2068.asset.marketAmount </t>
   </si>
   <si>
-    <t xml:space="preserve">transfered 8776581 - 3127973.218 (tax) = 5648607.782 from fond.2069.asset.marketAmount </t>
+    <t xml:space="preserve">transfered 8776581 - 0 (tax) = 8776581 from fond.2069.asset.marketAmount </t>
   </si>
   <si>
-    <t xml:space="preserve">transfered 9654239 - 3440770.742 (tax) = 6213468.258 from fond.2070.asset.marketAmount </t>
+    <t xml:space="preserve">transfered 9654239 - 0 (tax) = 9654239 from fond.2070.asset.marketAmount </t>
   </si>
   <si>
-    <t xml:space="preserve">transfered 10619663 - 3784847.414 (tax) = 6834815.586 from fond.2071.asset.marketAmount </t>
+    <t xml:space="preserve">transfered 10619663 - 0 (tax) = 10619663 from fond.2071.asset.marketAmount </t>
   </si>
   <si>
-    <t xml:space="preserve">transfered 11681630 - 4163333.14 (tax) = 7518296.86 from fond.2072.asset.marketAmount </t>
+    <t xml:space="preserve">transfered 11681630 - 1715290 (tax) = 9966340 from fond.2072.asset.marketAmount </t>
   </si>
   <si>
-    <t xml:space="preserve">transfered 12849793 - 4579666.554 (tax) = 8270126.446 from fond.2073.asset.marketAmount </t>
+    <t xml:space="preserve">transfered 12849793 - 4579667 (tax) = 8270126 from fond.2073.asset.marketAmount </t>
   </si>
   <si>
-    <t xml:space="preserve">transfered 14134772 - 5037633.016 (tax) = 9097138.984 from fond.2074.asset.marketAmount </t>
+    <t xml:space="preserve">transfered 14134772 - 4415703 (tax) = 9719069 from fond.2074.asset.marketAmount </t>
   </si>
   <si>
-    <t xml:space="preserve">transfered 15548249 - 5541395.522 (tax) = 10006853.478 from fond.2075.asset.marketAmount </t>
+    <t xml:space="preserve">transfered 15548249 - 5541396 (tax) = 10006853 from fond.2075.asset.marketAmount </t>
   </si>
   <si>
     <t>fond</t>
@@ -781,7 +781,7 @@
     <col min="26" max="26" width="9.283" bestFit="true" customWidth="true" style="0"/>
     <col min="27" max="27" width="12.854" bestFit="true" customWidth="true" style="0"/>
     <col min="28" max="28" width="13.997" bestFit="true" customWidth="true" style="0"/>
-    <col min="29" max="29" width="11.711" bestFit="true" customWidth="true" style="0"/>
+    <col min="29" max="29" width="12.854" bestFit="true" customWidth="true" style="0"/>
     <col min="30" max="30" width="9.283" bestFit="true" customWidth="true" style="0"/>
     <col min="31" max="31" width="21.138" bestFit="true" customWidth="true" style="0"/>
     <col min="32" max="32" width="11.711" bestFit="true" customWidth="true" style="0"/>
@@ -1336,13 +1336,13 @@
       </c>
       <c r="Z9" s="9"/>
       <c r="AA9" s="8">
-        <v>1005500.0</v>
+        <v>1005311.0</v>
       </c>
       <c r="AB9" s="8">
         <v>500.0</v>
       </c>
       <c r="AC9" s="8">
-        <v>0</v>
+        <v>189.0</v>
       </c>
       <c r="AD9" s="9"/>
       <c r="AE9" s="8">
@@ -1431,17 +1431,17 @@
       </c>
       <c r="Z10" s="2"/>
       <c r="AA10" s="1">
-        <v>1111550.0</v>
+        <v>1073123.0</v>
       </c>
       <c r="AB10" s="1">
         <v>101550.0</v>
       </c>
       <c r="AC10" s="1">
-        <v>0</v>
+        <v>38427.0</v>
       </c>
       <c r="AD10" s="2"/>
       <c r="AE10" s="1">
-        <v>56630.1</v>
+        <v>56630.0</v>
       </c>
       <c r="AF10" s="2"/>
       <c r="AG10" s="1">
@@ -1526,17 +1526,17 @@
       </c>
       <c r="Z11" s="2"/>
       <c r="AA11" s="1">
-        <v>1228205.0</v>
+        <v>1147528.0</v>
       </c>
       <c r="AB11" s="1">
         <v>213205.0</v>
       </c>
       <c r="AC11" s="1">
-        <v>0</v>
+        <v>80677.0</v>
       </c>
       <c r="AD11" s="2"/>
       <c r="AE11" s="1">
-        <v>83650.61</v>
+        <v>83651.0</v>
       </c>
       <c r="AF11" s="2"/>
       <c r="AG11" s="1">
@@ -1621,17 +1621,17 @@
       </c>
       <c r="Z12" s="2"/>
       <c r="AA12" s="1">
-        <v>1342679.182</v>
+        <v>1229185.0</v>
       </c>
       <c r="AB12" s="1">
         <v>336526.0</v>
       </c>
       <c r="AC12" s="1">
-        <v>13846.818</v>
+        <v>127341.0</v>
       </c>
       <c r="AD12" s="2"/>
       <c r="AE12" s="1">
-        <v>113494.182</v>
+        <v>113495.0</v>
       </c>
       <c r="AF12" s="2"/>
       <c r="AG12" s="1">
@@ -1716,17 +1716,17 @@
       </c>
       <c r="Z13" s="2"/>
       <c r="AA13" s="1">
-        <v>1465260.12</v>
+        <v>1318817.0</v>
       </c>
       <c r="AB13" s="1">
         <v>472679.0</v>
       </c>
       <c r="AC13" s="1">
-        <v>32418.88</v>
+        <v>178862.0</v>
       </c>
       <c r="AD13" s="2"/>
       <c r="AE13" s="1">
-        <v>146443.12</v>
+        <v>146444.0</v>
       </c>
       <c r="AF13" s="2"/>
       <c r="AG13" s="1">
@@ -1811,17 +1811,17 @@
       </c>
       <c r="Z14" s="2"/>
       <c r="AA14" s="1">
-        <v>1600031.954</v>
+        <v>1417224.0</v>
       </c>
       <c r="AB14" s="1">
         <v>622947.0</v>
       </c>
       <c r="AC14" s="1">
-        <v>52915.046</v>
+        <v>235723.0</v>
       </c>
       <c r="AD14" s="2"/>
       <c r="AE14" s="1">
-        <v>182807.954</v>
+        <v>182809.0</v>
       </c>
       <c r="AF14" s="2"/>
       <c r="AG14" s="1">
@@ -1906,17 +1906,17 @@
       </c>
       <c r="Z15" s="2"/>
       <c r="AA15" s="1">
-        <v>1748212.278</v>
+        <v>1525282.0</v>
       </c>
       <c r="AB15" s="1">
         <v>788742.0</v>
       </c>
       <c r="AC15" s="1">
-        <v>75529.722</v>
+        <v>298460.0</v>
       </c>
       <c r="AD15" s="2"/>
       <c r="AE15" s="1">
-        <v>222930.278</v>
+        <v>222931.0</v>
       </c>
       <c r="AF15" s="2"/>
       <c r="AG15" s="1">
@@ -2001,17 +2001,17 @@
       </c>
       <c r="Z16" s="2"/>
       <c r="AA16" s="1">
-        <v>1911142.83</v>
+        <v>1643957.0</v>
       </c>
       <c r="AB16" s="1">
         <v>971616.0</v>
       </c>
       <c r="AC16" s="1">
-        <v>100473.17</v>
+        <v>367659.0</v>
       </c>
       <c r="AD16" s="2"/>
       <c r="AE16" s="1">
-        <v>267185.83</v>
+        <v>267187.0</v>
       </c>
       <c r="AF16" s="2"/>
       <c r="AG16" s="1">
@@ -2096,17 +2096,17 @@
       </c>
       <c r="Z17" s="2"/>
       <c r="AA17" s="1">
-        <v>2090297.946</v>
+        <v>1774310.0</v>
       </c>
       <c r="AB17" s="1">
         <v>1173278.0</v>
       </c>
       <c r="AC17" s="1">
-        <v>127980.054</v>
+        <v>443968.0</v>
       </c>
       <c r="AD17" s="2"/>
       <c r="AE17" s="1">
-        <v>315987.946</v>
+        <v>315989.0</v>
       </c>
       <c r="AF17" s="2"/>
       <c r="AG17" s="1">
@@ -2191,17 +2191,17 @@
       </c>
       <c r="Z18" s="2"/>
       <c r="AA18" s="1">
-        <v>2287300.278</v>
+        <v>1917509.0</v>
       </c>
       <c r="AB18" s="1">
         <v>1395606.0</v>
       </c>
       <c r="AC18" s="1">
-        <v>158305.722</v>
+        <v>528097.0</v>
       </c>
       <c r="AD18" s="2"/>
       <c r="AE18" s="1">
-        <v>369791.278</v>
+        <v>369792.0</v>
       </c>
       <c r="AF18" s="2"/>
       <c r="AG18" s="1">
@@ -2286,17 +2286,17 @@
       </c>
       <c r="Z19" s="2"/>
       <c r="AA19" s="1">
-        <v>2503934.952</v>
+        <v>2074839.0</v>
       </c>
       <c r="AB19" s="1">
         <v>1640667.0</v>
       </c>
       <c r="AC19" s="1">
-        <v>191732.048</v>
+        <v>620828.0</v>
       </c>
       <c r="AD19" s="2"/>
       <c r="AE19" s="1">
-        <v>429095.952</v>
+        <v>429097.0</v>
       </c>
       <c r="AF19" s="2"/>
       <c r="AG19" s="1">
@@ -2381,17 +2381,17 @@
       </c>
       <c r="Z20" s="2"/>
       <c r="AA20" s="1">
-        <v>2742164.1</v>
+        <v>2247712.0</v>
       </c>
       <c r="AB20" s="1">
         <v>1910734.0</v>
       </c>
       <c r="AC20" s="1">
-        <v>228569.9</v>
+        <v>723022.0</v>
       </c>
       <c r="AD20" s="2"/>
       <c r="AE20" s="1">
-        <v>494452.1</v>
+        <v>494453.0</v>
       </c>
       <c r="AF20" s="2"/>
       <c r="AG20" s="1">
@@ -2476,17 +2476,17 @@
       </c>
       <c r="Z21" s="2"/>
       <c r="AA21" s="1">
-        <v>3004148.854</v>
+        <v>2437684.0</v>
       </c>
       <c r="AB21" s="1">
         <v>2208307.0</v>
       </c>
       <c r="AC21" s="1">
-        <v>269158.146</v>
+        <v>835623.0</v>
       </c>
       <c r="AD21" s="2"/>
       <c r="AE21" s="1">
-        <v>566464.854</v>
+        <v>566466.0</v>
       </c>
       <c r="AF21" s="2"/>
       <c r="AG21" s="1">
@@ -2571,17 +2571,17 @@
       </c>
       <c r="Z22" s="2"/>
       <c r="AA22" s="1">
-        <v>3292262.89</v>
+        <v>2646463.0</v>
       </c>
       <c r="AB22" s="1">
         <v>2536138.0</v>
       </c>
       <c r="AC22" s="1">
-        <v>313875.11</v>
+        <v>959675.0</v>
       </c>
       <c r="AD22" s="2"/>
       <c r="AE22" s="1">
-        <v>645799.89</v>
+        <v>645801.0</v>
       </c>
       <c r="AF22" s="2"/>
       <c r="AG22" s="1">
@@ -2666,17 +2666,17 @@
       </c>
       <c r="Z23" s="2"/>
       <c r="AA23" s="1">
-        <v>3609121.434</v>
+        <v>2875932.0</v>
       </c>
       <c r="AB23" s="1">
         <v>2897252.0</v>
       </c>
       <c r="AC23" s="1">
-        <v>363130.566</v>
+        <v>1096320.0</v>
       </c>
       <c r="AD23" s="2"/>
       <c r="AE23" s="1">
-        <v>733189.434</v>
+        <v>733191.0</v>
       </c>
       <c r="AF23" s="2"/>
       <c r="AG23" s="1">
@@ -2761,17 +2761,17 @@
       </c>
       <c r="Z24" s="2"/>
       <c r="AA24" s="1">
-        <v>3957596.928</v>
+        <v>3128158.0</v>
       </c>
       <c r="AB24" s="1">
         <v>3294977.0</v>
       </c>
       <c r="AC24" s="1">
-        <v>417380.072</v>
+        <v>1246819.0</v>
       </c>
       <c r="AD24" s="2"/>
       <c r="AE24" s="1">
-        <v>829438.928</v>
+        <v>829440.0</v>
       </c>
       <c r="AF24" s="2"/>
       <c r="AG24" s="1">
@@ -2856,17 +2856,17 @@
       </c>
       <c r="Z25" s="2"/>
       <c r="AA25" s="1">
-        <v>4340851.378</v>
+        <v>3405417.0</v>
       </c>
       <c r="AB25" s="1">
         <v>3732975.0</v>
       </c>
       <c r="AC25" s="1">
-        <v>477123.622</v>
+        <v>1412558.0</v>
       </c>
       <c r="AD25" s="2"/>
       <c r="AE25" s="1">
-        <v>935434.378</v>
+        <v>935435.0</v>
       </c>
       <c r="AF25" s="2"/>
       <c r="AG25" s="1">
@@ -2951,17 +2951,17 @@
       </c>
       <c r="Z26" s="2"/>
       <c r="AA26" s="1">
-        <v>4762364.384</v>
+        <v>3710214.0</v>
       </c>
       <c r="AB26" s="1">
         <v>4215273.0</v>
       </c>
       <c r="AC26" s="1">
-        <v>542908.616</v>
+        <v>1595059.0</v>
       </c>
       <c r="AD26" s="2"/>
       <c r="AE26" s="1">
-        <v>1052150.384</v>
+        <v>1052151.0</v>
       </c>
       <c r="AF26" s="2"/>
       <c r="AG26" s="1">
@@ -3046,17 +3046,17 @@
       </c>
       <c r="Z27" s="2"/>
       <c r="AA27" s="1">
-        <v>5225958.984</v>
+        <v>4045300.0</v>
       </c>
       <c r="AB27" s="1">
         <v>4746300.0</v>
       </c>
       <c r="AC27" s="1">
-        <v>615341.016</v>
+        <v>1796000.0</v>
       </c>
       <c r="AD27" s="2"/>
       <c r="AE27" s="1">
-        <v>1180658.984</v>
+        <v>1180660.0</v>
       </c>
       <c r="AF27" s="2"/>
       <c r="AG27" s="1">
@@ -3141,17 +3141,17 @@
       </c>
       <c r="Z28" s="2"/>
       <c r="AA28" s="1">
-        <v>5735845.444</v>
+        <v>4413706.0</v>
       </c>
       <c r="AB28" s="1">
         <v>5330930.0</v>
       </c>
       <c r="AC28" s="1">
-        <v>695084.556</v>
+        <v>2017224.0</v>
       </c>
       <c r="AD28" s="2"/>
       <c r="AE28" s="1">
-        <v>1322139.444</v>
+        <v>1322140.0</v>
       </c>
       <c r="AF28" s="2"/>
       <c r="AG28" s="1">
@@ -3236,17 +3236,17 @@
       </c>
       <c r="Z29" s="2"/>
       <c r="AA29" s="1">
-        <v>6296651.95</v>
+        <v>4818763.0</v>
       </c>
       <c r="AB29" s="1">
         <v>5974523.0</v>
       </c>
       <c r="AC29" s="1">
-        <v>782871.05</v>
+        <v>2260760.0</v>
       </c>
       <c r="AD29" s="2"/>
       <c r="AE29" s="1">
-        <v>1477888.95</v>
+        <v>1477890.0</v>
       </c>
       <c r="AF29" s="2"/>
       <c r="AG29" s="1">
@@ -3331,17 +3331,17 @@
       </c>
       <c r="Z30" s="2"/>
       <c r="AA30" s="1">
-        <v>6913471.4</v>
+        <v>5264137.0</v>
       </c>
       <c r="AB30" s="1">
         <v>6682975.0</v>
       </c>
       <c r="AC30" s="1">
-        <v>879503.6</v>
+        <v>2528838.0</v>
       </c>
       <c r="AD30" s="2"/>
       <c r="AE30" s="1">
-        <v>1649334.4</v>
+        <v>1649335.0</v>
       </c>
       <c r="AF30" s="2"/>
       <c r="AG30" s="1">
@@ -3426,17 +3426,17 @@
       </c>
       <c r="Z31" s="2"/>
       <c r="AA31" s="1">
-        <v>7591905.406</v>
+        <v>5753860.0</v>
       </c>
       <c r="AB31" s="1">
         <v>7462773.0</v>
       </c>
       <c r="AC31" s="1">
-        <v>985867.594</v>
+        <v>2823913.0</v>
       </c>
       <c r="AD31" s="2"/>
       <c r="AE31" s="1">
-        <v>1838045.406</v>
+        <v>1838046.0</v>
       </c>
       <c r="AF31" s="2"/>
       <c r="AG31" s="1">
@@ -3521,17 +3521,17 @@
       </c>
       <c r="Z32" s="2"/>
       <c r="AA32" s="1">
-        <v>8338113.506</v>
+        <v>6292365.0</v>
       </c>
       <c r="AB32" s="1">
         <v>8321050.0</v>
       </c>
       <c r="AC32" s="1">
-        <v>1102936.494</v>
+        <v>3148685.0</v>
       </c>
       <c r="AD32" s="2"/>
       <c r="AE32" s="1">
-        <v>2045748.506</v>
+        <v>2045749.0</v>
       </c>
       <c r="AF32" s="2"/>
       <c r="AG32" s="1">
@@ -3616,17 +3616,17 @@
       </c>
       <c r="Z33" s="2"/>
       <c r="AA33" s="1">
-        <v>9158873.916</v>
+        <v>6884531.0</v>
       </c>
       <c r="AB33" s="1">
         <v>9265655.0</v>
       </c>
       <c r="AC33" s="1">
-        <v>1231781.084</v>
+        <v>3506124.0</v>
       </c>
       <c r="AD33" s="2"/>
       <c r="AE33" s="1">
-        <v>2274342.916</v>
+        <v>2274343.0</v>
       </c>
       <c r="AF33" s="2"/>
       <c r="AG33" s="1">
@@ -3711,17 +3711,17 @@
       </c>
       <c r="Z34" s="2"/>
       <c r="AA34" s="1">
-        <v>10061642.778</v>
+        <v>7535725.0</v>
       </c>
       <c r="AB34" s="1">
         <v>10305221.0</v>
       </c>
       <c r="AC34" s="1">
-        <v>1373578.222</v>
+        <v>3899496.0</v>
       </c>
       <c r="AD34" s="2"/>
       <c r="AE34" s="1">
-        <v>2525917.778</v>
+        <v>2525918.0</v>
       </c>
       <c r="AF34" s="2"/>
       <c r="AG34" s="1">
@@ -3806,17 +3806,17 @@
       </c>
       <c r="Z35" s="2"/>
       <c r="AA35" s="1">
-        <v>11054620.124</v>
+        <v>8251849.0</v>
       </c>
       <c r="AB35" s="1">
         <v>11449243.0</v>
       </c>
       <c r="AC35" s="1">
-        <v>1529622.876</v>
+        <v>4332394.0</v>
       </c>
       <c r="AD35" s="2"/>
       <c r="AE35" s="1">
-        <v>2802771.124</v>
+        <v>2802771.0</v>
       </c>
       <c r="AF35" s="2"/>
       <c r="AG35" s="1">
@@ -3901,17 +3901,17 @@
       </c>
       <c r="Z36" s="2"/>
       <c r="AA36" s="1">
-        <v>12146827.798</v>
+        <v>9039397.0</v>
       </c>
       <c r="AB36" s="1">
         <v>12708167.0</v>
       </c>
       <c r="AC36" s="1">
-        <v>1701339.202</v>
+        <v>4808770.0</v>
       </c>
       <c r="AD36" s="2"/>
       <c r="AE36" s="1">
-        <v>3107430.798</v>
+        <v>3107431.0</v>
       </c>
       <c r="AF36" s="2"/>
       <c r="AG36" s="1">
@@ -3996,17 +3996,17 @@
       </c>
       <c r="Z37" s="2"/>
       <c r="AA37" s="1">
-        <v>13348187.446</v>
+        <v>9905510.0</v>
       </c>
       <c r="AB37" s="1">
         <v>14093484.0</v>
       </c>
       <c r="AC37" s="1">
-        <v>1890296.554</v>
+        <v>5332974.0</v>
       </c>
       <c r="AD37" s="2"/>
       <c r="AE37" s="1">
-        <v>3442677.446</v>
+        <v>3442678.0</v>
       </c>
       <c r="AF37" s="2"/>
       <c r="AG37" s="1">
@@ -4091,17 +4091,17 @@
       </c>
       <c r="Z38" s="2"/>
       <c r="AA38" s="1">
-        <v>14669613.75</v>
+        <v>10858044.0</v>
       </c>
       <c r="AB38" s="1">
         <v>15617832.0</v>
       </c>
       <c r="AC38" s="1">
-        <v>2098218.25</v>
+        <v>5909788.0</v>
       </c>
       <c r="AD38" s="2"/>
       <c r="AE38" s="1">
-        <v>3811569.75</v>
+        <v>3811570.0</v>
       </c>
       <c r="AF38" s="2"/>
       <c r="AG38" s="1">
@@ -4186,17 +4186,17 @@
       </c>
       <c r="Z39" s="2"/>
       <c r="AA39" s="1">
-        <v>16123115.28</v>
+        <v>11905643.0</v>
       </c>
       <c r="AB39" s="1">
         <v>17295115.0</v>
       </c>
       <c r="AC39" s="1">
-        <v>2326999.72</v>
+        <v>6544472.0</v>
       </c>
       <c r="AD39" s="2"/>
       <c r="AE39" s="1">
-        <v>4217472.28</v>
+        <v>4217473.0</v>
       </c>
       <c r="AF39" s="2"/>
       <c r="AG39" s="1">
@@ -4281,17 +4281,17 @@
       </c>
       <c r="Z40" s="12"/>
       <c r="AA40" s="11">
-        <v>17721900.074</v>
+        <v>13057814.0</v>
       </c>
       <c r="AB40" s="11">
         <v>19140627.0</v>
       </c>
       <c r="AC40" s="11">
-        <v>2578726.926</v>
+        <v>7242813.0</v>
       </c>
       <c r="AD40" s="12"/>
       <c r="AE40" s="11">
-        <v>4664086.074</v>
+        <v>4664087.0</v>
       </c>
       <c r="AF40" s="12"/>
       <c r="AG40" s="11">
@@ -4376,17 +4376,17 @@
       </c>
       <c r="Z41" s="2"/>
       <c r="AA41" s="1">
-        <v>19480494.254</v>
+        <v>14325012.0</v>
       </c>
       <c r="AB41" s="1">
         <v>21171190.0</v>
       </c>
       <c r="AC41" s="1">
-        <v>2855695.746</v>
+        <v>8011178.0</v>
       </c>
       <c r="AD41" s="2"/>
       <c r="AE41" s="1">
-        <v>5155482.254</v>
+        <v>5155483.0</v>
       </c>
       <c r="AF41" s="2"/>
       <c r="AG41" s="1">
@@ -4471,17 +4471,17 @@
       </c>
       <c r="Z42" s="2"/>
       <c r="AA42" s="1">
-        <v>21414879.052</v>
+        <v>15718740.0</v>
       </c>
       <c r="AB42" s="1">
         <v>23405309.0</v>
       </c>
       <c r="AC42" s="1">
-        <v>3160429.948</v>
+        <v>8856569.0</v>
       </c>
       <c r="AD42" s="2"/>
       <c r="AE42" s="1">
-        <v>5696139.052</v>
+        <v>5696140.0</v>
       </c>
       <c r="AF42" s="2"/>
       <c r="AG42" s="1">
@@ -4566,17 +4566,17 @@
       </c>
       <c r="Z43" s="2"/>
       <c r="AA43" s="1">
-        <v>23542634.532</v>
+        <v>17251652.0</v>
       </c>
       <c r="AB43" s="1">
         <v>25863340.0</v>
       </c>
       <c r="AC43" s="1">
-        <v>3495705.468</v>
+        <v>9786688.0</v>
       </c>
       <c r="AD43" s="2"/>
       <c r="AE43" s="1">
-        <v>6290982.532</v>
+        <v>6290983.0</v>
       </c>
       <c r="AF43" s="2"/>
       <c r="AG43" s="1">
@@ -4661,17 +4661,17 @@
       </c>
       <c r="Z44" s="2"/>
       <c r="AA44" s="1">
-        <v>25883097.36</v>
+        <v>18937666.0</v>
       </c>
       <c r="AB44" s="1">
         <v>28567674.0</v>
       </c>
       <c r="AC44" s="1">
-        <v>3864576.64</v>
+        <v>10810008.0</v>
       </c>
       <c r="AD44" s="2"/>
       <c r="AE44" s="1">
-        <v>6945431.36</v>
+        <v>6945432.0</v>
       </c>
       <c r="AF44" s="2"/>
       <c r="AG44" s="1">
@@ -4756,17 +4756,17 @@
       </c>
       <c r="Z45" s="2"/>
       <c r="AA45" s="1">
-        <v>28457538.062</v>
+        <v>20792092.0</v>
       </c>
       <c r="AB45" s="1">
         <v>31542941.0</v>
       </c>
       <c r="AC45" s="1">
-        <v>4270402.938</v>
+        <v>11935849.0</v>
       </c>
       <c r="AD45" s="2"/>
       <c r="AE45" s="1">
-        <v>7665446.062</v>
+        <v>7665447.0</v>
       </c>
       <c r="AF45" s="2"/>
       <c r="AG45" s="1">
@@ -4851,17 +4851,17 @@
       </c>
       <c r="Z46" s="2"/>
       <c r="AA46" s="1">
-        <v>31289355.232</v>
+        <v>22831772.0</v>
       </c>
       <c r="AB46" s="1">
         <v>34816235.0</v>
       </c>
       <c r="AC46" s="1">
-        <v>4716879.768</v>
+        <v>13174463.0</v>
       </c>
       <c r="AD46" s="2"/>
       <c r="AE46" s="1">
-        <v>8457583.232</v>
+        <v>8457584.0</v>
       </c>
       <c r="AF46" s="2"/>
       <c r="AG46" s="1">
@@ -4946,17 +4946,17 @@
       </c>
       <c r="Z47" s="2"/>
       <c r="AA47" s="1">
-        <v>34404285.13</v>
+        <v>25075230.0</v>
       </c>
       <c r="AB47" s="1">
         <v>38417359.0</v>
       </c>
       <c r="AC47" s="1">
-        <v>5208073.87</v>
+        <v>14537129.0</v>
       </c>
       <c r="AD47" s="2"/>
       <c r="AE47" s="1">
-        <v>9329055.13</v>
+        <v>9329056.0</v>
       </c>
       <c r="AF47" s="2"/>
       <c r="AG47" s="1">
@@ -5041,17 +5041,17 @@
       </c>
       <c r="Z48" s="2"/>
       <c r="AA48" s="1">
-        <v>37830640.22</v>
+        <v>27542845.0</v>
       </c>
       <c r="AB48" s="1">
         <v>42379095.0</v>
       </c>
       <c r="AC48" s="1">
-        <v>5748454.78</v>
+        <v>16036250.0</v>
       </c>
       <c r="AD48" s="2"/>
       <c r="AE48" s="1">
-        <v>10287795.22</v>
+        <v>10287796.0</v>
       </c>
       <c r="AF48" s="2"/>
       <c r="AG48" s="1">
@@ -5136,17 +5136,17 @@
       </c>
       <c r="Z49" s="2"/>
       <c r="AA49" s="1">
-        <v>41599563.33</v>
+        <v>30257033.0</v>
       </c>
       <c r="AB49" s="1">
         <v>46737505.0</v>
       </c>
       <c r="AC49" s="1">
-        <v>6342941.67</v>
+        <v>17685472.0</v>
       </c>
       <c r="AD49" s="2"/>
       <c r="AE49" s="1">
-        <v>11342530.33</v>
+        <v>11342531.0</v>
       </c>
       <c r="AF49" s="2"/>
       <c r="AG49" s="1">
@@ -5231,17 +5231,17 @@
       </c>
       <c r="Z50" s="2"/>
       <c r="AA50" s="1">
-        <v>45745309.962</v>
+        <v>33242450.0</v>
       </c>
       <c r="AB50" s="1">
         <v>51532256.0</v>
       </c>
       <c r="AC50" s="1">
-        <v>6996946.038</v>
+        <v>19499806.0</v>
       </c>
       <c r="AD50" s="2"/>
       <c r="AE50" s="1">
-        <v>12502859.962</v>
+        <v>12502861.0</v>
       </c>
       <c r="AF50" s="2"/>
       <c r="AG50" s="1">
@@ -5326,17 +5326,17 @@
       </c>
       <c r="Z51" s="2"/>
       <c r="AA51" s="1">
-        <v>50305563.566</v>
+        <v>36526220.0</v>
       </c>
       <c r="AB51" s="1">
         <v>56806982.0</v>
       </c>
       <c r="AC51" s="1">
-        <v>7716418.434</v>
+        <v>21495762.0</v>
       </c>
       <c r="AD51" s="2"/>
       <c r="AE51" s="1">
-        <v>13779343.566</v>
+        <v>13779345.0</v>
       </c>
       <c r="AF51" s="2"/>
       <c r="AG51" s="1">
@@ -5421,17 +5421,17 @@
       </c>
       <c r="Z52" s="2"/>
       <c r="AA52" s="1">
-        <v>55321773.526</v>
+        <v>40138177.0</v>
       </c>
       <c r="AB52" s="1">
         <v>62609680.0</v>
       </c>
       <c r="AC52" s="1">
-        <v>8507906.474</v>
+        <v>23691503.0</v>
       </c>
       <c r="AD52" s="2"/>
       <c r="AE52" s="1">
-        <v>15183596.526</v>
+        <v>15183598.0</v>
       </c>
       <c r="AF52" s="2"/>
       <c r="AG52" s="1">
@@ -5462,7 +5462,7 @@
         <v>63</v>
       </c>
       <c r="C53" s="13">
-        <v>5596745.62</v>
+        <v>7978710.0</v>
       </c>
       <c r="D53" s="14"/>
       <c r="E53" s="13">
@@ -5516,17 +5516,17 @@
       </c>
       <c r="Z53" s="14"/>
       <c r="AA53" s="13">
-        <v>52166353.0</v>
+        <v>35631163.0</v>
       </c>
       <c r="AB53" s="13">
         <v>68194777.0</v>
       </c>
       <c r="AC53" s="13">
-        <v>9269714.0</v>
+        <v>25804904.0</v>
       </c>
       <c r="AD53" s="14"/>
       <c r="AE53" s="13">
-        <v>16535190.0</v>
+        <v>12801634.0</v>
       </c>
       <c r="AF53" s="14"/>
       <c r="AG53" s="13">
@@ -5537,10 +5537,10 @@
       </c>
       <c r="AI53" s="14"/>
       <c r="AJ53" s="13">
-        <v>5596745.62</v>
+        <v>7978710.0</v>
       </c>
       <c r="AK53" s="13">
-        <v>27983728.1</v>
+        <v>39893550.0</v>
       </c>
       <c r="AL53" s="13">
         <v>-1220000.0</v>
@@ -5557,7 +5557,7 @@
         <v>64</v>
       </c>
       <c r="C54" s="4">
-        <v>5648607.782</v>
+        <v>8776581.0</v>
       </c>
       <c r="D54" s="2"/>
       <c r="E54" s="5">
@@ -5611,17 +5611,17 @@
       </c>
       <c r="Z54" s="2"/>
       <c r="AA54" s="1">
-        <v>50494941.4678</v>
+        <v>32685391.9</v>
       </c>
       <c r="AB54" s="1">
         <v>66702015.9</v>
       </c>
       <c r="AC54" s="1">
-        <v>7430493.4322</v>
+        <v>25240043.0</v>
       </c>
       <c r="AD54" s="2"/>
       <c r="AE54" s="1">
-        <v>17809549.5678</v>
+        <v>9673661.0</v>
       </c>
       <c r="AF54" s="2"/>
       <c r="AG54" s="1">
@@ -5632,10 +5632,10 @@
       </c>
       <c r="AI54" s="2"/>
       <c r="AJ54" s="1">
-        <v>5648607.782</v>
+        <v>8776581.0</v>
       </c>
       <c r="AK54" s="1">
-        <v>28243038.91</v>
+        <v>43882905.0</v>
       </c>
       <c r="AL54" s="1">
         <v>0</v>
@@ -5652,7 +5652,7 @@
         <v>65</v>
       </c>
       <c r="C55" s="4">
-        <v>6213468.258</v>
+        <v>9654239.0</v>
       </c>
       <c r="D55" s="2"/>
       <c r="E55" s="5">
@@ -5706,17 +5706,17 @@
       </c>
       <c r="Z55" s="2"/>
       <c r="AA55" s="1">
-        <v>48330461.622</v>
+        <v>29352749.1</v>
       </c>
       <c r="AB55" s="1">
         <v>62752555.1</v>
       </c>
       <c r="AC55" s="1">
-        <v>4767854.478</v>
+        <v>23745567.0</v>
       </c>
       <c r="AD55" s="2"/>
       <c r="AE55" s="1">
-        <v>18977712.522</v>
+        <v>6232890.0</v>
       </c>
       <c r="AF55" s="2"/>
       <c r="AG55" s="1">
@@ -5727,10 +5727,10 @@
       </c>
       <c r="AI55" s="2"/>
       <c r="AJ55" s="1">
-        <v>6213468.258</v>
+        <v>9654239.0</v>
       </c>
       <c r="AK55" s="1">
-        <v>31067341.29</v>
+        <v>48271195.0</v>
       </c>
       <c r="AL55" s="1">
         <v>0</v>
@@ -5747,7 +5747,7 @@
         <v>66</v>
       </c>
       <c r="C56" s="4">
-        <v>6834815.586</v>
+        <v>10619663.0</v>
       </c>
       <c r="D56" s="2"/>
       <c r="E56" s="5">
@@ -5801,17 +5801,17 @@
       </c>
       <c r="Z56" s="2"/>
       <c r="AA56" s="1">
-        <v>45032419.6334</v>
+        <v>25026723.7</v>
       </c>
       <c r="AB56" s="1">
         <v>57346181.7</v>
       </c>
       <c r="AC56" s="1">
-        <v>1694099.0666</v>
+        <v>21699795.0</v>
       </c>
       <c r="AD56" s="2"/>
       <c r="AE56" s="1">
-        <v>20005695.9334</v>
+        <v>2448043.0</v>
       </c>
       <c r="AF56" s="2"/>
       <c r="AG56" s="1">
@@ -5822,10 +5822,10 @@
       </c>
       <c r="AI56" s="2"/>
       <c r="AJ56" s="1">
-        <v>6834815.586</v>
+        <v>10619663.0</v>
       </c>
       <c r="AK56" s="1">
-        <v>34174077.93</v>
+        <v>53098315.0</v>
       </c>
       <c r="AL56" s="1">
         <v>0</v>
@@ -5842,7 +5842,7 @@
         <v>67</v>
       </c>
       <c r="C57" s="13">
-        <v>7518296.86</v>
+        <v>9966340.0</v>
       </c>
       <c r="D57" s="14"/>
       <c r="E57" s="13">
@@ -5896,17 +5896,17 @@
       </c>
       <c r="Z57" s="14"/>
       <c r="AA57" s="13">
-        <v>38549378.0</v>
+        <v>19541965.0</v>
       </c>
       <c r="AB57" s="13">
         <v>50231008.0</v>
       </c>
       <c r="AC57" s="13">
-        <v>0</v>
+        <v>19007413.0</v>
       </c>
       <c r="AD57" s="14"/>
       <c r="AE57" s="13">
-        <v>20853782.2494</v>
+        <v>0</v>
       </c>
       <c r="AF57" s="14"/>
       <c r="AG57" s="13">
@@ -5917,10 +5917,10 @@
       </c>
       <c r="AI57" s="14"/>
       <c r="AJ57" s="13">
-        <v>7518296.86</v>
+        <v>9966340.0</v>
       </c>
       <c r="AK57" s="13">
-        <v>37591484.3</v>
+        <v>49831700.0</v>
       </c>
       <c r="AL57" s="13">
         <v>0</v>
@@ -5937,7 +5937,7 @@
         <v>68</v>
       </c>
       <c r="C58" s="4">
-        <v>8270126.446</v>
+        <v>8270126.0</v>
       </c>
       <c r="D58" s="2"/>
       <c r="E58" s="5">
@@ -5991,17 +5991,17 @@
       </c>
       <c r="Z58" s="2"/>
       <c r="AA58" s="1">
-        <v>28269543.7</v>
+        <v>12709986.7</v>
       </c>
       <c r="AB58" s="1">
         <v>41119336.7</v>
       </c>
       <c r="AC58" s="1">
-        <v>0</v>
+        <v>15559557.0</v>
       </c>
       <c r="AD58" s="2"/>
       <c r="AE58" s="1">
-        <v>21475712.2108</v>
+        <v>621930.0</v>
       </c>
       <c r="AF58" s="2"/>
       <c r="AG58" s="1">
@@ -6012,10 +6012,10 @@
       </c>
       <c r="AI58" s="2"/>
       <c r="AJ58" s="1">
-        <v>8270126.446</v>
+        <v>8270126.0</v>
       </c>
       <c r="AK58" s="1">
-        <v>41350632.23</v>
+        <v>41350630.0</v>
       </c>
       <c r="AL58" s="1">
         <v>0</v>
@@ -6032,7 +6032,7 @@
         <v>69</v>
       </c>
       <c r="C59" s="4">
-        <v>9097138.984</v>
+        <v>9719069.0</v>
       </c>
       <c r="D59" s="2"/>
       <c r="E59" s="5">
@@ -6086,17 +6086,17 @@
       </c>
       <c r="Z59" s="2"/>
       <c r="AA59" s="1">
-        <v>15548248.8</v>
+        <v>4316193.8</v>
       </c>
       <c r="AB59" s="1">
         <v>29683020.8</v>
       </c>
       <c r="AC59" s="1">
-        <v>0</v>
+        <v>11232055.0</v>
       </c>
       <c r="AD59" s="2"/>
       <c r="AE59" s="1">
-        <v>21817773.6844</v>
+        <v>0</v>
       </c>
       <c r="AF59" s="2"/>
       <c r="AG59" s="1">
@@ -6107,10 +6107,10 @@
       </c>
       <c r="AI59" s="2"/>
       <c r="AJ59" s="1">
-        <v>9097138.984</v>
+        <v>9719069.0</v>
       </c>
       <c r="AK59" s="1">
-        <v>45485694.92</v>
+        <v>48595345.0</v>
       </c>
       <c r="AL59" s="1">
         <v>0</v>
@@ -6127,7 +6127,7 @@
         <v>70</v>
       </c>
       <c r="C60" s="5">
-        <v>10006853.478</v>
+        <v>10006853.0</v>
       </c>
       <c r="D60" s="16"/>
       <c r="E60" s="5">
@@ -6181,17 +6181,17 @@
       </c>
       <c r="Z60" s="16"/>
       <c r="AA60" s="5">
-        <v>0.099999997764826</v>
+        <v>-5883456.9</v>
       </c>
       <c r="AB60" s="5">
         <v>15548249.1</v>
       </c>
       <c r="AC60" s="5">
-        <v>0</v>
+        <v>5883457.0</v>
       </c>
       <c r="AD60" s="16"/>
       <c r="AE60" s="5">
-        <v>21817773.6866</v>
+        <v>0.0</v>
       </c>
       <c r="AF60" s="16"/>
       <c r="AG60" s="5">
@@ -6202,10 +6202,10 @@
       </c>
       <c r="AI60" s="16"/>
       <c r="AJ60" s="5">
-        <v>10006853.478</v>
+        <v>10006853.0</v>
       </c>
       <c r="AK60" s="5">
-        <v>50034267.39</v>
+        <v>50034265.0</v>
       </c>
       <c r="AL60" s="5">
         <v>0</v>
@@ -10526,7 +10526,7 @@
         <v>63</v>
       </c>
       <c r="C53" s="13">
-        <v>5596745.62</v>
+        <v>7978710.0</v>
       </c>
       <c r="D53" s="14"/>
       <c r="E53" s="13">
@@ -10571,10 +10571,10 @@
       </c>
       <c r="AI53" s="14"/>
       <c r="AJ53" s="13">
-        <v>5596745.62</v>
+        <v>7978710.0</v>
       </c>
       <c r="AK53" s="13">
-        <v>27983728.1</v>
+        <v>39893550.0</v>
       </c>
       <c r="AL53" s="13">
         <v>0</v>
@@ -10593,7 +10593,7 @@
         <v>64</v>
       </c>
       <c r="C54" s="4">
-        <v>5648607.782</v>
+        <v>8776581.0</v>
       </c>
       <c r="D54" s="2"/>
       <c r="E54" s="5">
@@ -10638,10 +10638,10 @@
       </c>
       <c r="AI54" s="2"/>
       <c r="AJ54" s="1">
-        <v>5648607.782</v>
+        <v>8776581.0</v>
       </c>
       <c r="AK54" s="1">
-        <v>28243038.91</v>
+        <v>43882905.0</v>
       </c>
       <c r="AL54" s="1">
         <v>0</v>
@@ -10660,7 +10660,7 @@
         <v>65</v>
       </c>
       <c r="C55" s="4">
-        <v>6213468.258</v>
+        <v>9654239.0</v>
       </c>
       <c r="D55" s="2"/>
       <c r="E55" s="5">
@@ -10705,10 +10705,10 @@
       </c>
       <c r="AI55" s="2"/>
       <c r="AJ55" s="1">
-        <v>6213468.258</v>
+        <v>9654239.0</v>
       </c>
       <c r="AK55" s="1">
-        <v>31067341.29</v>
+        <v>48271195.0</v>
       </c>
       <c r="AL55" s="1">
         <v>0</v>
@@ -10727,7 +10727,7 @@
         <v>66</v>
       </c>
       <c r="C56" s="4">
-        <v>6834815.586</v>
+        <v>10619663.0</v>
       </c>
       <c r="D56" s="2"/>
       <c r="E56" s="5">
@@ -10772,10 +10772,10 @@
       </c>
       <c r="AI56" s="2"/>
       <c r="AJ56" s="1">
-        <v>6834815.586</v>
+        <v>10619663.0</v>
       </c>
       <c r="AK56" s="1">
-        <v>34174077.93</v>
+        <v>53098315.0</v>
       </c>
       <c r="AL56" s="1">
         <v>0</v>
@@ -10794,7 +10794,7 @@
         <v>67</v>
       </c>
       <c r="C57" s="13">
-        <v>7518296.86</v>
+        <v>9966340.0</v>
       </c>
       <c r="D57" s="14"/>
       <c r="E57" s="13">
@@ -10839,10 +10839,10 @@
       </c>
       <c r="AI57" s="14"/>
       <c r="AJ57" s="13">
-        <v>7518296.86</v>
+        <v>9966340.0</v>
       </c>
       <c r="AK57" s="13">
-        <v>37591484.3</v>
+        <v>49831700.0</v>
       </c>
       <c r="AL57" s="13">
         <v>0</v>
@@ -10861,7 +10861,7 @@
         <v>68</v>
       </c>
       <c r="C58" s="4">
-        <v>8270126.446</v>
+        <v>8270126.0</v>
       </c>
       <c r="D58" s="2"/>
       <c r="E58" s="5">
@@ -10906,10 +10906,10 @@
       </c>
       <c r="AI58" s="2"/>
       <c r="AJ58" s="1">
-        <v>8270126.446</v>
+        <v>8270126.0</v>
       </c>
       <c r="AK58" s="1">
-        <v>41350632.23</v>
+        <v>41350630.0</v>
       </c>
       <c r="AL58" s="1">
         <v>0</v>
@@ -10928,7 +10928,7 @@
         <v>69</v>
       </c>
       <c r="C59" s="4">
-        <v>9097138.984</v>
+        <v>9719069.0</v>
       </c>
       <c r="D59" s="2"/>
       <c r="E59" s="5">
@@ -10973,10 +10973,10 @@
       </c>
       <c r="AI59" s="2"/>
       <c r="AJ59" s="1">
-        <v>9097138.984</v>
+        <v>9719069.0</v>
       </c>
       <c r="AK59" s="1">
-        <v>45485694.92</v>
+        <v>48595345.0</v>
       </c>
       <c r="AL59" s="1">
         <v>0</v>
@@ -10995,7 +10995,7 @@
         <v>70</v>
       </c>
       <c r="C60" s="5">
-        <v>10006853.478</v>
+        <v>10006853.0</v>
       </c>
       <c r="D60" s="16"/>
       <c r="E60" s="5">
@@ -11040,10 +11040,10 @@
       </c>
       <c r="AI60" s="16"/>
       <c r="AJ60" s="5">
-        <v>10006853.478</v>
+        <v>10006853.0</v>
       </c>
       <c r="AK60" s="5">
-        <v>50034267.39</v>
+        <v>50034265.0</v>
       </c>
       <c r="AL60" s="5">
         <v>0</v>
@@ -11931,7 +11931,7 @@
     <col min="26" max="26" width="9.283" bestFit="true" customWidth="true" style="0"/>
     <col min="27" max="27" width="12.854" bestFit="true" customWidth="true" style="0"/>
     <col min="28" max="28" width="13.997" bestFit="true" customWidth="true" style="0"/>
-    <col min="29" max="29" width="11.711" bestFit="true" customWidth="true" style="0"/>
+    <col min="29" max="29" width="12.854" bestFit="true" customWidth="true" style="0"/>
     <col min="30" max="30" width="9.283" bestFit="true" customWidth="true" style="0"/>
     <col min="31" max="31" width="21.138" bestFit="true" customWidth="true" style="0"/>
     <col min="32" max="32" width="11.711" bestFit="true" customWidth="true" style="0"/>
@@ -12370,13 +12370,13 @@
       <c r="Y9" s="8"/>
       <c r="Z9" s="9"/>
       <c r="AA9" s="8">
-        <v>1005500.0</v>
+        <v>1005311.0</v>
       </c>
       <c r="AB9" s="8">
         <v>500.0</v>
       </c>
       <c r="AC9" s="8">
-        <v>0</v>
+        <v>189.0</v>
       </c>
       <c r="AD9" s="9">
         <v>0.3784</v>
@@ -12463,19 +12463,19 @@
       <c r="Y10" s="1"/>
       <c r="Z10" s="2"/>
       <c r="AA10" s="1">
-        <v>1111550.0</v>
+        <v>1073123.0</v>
       </c>
       <c r="AB10" s="1">
         <v>101550.0</v>
       </c>
       <c r="AC10" s="1">
-        <v>0</v>
+        <v>38427.0</v>
       </c>
       <c r="AD10" s="2">
         <v>0.3784</v>
       </c>
       <c r="AE10" s="1">
-        <v>56630.1</v>
+        <v>56630.0</v>
       </c>
       <c r="AF10" s="2">
         <v>0.022</v>
@@ -12556,19 +12556,19 @@
       <c r="Y11" s="1"/>
       <c r="Z11" s="2"/>
       <c r="AA11" s="1">
-        <v>1228205.0</v>
+        <v>1147528.0</v>
       </c>
       <c r="AB11" s="1">
         <v>213205.0</v>
       </c>
       <c r="AC11" s="1">
-        <v>0</v>
+        <v>80677.0</v>
       </c>
       <c r="AD11" s="2">
         <v>0.3784</v>
       </c>
       <c r="AE11" s="1">
-        <v>83650.61</v>
+        <v>83651.0</v>
       </c>
       <c r="AF11" s="2">
         <v>0.022</v>
@@ -12649,19 +12649,19 @@
       <c r="Y12" s="1"/>
       <c r="Z12" s="2"/>
       <c r="AA12" s="1">
-        <v>1342679.182</v>
+        <v>1229185.0</v>
       </c>
       <c r="AB12" s="1">
         <v>336526.0</v>
       </c>
       <c r="AC12" s="1">
-        <v>13846.818</v>
+        <v>127341.0</v>
       </c>
       <c r="AD12" s="2">
         <v>0.3784</v>
       </c>
       <c r="AE12" s="1">
-        <v>113494.182</v>
+        <v>113495.0</v>
       </c>
       <c r="AF12" s="2">
         <v>0.022</v>
@@ -12742,19 +12742,19 @@
       <c r="Y13" s="1"/>
       <c r="Z13" s="2"/>
       <c r="AA13" s="1">
-        <v>1465260.12</v>
+        <v>1318817.0</v>
       </c>
       <c r="AB13" s="1">
         <v>472679.0</v>
       </c>
       <c r="AC13" s="1">
-        <v>32418.88</v>
+        <v>178862.0</v>
       </c>
       <c r="AD13" s="2">
         <v>0.3784</v>
       </c>
       <c r="AE13" s="1">
-        <v>146443.12</v>
+        <v>146444.0</v>
       </c>
       <c r="AF13" s="2">
         <v>0.022</v>
@@ -12835,19 +12835,19 @@
       <c r="Y14" s="1"/>
       <c r="Z14" s="2"/>
       <c r="AA14" s="1">
-        <v>1600031.954</v>
+        <v>1417224.0</v>
       </c>
       <c r="AB14" s="1">
         <v>622947.0</v>
       </c>
       <c r="AC14" s="1">
-        <v>52915.046</v>
+        <v>235723.0</v>
       </c>
       <c r="AD14" s="2">
         <v>0.3784</v>
       </c>
       <c r="AE14" s="1">
-        <v>182807.954</v>
+        <v>182809.0</v>
       </c>
       <c r="AF14" s="2">
         <v>0.022</v>
@@ -12928,19 +12928,19 @@
       <c r="Y15" s="1"/>
       <c r="Z15" s="2"/>
       <c r="AA15" s="1">
-        <v>1748212.278</v>
+        <v>1525282.0</v>
       </c>
       <c r="AB15" s="1">
         <v>788742.0</v>
       </c>
       <c r="AC15" s="1">
-        <v>75529.722</v>
+        <v>298460.0</v>
       </c>
       <c r="AD15" s="2">
         <v>0.3784</v>
       </c>
       <c r="AE15" s="1">
-        <v>222930.278</v>
+        <v>222931.0</v>
       </c>
       <c r="AF15" s="2">
         <v>0.022</v>
@@ -13021,19 +13021,19 @@
       <c r="Y16" s="1"/>
       <c r="Z16" s="2"/>
       <c r="AA16" s="1">
-        <v>1911142.83</v>
+        <v>1643957.0</v>
       </c>
       <c r="AB16" s="1">
         <v>971616.0</v>
       </c>
       <c r="AC16" s="1">
-        <v>100473.17</v>
+        <v>367659.0</v>
       </c>
       <c r="AD16" s="2">
         <v>0.3784</v>
       </c>
       <c r="AE16" s="1">
-        <v>267185.83</v>
+        <v>267187.0</v>
       </c>
       <c r="AF16" s="2">
         <v>0.022</v>
@@ -13114,19 +13114,19 @@
       <c r="Y17" s="1"/>
       <c r="Z17" s="2"/>
       <c r="AA17" s="1">
-        <v>2090297.946</v>
+        <v>1774310.0</v>
       </c>
       <c r="AB17" s="1">
         <v>1173278.0</v>
       </c>
       <c r="AC17" s="1">
-        <v>127980.054</v>
+        <v>443968.0</v>
       </c>
       <c r="AD17" s="2">
         <v>0.3784</v>
       </c>
       <c r="AE17" s="1">
-        <v>315987.946</v>
+        <v>315989.0</v>
       </c>
       <c r="AF17" s="2">
         <v>0.022</v>
@@ -13207,19 +13207,19 @@
       <c r="Y18" s="1"/>
       <c r="Z18" s="2"/>
       <c r="AA18" s="1">
-        <v>2287300.278</v>
+        <v>1917509.0</v>
       </c>
       <c r="AB18" s="1">
         <v>1395606.0</v>
       </c>
       <c r="AC18" s="1">
-        <v>158305.722</v>
+        <v>528097.0</v>
       </c>
       <c r="AD18" s="2">
         <v>0.3784</v>
       </c>
       <c r="AE18" s="1">
-        <v>369791.278</v>
+        <v>369792.0</v>
       </c>
       <c r="AF18" s="2">
         <v>0.022</v>
@@ -13300,19 +13300,19 @@
       <c r="Y19" s="1"/>
       <c r="Z19" s="2"/>
       <c r="AA19" s="1">
-        <v>2503934.952</v>
+        <v>2074839.0</v>
       </c>
       <c r="AB19" s="1">
         <v>1640667.0</v>
       </c>
       <c r="AC19" s="1">
-        <v>191732.048</v>
+        <v>620828.0</v>
       </c>
       <c r="AD19" s="2">
         <v>0.3784</v>
       </c>
       <c r="AE19" s="1">
-        <v>429095.952</v>
+        <v>429097.0</v>
       </c>
       <c r="AF19" s="2">
         <v>0.022</v>
@@ -13393,19 +13393,19 @@
       <c r="Y20" s="1"/>
       <c r="Z20" s="2"/>
       <c r="AA20" s="1">
-        <v>2742164.1</v>
+        <v>2247712.0</v>
       </c>
       <c r="AB20" s="1">
         <v>1910734.0</v>
       </c>
       <c r="AC20" s="1">
-        <v>228569.9</v>
+        <v>723022.0</v>
       </c>
       <c r="AD20" s="2">
         <v>0.3784</v>
       </c>
       <c r="AE20" s="1">
-        <v>494452.1</v>
+        <v>494453.0</v>
       </c>
       <c r="AF20" s="2">
         <v>0.022</v>
@@ -13486,19 +13486,19 @@
       <c r="Y21" s="1"/>
       <c r="Z21" s="2"/>
       <c r="AA21" s="1">
-        <v>3004148.854</v>
+        <v>2437684.0</v>
       </c>
       <c r="AB21" s="1">
         <v>2208307.0</v>
       </c>
       <c r="AC21" s="1">
-        <v>269158.146</v>
+        <v>835623.0</v>
       </c>
       <c r="AD21" s="2">
         <v>0.3784</v>
       </c>
       <c r="AE21" s="1">
-        <v>566464.854</v>
+        <v>566466.0</v>
       </c>
       <c r="AF21" s="2">
         <v>0.022</v>
@@ -13579,19 +13579,19 @@
       <c r="Y22" s="1"/>
       <c r="Z22" s="2"/>
       <c r="AA22" s="1">
-        <v>3292262.89</v>
+        <v>2646463.0</v>
       </c>
       <c r="AB22" s="1">
         <v>2536138.0</v>
       </c>
       <c r="AC22" s="1">
-        <v>313875.11</v>
+        <v>959675.0</v>
       </c>
       <c r="AD22" s="2">
         <v>0.3784</v>
       </c>
       <c r="AE22" s="1">
-        <v>645799.89</v>
+        <v>645801.0</v>
       </c>
       <c r="AF22" s="2">
         <v>0.022</v>
@@ -13672,19 +13672,19 @@
       <c r="Y23" s="1"/>
       <c r="Z23" s="2"/>
       <c r="AA23" s="1">
-        <v>3609121.434</v>
+        <v>2875932.0</v>
       </c>
       <c r="AB23" s="1">
         <v>2897252.0</v>
       </c>
       <c r="AC23" s="1">
-        <v>363130.566</v>
+        <v>1096320.0</v>
       </c>
       <c r="AD23" s="2">
         <v>0.3784</v>
       </c>
       <c r="AE23" s="1">
-        <v>733189.434</v>
+        <v>733191.0</v>
       </c>
       <c r="AF23" s="2">
         <v>0.022</v>
@@ -13765,19 +13765,19 @@
       <c r="Y24" s="1"/>
       <c r="Z24" s="2"/>
       <c r="AA24" s="1">
-        <v>3957596.928</v>
+        <v>3128158.0</v>
       </c>
       <c r="AB24" s="1">
         <v>3294977.0</v>
       </c>
       <c r="AC24" s="1">
-        <v>417380.072</v>
+        <v>1246819.0</v>
       </c>
       <c r="AD24" s="2">
         <v>0.3784</v>
       </c>
       <c r="AE24" s="1">
-        <v>829438.928</v>
+        <v>829440.0</v>
       </c>
       <c r="AF24" s="2">
         <v>0.022</v>
@@ -13858,19 +13858,19 @@
       <c r="Y25" s="1"/>
       <c r="Z25" s="2"/>
       <c r="AA25" s="1">
-        <v>4340851.378</v>
+        <v>3405417.0</v>
       </c>
       <c r="AB25" s="1">
         <v>3732975.0</v>
       </c>
       <c r="AC25" s="1">
-        <v>477123.622</v>
+        <v>1412558.0</v>
       </c>
       <c r="AD25" s="2">
         <v>0.3784</v>
       </c>
       <c r="AE25" s="1">
-        <v>935434.378</v>
+        <v>935435.0</v>
       </c>
       <c r="AF25" s="2">
         <v>0.022</v>
@@ -13951,19 +13951,19 @@
       <c r="Y26" s="1"/>
       <c r="Z26" s="2"/>
       <c r="AA26" s="1">
-        <v>4762364.384</v>
+        <v>3710214.0</v>
       </c>
       <c r="AB26" s="1">
         <v>4215273.0</v>
       </c>
       <c r="AC26" s="1">
-        <v>542908.616</v>
+        <v>1595059.0</v>
       </c>
       <c r="AD26" s="2">
         <v>0.3784</v>
       </c>
       <c r="AE26" s="1">
-        <v>1052150.384</v>
+        <v>1052151.0</v>
       </c>
       <c r="AF26" s="2">
         <v>0.022</v>
@@ -14044,19 +14044,19 @@
       <c r="Y27" s="1"/>
       <c r="Z27" s="2"/>
       <c r="AA27" s="1">
-        <v>5225958.984</v>
+        <v>4045300.0</v>
       </c>
       <c r="AB27" s="1">
         <v>4746300.0</v>
       </c>
       <c r="AC27" s="1">
-        <v>615341.016</v>
+        <v>1796000.0</v>
       </c>
       <c r="AD27" s="2">
         <v>0.3784</v>
       </c>
       <c r="AE27" s="1">
-        <v>1180658.984</v>
+        <v>1180660.0</v>
       </c>
       <c r="AF27" s="2">
         <v>0.022</v>
@@ -14137,19 +14137,19 @@
       <c r="Y28" s="1"/>
       <c r="Z28" s="2"/>
       <c r="AA28" s="1">
-        <v>5735845.444</v>
+        <v>4413706.0</v>
       </c>
       <c r="AB28" s="1">
         <v>5330930.0</v>
       </c>
       <c r="AC28" s="1">
-        <v>695084.556</v>
+        <v>2017224.0</v>
       </c>
       <c r="AD28" s="2">
         <v>0.3784</v>
       </c>
       <c r="AE28" s="1">
-        <v>1322139.444</v>
+        <v>1322140.0</v>
       </c>
       <c r="AF28" s="2">
         <v>0.022</v>
@@ -14230,19 +14230,19 @@
       <c r="Y29" s="1"/>
       <c r="Z29" s="2"/>
       <c r="AA29" s="1">
-        <v>6296651.95</v>
+        <v>4818763.0</v>
       </c>
       <c r="AB29" s="1">
         <v>5974523.0</v>
       </c>
       <c r="AC29" s="1">
-        <v>782871.05</v>
+        <v>2260760.0</v>
       </c>
       <c r="AD29" s="2">
         <v>0.3784</v>
       </c>
       <c r="AE29" s="1">
-        <v>1477888.95</v>
+        <v>1477890.0</v>
       </c>
       <c r="AF29" s="2">
         <v>0.022</v>
@@ -14323,19 +14323,19 @@
       <c r="Y30" s="1"/>
       <c r="Z30" s="2"/>
       <c r="AA30" s="1">
-        <v>6913471.4</v>
+        <v>5264137.0</v>
       </c>
       <c r="AB30" s="1">
         <v>6682975.0</v>
       </c>
       <c r="AC30" s="1">
-        <v>879503.6</v>
+        <v>2528838.0</v>
       </c>
       <c r="AD30" s="2">
         <v>0.3784</v>
       </c>
       <c r="AE30" s="1">
-        <v>1649334.4</v>
+        <v>1649335.0</v>
       </c>
       <c r="AF30" s="2">
         <v>0.022</v>
@@ -14416,19 +14416,19 @@
       <c r="Y31" s="1"/>
       <c r="Z31" s="2"/>
       <c r="AA31" s="1">
-        <v>7591905.406</v>
+        <v>5753860.0</v>
       </c>
       <c r="AB31" s="1">
         <v>7462773.0</v>
       </c>
       <c r="AC31" s="1">
-        <v>985867.594</v>
+        <v>2823913.0</v>
       </c>
       <c r="AD31" s="2">
         <v>0.3784</v>
       </c>
       <c r="AE31" s="1">
-        <v>1838045.406</v>
+        <v>1838046.0</v>
       </c>
       <c r="AF31" s="2">
         <v>0.022</v>
@@ -14509,19 +14509,19 @@
       <c r="Y32" s="1"/>
       <c r="Z32" s="2"/>
       <c r="AA32" s="1">
-        <v>8338113.506</v>
+        <v>6292365.0</v>
       </c>
       <c r="AB32" s="1">
         <v>8321050.0</v>
       </c>
       <c r="AC32" s="1">
-        <v>1102936.494</v>
+        <v>3148685.0</v>
       </c>
       <c r="AD32" s="2">
         <v>0.3784</v>
       </c>
       <c r="AE32" s="1">
-        <v>2045748.506</v>
+        <v>2045749.0</v>
       </c>
       <c r="AF32" s="2">
         <v>0.022</v>
@@ -14602,19 +14602,19 @@
       <c r="Y33" s="1"/>
       <c r="Z33" s="2"/>
       <c r="AA33" s="1">
-        <v>9158873.916</v>
+        <v>6884531.0</v>
       </c>
       <c r="AB33" s="1">
         <v>9265655.0</v>
       </c>
       <c r="AC33" s="1">
-        <v>1231781.084</v>
+        <v>3506124.0</v>
       </c>
       <c r="AD33" s="2">
         <v>0.3784</v>
       </c>
       <c r="AE33" s="1">
-        <v>2274342.916</v>
+        <v>2274343.0</v>
       </c>
       <c r="AF33" s="2">
         <v>0.022</v>
@@ -14695,19 +14695,19 @@
       <c r="Y34" s="1"/>
       <c r="Z34" s="2"/>
       <c r="AA34" s="1">
-        <v>10061642.778</v>
+        <v>7535725.0</v>
       </c>
       <c r="AB34" s="1">
         <v>10305221.0</v>
       </c>
       <c r="AC34" s="1">
-        <v>1373578.222</v>
+        <v>3899496.0</v>
       </c>
       <c r="AD34" s="2">
         <v>0.3784</v>
       </c>
       <c r="AE34" s="1">
-        <v>2525917.778</v>
+        <v>2525918.0</v>
       </c>
       <c r="AF34" s="2">
         <v>0.022</v>
@@ -14788,19 +14788,19 @@
       <c r="Y35" s="1"/>
       <c r="Z35" s="2"/>
       <c r="AA35" s="1">
-        <v>11054620.124</v>
+        <v>8251849.0</v>
       </c>
       <c r="AB35" s="1">
         <v>11449243.0</v>
       </c>
       <c r="AC35" s="1">
-        <v>1529622.876</v>
+        <v>4332394.0</v>
       </c>
       <c r="AD35" s="2">
         <v>0.3784</v>
       </c>
       <c r="AE35" s="1">
-        <v>2802771.124</v>
+        <v>2802771.0</v>
       </c>
       <c r="AF35" s="2">
         <v>0.022</v>
@@ -14881,19 +14881,19 @@
       <c r="Y36" s="1"/>
       <c r="Z36" s="2"/>
       <c r="AA36" s="1">
-        <v>12146827.798</v>
+        <v>9039397.0</v>
       </c>
       <c r="AB36" s="1">
         <v>12708167.0</v>
       </c>
       <c r="AC36" s="1">
-        <v>1701339.202</v>
+        <v>4808770.0</v>
       </c>
       <c r="AD36" s="2">
         <v>0.3784</v>
       </c>
       <c r="AE36" s="1">
-        <v>3107430.798</v>
+        <v>3107431.0</v>
       </c>
       <c r="AF36" s="2">
         <v>0.022</v>
@@ -14974,19 +14974,19 @@
       <c r="Y37" s="1"/>
       <c r="Z37" s="2"/>
       <c r="AA37" s="1">
-        <v>13348187.446</v>
+        <v>9905510.0</v>
       </c>
       <c r="AB37" s="1">
         <v>14093484.0</v>
       </c>
       <c r="AC37" s="1">
-        <v>1890296.554</v>
+        <v>5332974.0</v>
       </c>
       <c r="AD37" s="2">
         <v>0.3784</v>
       </c>
       <c r="AE37" s="1">
-        <v>3442677.446</v>
+        <v>3442678.0</v>
       </c>
       <c r="AF37" s="2">
         <v>0.022</v>
@@ -15067,19 +15067,19 @@
       <c r="Y38" s="1"/>
       <c r="Z38" s="2"/>
       <c r="AA38" s="1">
-        <v>14669613.75</v>
+        <v>10858044.0</v>
       </c>
       <c r="AB38" s="1">
         <v>15617832.0</v>
       </c>
       <c r="AC38" s="1">
-        <v>2098218.25</v>
+        <v>5909788.0</v>
       </c>
       <c r="AD38" s="2">
         <v>0.3784</v>
       </c>
       <c r="AE38" s="1">
-        <v>3811569.75</v>
+        <v>3811570.0</v>
       </c>
       <c r="AF38" s="2">
         <v>0.022</v>
@@ -15160,19 +15160,19 @@
       <c r="Y39" s="1"/>
       <c r="Z39" s="2"/>
       <c r="AA39" s="1">
-        <v>16123115.28</v>
+        <v>11905643.0</v>
       </c>
       <c r="AB39" s="1">
         <v>17295115.0</v>
       </c>
       <c r="AC39" s="1">
-        <v>2326999.72</v>
+        <v>6544472.0</v>
       </c>
       <c r="AD39" s="2">
         <v>0.3784</v>
       </c>
       <c r="AE39" s="1">
-        <v>4217472.28</v>
+        <v>4217473.0</v>
       </c>
       <c r="AF39" s="2">
         <v>0.022</v>
@@ -15253,19 +15253,19 @@
       <c r="Y40" s="11"/>
       <c r="Z40" s="12"/>
       <c r="AA40" s="11">
-        <v>17721900.074</v>
+        <v>13057814.0</v>
       </c>
       <c r="AB40" s="11">
         <v>19140627.0</v>
       </c>
       <c r="AC40" s="11">
-        <v>2578726.926</v>
+        <v>7242813.0</v>
       </c>
       <c r="AD40" s="12">
         <v>0.3784</v>
       </c>
       <c r="AE40" s="11">
-        <v>4664086.074</v>
+        <v>4664087.0</v>
       </c>
       <c r="AF40" s="12">
         <v>0.022</v>
@@ -15346,19 +15346,19 @@
       <c r="Y41" s="1"/>
       <c r="Z41" s="2"/>
       <c r="AA41" s="1">
-        <v>19480494.254</v>
+        <v>14325012.0</v>
       </c>
       <c r="AB41" s="1">
         <v>21171190.0</v>
       </c>
       <c r="AC41" s="1">
-        <v>2855695.746</v>
+        <v>8011178.0</v>
       </c>
       <c r="AD41" s="2">
         <v>0.3784</v>
       </c>
       <c r="AE41" s="1">
-        <v>5155482.254</v>
+        <v>5155483.0</v>
       </c>
       <c r="AF41" s="2">
         <v>0.022</v>
@@ -15439,19 +15439,19 @@
       <c r="Y42" s="1"/>
       <c r="Z42" s="2"/>
       <c r="AA42" s="1">
-        <v>21414879.052</v>
+        <v>15718740.0</v>
       </c>
       <c r="AB42" s="1">
         <v>23405309.0</v>
       </c>
       <c r="AC42" s="1">
-        <v>3160429.948</v>
+        <v>8856569.0</v>
       </c>
       <c r="AD42" s="2">
         <v>0.3784</v>
       </c>
       <c r="AE42" s="1">
-        <v>5696139.052</v>
+        <v>5696140.0</v>
       </c>
       <c r="AF42" s="2">
         <v>0.022</v>
@@ -15532,19 +15532,19 @@
       <c r="Y43" s="1"/>
       <c r="Z43" s="2"/>
       <c r="AA43" s="1">
-        <v>23542634.532</v>
+        <v>17251652.0</v>
       </c>
       <c r="AB43" s="1">
         <v>25863340.0</v>
       </c>
       <c r="AC43" s="1">
-        <v>3495705.468</v>
+        <v>9786688.0</v>
       </c>
       <c r="AD43" s="2">
         <v>0.3784</v>
       </c>
       <c r="AE43" s="1">
-        <v>6290982.532</v>
+        <v>6290983.0</v>
       </c>
       <c r="AF43" s="2">
         <v>0.022</v>
@@ -15625,19 +15625,19 @@
       <c r="Y44" s="1"/>
       <c r="Z44" s="2"/>
       <c r="AA44" s="1">
-        <v>25883097.36</v>
+        <v>18937666.0</v>
       </c>
       <c r="AB44" s="1">
         <v>28567674.0</v>
       </c>
       <c r="AC44" s="1">
-        <v>3864576.64</v>
+        <v>10810008.0</v>
       </c>
       <c r="AD44" s="2">
         <v>0.3784</v>
       </c>
       <c r="AE44" s="1">
-        <v>6945431.36</v>
+        <v>6945432.0</v>
       </c>
       <c r="AF44" s="2">
         <v>0.022</v>
@@ -15718,19 +15718,19 @@
       <c r="Y45" s="1"/>
       <c r="Z45" s="2"/>
       <c r="AA45" s="1">
-        <v>28457538.062</v>
+        <v>20792092.0</v>
       </c>
       <c r="AB45" s="1">
         <v>31542941.0</v>
       </c>
       <c r="AC45" s="1">
-        <v>4270402.938</v>
+        <v>11935849.0</v>
       </c>
       <c r="AD45" s="2">
         <v>0.3784</v>
       </c>
       <c r="AE45" s="1">
-        <v>7665446.062</v>
+        <v>7665447.0</v>
       </c>
       <c r="AF45" s="2">
         <v>0.022</v>
@@ -15811,19 +15811,19 @@
       <c r="Y46" s="1"/>
       <c r="Z46" s="2"/>
       <c r="AA46" s="1">
-        <v>31289355.232</v>
+        <v>22831772.0</v>
       </c>
       <c r="AB46" s="1">
         <v>34816235.0</v>
       </c>
       <c r="AC46" s="1">
-        <v>4716879.768</v>
+        <v>13174463.0</v>
       </c>
       <c r="AD46" s="2">
         <v>0.3784</v>
       </c>
       <c r="AE46" s="1">
-        <v>8457583.232</v>
+        <v>8457584.0</v>
       </c>
       <c r="AF46" s="2">
         <v>0.022</v>
@@ -15904,19 +15904,19 @@
       <c r="Y47" s="1"/>
       <c r="Z47" s="2"/>
       <c r="AA47" s="1">
-        <v>34404285.13</v>
+        <v>25075230.0</v>
       </c>
       <c r="AB47" s="1">
         <v>38417359.0</v>
       </c>
       <c r="AC47" s="1">
-        <v>5208073.87</v>
+        <v>14537129.0</v>
       </c>
       <c r="AD47" s="2">
         <v>0.3784</v>
       </c>
       <c r="AE47" s="1">
-        <v>9329055.13</v>
+        <v>9329056.0</v>
       </c>
       <c r="AF47" s="2">
         <v>0.022</v>
@@ -15997,19 +15997,19 @@
       <c r="Y48" s="1"/>
       <c r="Z48" s="2"/>
       <c r="AA48" s="1">
-        <v>37830640.22</v>
+        <v>27542845.0</v>
       </c>
       <c r="AB48" s="1">
         <v>42379095.0</v>
       </c>
       <c r="AC48" s="1">
-        <v>5748454.78</v>
+        <v>16036250.0</v>
       </c>
       <c r="AD48" s="2">
         <v>0.3784</v>
       </c>
       <c r="AE48" s="1">
-        <v>10287795.22</v>
+        <v>10287796.0</v>
       </c>
       <c r="AF48" s="2">
         <v>0.022</v>
@@ -16090,19 +16090,19 @@
       <c r="Y49" s="1"/>
       <c r="Z49" s="2"/>
       <c r="AA49" s="1">
-        <v>41599563.33</v>
+        <v>30257033.0</v>
       </c>
       <c r="AB49" s="1">
         <v>46737505.0</v>
       </c>
       <c r="AC49" s="1">
-        <v>6342941.67</v>
+        <v>17685472.0</v>
       </c>
       <c r="AD49" s="2">
         <v>0.3784</v>
       </c>
       <c r="AE49" s="1">
-        <v>11342530.33</v>
+        <v>11342531.0</v>
       </c>
       <c r="AF49" s="2">
         <v>0.022</v>
@@ -16183,19 +16183,19 @@
       <c r="Y50" s="1"/>
       <c r="Z50" s="2"/>
       <c r="AA50" s="1">
-        <v>45745309.962</v>
+        <v>33242450.0</v>
       </c>
       <c r="AB50" s="1">
         <v>51532256.0</v>
       </c>
       <c r="AC50" s="1">
-        <v>6996946.038</v>
+        <v>19499806.0</v>
       </c>
       <c r="AD50" s="2">
         <v>0.3784</v>
       </c>
       <c r="AE50" s="1">
-        <v>12502859.962</v>
+        <v>12502861.0</v>
       </c>
       <c r="AF50" s="2">
         <v>0.022</v>
@@ -16276,19 +16276,19 @@
       <c r="Y51" s="1"/>
       <c r="Z51" s="2"/>
       <c r="AA51" s="1">
-        <v>50305563.566</v>
+        <v>36526220.0</v>
       </c>
       <c r="AB51" s="1">
         <v>56806982.0</v>
       </c>
       <c r="AC51" s="1">
-        <v>7716418.434</v>
+        <v>21495762.0</v>
       </c>
       <c r="AD51" s="2">
         <v>0.3784</v>
       </c>
       <c r="AE51" s="1">
-        <v>13779343.566</v>
+        <v>13779345.0</v>
       </c>
       <c r="AF51" s="2">
         <v>0.022</v>
@@ -16369,19 +16369,19 @@
       <c r="Y52" s="1"/>
       <c r="Z52" s="2"/>
       <c r="AA52" s="1">
-        <v>55321773.526</v>
+        <v>40138177.0</v>
       </c>
       <c r="AB52" s="1">
         <v>62609680.0</v>
       </c>
       <c r="AC52" s="1">
-        <v>8507906.474</v>
+        <v>23691503.0</v>
       </c>
       <c r="AD52" s="2">
         <v>0.3784</v>
       </c>
       <c r="AE52" s="1">
-        <v>15183596.526</v>
+        <v>15183598.0</v>
       </c>
       <c r="AF52" s="2">
         <v>0.022</v>
@@ -16462,19 +16462,19 @@
       <c r="Y53" s="13"/>
       <c r="Z53" s="14"/>
       <c r="AA53" s="13">
-        <v>52166353.0</v>
+        <v>35631163.0</v>
       </c>
       <c r="AB53" s="13">
         <v>68194777.0</v>
       </c>
       <c r="AC53" s="13">
-        <v>9269714.0</v>
+        <v>25804904.0</v>
       </c>
       <c r="AD53" s="14">
         <v>0.3784</v>
       </c>
       <c r="AE53" s="13">
-        <v>16535190.0</v>
+        <v>12801634.0</v>
       </c>
       <c r="AF53" s="14">
         <v>0.022</v>
@@ -16553,19 +16553,19 @@
       <c r="Y54" s="1"/>
       <c r="Z54" s="2"/>
       <c r="AA54" s="1">
-        <v>50494941.4678</v>
+        <v>32685391.9</v>
       </c>
       <c r="AB54" s="1">
         <v>66702015.9</v>
       </c>
       <c r="AC54" s="1">
-        <v>7430493.4322</v>
+        <v>25240043.0</v>
       </c>
       <c r="AD54" s="2">
         <v>0.3784</v>
       </c>
       <c r="AE54" s="1">
-        <v>17809549.5678</v>
+        <v>9673661.0</v>
       </c>
       <c r="AF54" s="2">
         <v>0.022</v>
@@ -16644,19 +16644,19 @@
       <c r="Y55" s="1"/>
       <c r="Z55" s="2"/>
       <c r="AA55" s="1">
-        <v>48330461.622</v>
+        <v>29352749.1</v>
       </c>
       <c r="AB55" s="1">
         <v>62752555.1</v>
       </c>
       <c r="AC55" s="1">
-        <v>4767854.478</v>
+        <v>23745567.0</v>
       </c>
       <c r="AD55" s="2">
         <v>0.3784</v>
       </c>
       <c r="AE55" s="1">
-        <v>18977712.522</v>
+        <v>6232890.0</v>
       </c>
       <c r="AF55" s="2">
         <v>0.022</v>
@@ -16735,19 +16735,19 @@
       <c r="Y56" s="1"/>
       <c r="Z56" s="2"/>
       <c r="AA56" s="1">
-        <v>45032419.6334</v>
+        <v>25026723.7</v>
       </c>
       <c r="AB56" s="1">
         <v>57346181.7</v>
       </c>
       <c r="AC56" s="1">
-        <v>1694099.0666</v>
+        <v>21699795.0</v>
       </c>
       <c r="AD56" s="2">
         <v>0.3784</v>
       </c>
       <c r="AE56" s="1">
-        <v>20005695.9334</v>
+        <v>2448043.0</v>
       </c>
       <c r="AF56" s="2">
         <v>0.022</v>
@@ -16826,23 +16826,21 @@
       <c r="Y57" s="13"/>
       <c r="Z57" s="14"/>
       <c r="AA57" s="13">
-        <v>38549378.0</v>
+        <v>19541965.0</v>
       </c>
       <c r="AB57" s="13">
         <v>50231008.0</v>
       </c>
       <c r="AC57" s="13">
-        <v>0</v>
+        <v>19007413.0</v>
       </c>
       <c r="AD57" s="14">
         <v>0.3784</v>
       </c>
       <c r="AE57" s="13">
-        <v>20853782.2494</v>
-      </c>
-      <c r="AF57" s="14">
-        <v>0.022</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="AF57" s="14"/>
       <c r="AG57" s="13">
         <v>-394193.368</v>
       </c>
@@ -16917,19 +16915,19 @@
       <c r="Y58" s="1"/>
       <c r="Z58" s="2"/>
       <c r="AA58" s="1">
-        <v>28269543.7</v>
+        <v>12709986.7</v>
       </c>
       <c r="AB58" s="1">
         <v>41119336.7</v>
       </c>
       <c r="AC58" s="1">
-        <v>0</v>
+        <v>15559557.0</v>
       </c>
       <c r="AD58" s="2">
         <v>0.3784</v>
       </c>
       <c r="AE58" s="1">
-        <v>21475712.2108</v>
+        <v>621930.0</v>
       </c>
       <c r="AF58" s="2">
         <v>0.022</v>
@@ -17008,23 +17006,21 @@
       <c r="Y59" s="1"/>
       <c r="Z59" s="2"/>
       <c r="AA59" s="1">
-        <v>15548248.8</v>
+        <v>4316193.8</v>
       </c>
       <c r="AB59" s="1">
         <v>29683020.8</v>
       </c>
       <c r="AC59" s="1">
-        <v>0</v>
+        <v>11232055.0</v>
       </c>
       <c r="AD59" s="2">
         <v>0.3784</v>
       </c>
       <c r="AE59" s="1">
-        <v>21817773.6844</v>
-      </c>
-      <c r="AF59" s="2">
-        <v>0.022</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="AF59" s="2"/>
       <c r="AG59" s="1">
         <v>-231771.984</v>
       </c>
@@ -17099,23 +17095,21 @@
       <c r="Y60" s="5"/>
       <c r="Z60" s="16"/>
       <c r="AA60" s="5">
-        <v>0.099999997764826</v>
+        <v>-5883456.9</v>
       </c>
       <c r="AB60" s="5">
         <v>15548249.1</v>
       </c>
       <c r="AC60" s="5">
-        <v>0</v>
+        <v>5883457.0</v>
       </c>
       <c r="AD60" s="16">
         <v>0.3784</v>
       </c>
       <c r="AE60" s="5">
-        <v>21817773.6866</v>
-      </c>
-      <c r="AF60" s="16">
-        <v>0.022</v>
-      </c>
+        <v>0.0</v>
+      </c>
+      <c r="AF60" s="16"/>
       <c r="AG60" s="5">
         <v>-119824.592</v>
       </c>

</xml_diff>